<commit_message>
changing generate to be more efficient
</commit_message>
<xml_diff>
--- a/Datasets_all.xlsx
+++ b/Datasets_all.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k23030440/Pseudovisium/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF2E163-146E-9744-A24C-721B2915B753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F112D47-D643-0649-9668-7C7589D778CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="1220" windowWidth="28040" windowHeight="17440" xr2:uid="{419F9F52-EC29-7E45-8CDA-DBEF0D21635D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -845,7 +845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F01D6A24-CDB1-1E4B-87EB-E299D59C8055}">
   <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" zoomScale="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed quality filter in new pv_generate implementation
</commit_message>
<xml_diff>
--- a/Datasets_all.xlsx
+++ b/Datasets_all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k23030440/Pseudovisium/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8598C9E5-7959-BE43-A51A-5ED8ECD4C3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BEA131-C53F-7C42-9CA1-7BC1A51EBA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="1200" windowWidth="28040" windowHeight="17440" xr2:uid="{419F9F52-EC29-7E45-8CDA-DBEF0D21635D}"/>
+    <workbookView xWindow="5580" yWindow="6380" windowWidth="28040" windowHeight="17440" xr2:uid="{419F9F52-EC29-7E45-8CDA-DBEF0D21635D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="232">
   <si>
     <t>Author</t>
   </si>
@@ -642,6 +642,96 @@
   </si>
   <si>
     <t>Visium_ovarian</t>
+  </si>
+  <si>
+    <t>https://81ntra.bl.files.1drv.com/y4mCeIG43Quqb1PmlbdxVyJw_FFaZ1wei7AHR-p_6hzYPpcKirP0gEUoDiP1roiyLoPlXMB_tcSPZqdQrsPRJOCyKI1HjRuAijOcOzigUj6I6Wmxaf9LBPMqqYnfkNH_SkH6bqwCqvsuYeKU6Pib1pTqGIQyYf0kmWrIRuJ5EBLVlQdD6mAcYjLYvpVq_6-K4pyJIoo0dVUt0nlhAUMQc1ejg</t>
+  </si>
+  <si>
+    <t>https://h4hpuq.bl.files.1drv.com/y4mus933jqzh4PA90n6Qk7EUdIvpXhXV-iASfKlbi8Bmp7CsHAnTEn-MNklkpVkzDKmkAmV6iQ3f80e_jJ49Z0nmvuj5Y7CTw77D-ZYcS0cqDZOaQHgbUrh-RuDEGqcEzwGRqpvQsohSZalRqmFOddyffeycqvfLC-danHDXtLtwuYIHDTSrS8KynxqC0TpDS7f0YICtrwVoziwEkyCT6vQpg</t>
+  </si>
+  <si>
+    <t>https://vwoeqw.bl.files.1drv.com/y4moHojDYpOe3GKr_7_GUQFwC-o3S3sxYx8rP5TSgyT5wMwl67cU7uK4bdwxRjiWktLcwpjY1q_sBiMykYOvLM6GfxlZO0Z6O-M8JD8OFuNvzMunOCfa2VVZG3AYeh5_HpZn31gp5gPynr0hylzORbraeKNo97SxVQpPXqSvsbXLtcA1qhxpWJ93ghipADm1K-5aIcqhXMvh5_e8WEXetyopA</t>
+  </si>
+  <si>
+    <t>https://ivz2xa.bl.files.1drv.com/y4mlOmzWwABvkcmkK0yYu61bIsUM04VgvJZrYJfOI74_AtOBaiRoCaZv5KER_9eS4CEMrLD-BuKFZbHW5SATud5X20gVbuZVIeUQp14r2a3ZFJ54325EnmaclmGjjf-q0H3O9NH3mr4cN_oVCwRBHXCw15Cz7Nc1E4vhL4GUTcr29LvtpdYcM8EK51lnYw68xgyuGRqeaifdP_JMX_wGHw56Q</t>
+  </si>
+  <si>
+    <t>https://ael3ng.bl.files.1drv.com/y4m1UhtPBAUrjjYmm4dgdWCNsU5DYwc-46Ewo2w-MBtCng3XofzVBscU0HSBW6caQkYv-h6UlEPYNc5EBmr5sLBVOlZaQGZiM1LK45OMOb-u_TN1NjiGWSvO1mW6njkvorDBaLAFvO2j2C22mPpjqaj2yFn6_gnE-CqiKTpFvcv7fIJLbHIJyZFOW5Qhx77cSmzfyBtPW6nQtrNkZG5vjy63Q</t>
+  </si>
+  <si>
+    <t>https://7awofw.bl.files.1drv.com/y4mQA4-eC-NUFuCVZ4szvAzFE98delLuJVREpCkpn6iuDFmegwUuGztiqHmF6fVBEc47sF97sUc5ZtoyJ4sz8ZY7IdKXf_-bNYWWlVnYCZp-erjmw1EhQ-ehwXIpfgNgytPbbaZouJWsvlMQLPoq9QOu3Ip1jRGUnKhf_Ho72TqE0ItidTkHiy6YUEqoF755ZPpz7RH3MfikqApEtK4nwYHOA</t>
+  </si>
+  <si>
+    <t>Vizgen_colon_pt2</t>
+  </si>
+  <si>
+    <t>Vizgen_liver_cancer_pt1</t>
+  </si>
+  <si>
+    <t>Vizgen_ovarian_cancer_pt1</t>
+  </si>
+  <si>
+    <t>Vizgen_liver_1</t>
+  </si>
+  <si>
+    <t>Vizgen_liver_2</t>
+  </si>
+  <si>
+    <t>https://81nura.bl.files.1drv.com/y4mk3sYMu93m6og5E0uxDGZhrurZLtJOUcN-iqxlcxwyZoGiqnzkjjCnOWD5dLWTAMraM7MP-6bIwYHjPXaj4YBBBZkS6EWWvjxcWfnapswn0lp6TNhmOqY5wPeC2rkPvpyaQpq21iso45SWBGFnV20VF7ZpEqIrv1BGUdxWgp_0DC6yyt4MO09HlKL101KCZ0eCiG_d_oqHNlPnK9KeCWXCQ</t>
+  </si>
+  <si>
+    <t>https://jsgv5w.bl.files.1drv.com/y4mEl3V-IAI9M9sKQwbzKOBflvKAfWGfBvzxg4koxYyTWFO15UjdRca8Bl2fyKVlSWqboNl3AQCg5VDVlj4g5nFG0mgYBbCTHekJBaIdF6JXkzaFFia5dLx9A3lGaUTTjlli8yR3tXQSOcg8cE84LxiwjuHKqwtUqDN_6Kha-FW7XKQgkw_GVv7WkJuCfvBbqStMGAv1-tzeIGaYGDaHJhfCg</t>
+  </si>
+  <si>
+    <t>https://vwogqw.bl.files.1drv.com/y4mfo0Wvk43oAStRyFWtIdXiq0wRfaWeT12_wjOs8HGkiL3NTgB2kWAIaf2QQxD-bc9_T-NHhY3Dxe6YyFr8ZEBvdQnrexXg62kfJg2dSwc1FfxttAeCrSKsrc6Z8PFeM5HAz7sCaY4g1gsEIgviHwEFgFRMiH4AhVLQwx5SIsgGu-eOd-DOR9rbdFGTU4YpjirFF0wKO9nRMHtm19kaFbptw</t>
+  </si>
+  <si>
+    <t>https://wnqgoq.bl.files.1drv.com/y4mci_gZEAiljkwusJY2QckiRi0cvDdCZJBapdqcdL-wDiXOFE1LJfjO_aX2NK5KfRjefwmM1abNazREWdIUyKHEo6eXXGwAo6JMdEzUomgfTQKaPoeSfiFUCfksvafHXHLndLScQ3jk5yHv3MegLW8501GI1UBwo_kEVYvDNYlFxuxwmVB0ykKo8O51tgn7YQQxIC2oa9YjKq-D7MZWW8PPw</t>
+  </si>
+  <si>
+    <t>https://kt29iq.bl.files.1drv.com/y4mCpagDU-VBSEIZ_xXO7q1wj5xVrg-t1QMYHGJmKvBYf8feyFiTu5IKAfUzPVnz6o6-Ytluw1QE9s5r73qqWZ6kRoF26b8ItB1-P2JY319vPiAztZ8JisPGovQTK4tG48c3vd3FxScGEx5DtAu14HlKl41ojAe5yDqBpDCWnV3Boo-8lmHRTZ4A5PS21R9n-Mz-9FAPjOSNkqZPigWO5U3OQ</t>
+  </si>
+  <si>
+    <t>Liver</t>
+  </si>
+  <si>
+    <t>Liver cancer</t>
+  </si>
+  <si>
+    <t>Ovarian cancer</t>
+  </si>
+  <si>
+    <t>https://console.cloud.google.com/storage/browser/vz-ffpe-showcase/</t>
+  </si>
+  <si>
+    <t>https://console.cloud.google.com/storage/browser/vz-liver-showcase</t>
+  </si>
+  <si>
+    <t>Ovary</t>
+  </si>
+  <si>
+    <t>Curio_ovary_1</t>
+  </si>
+  <si>
+    <t>Curio_ovary_2</t>
+  </si>
+  <si>
+    <t>Curio_ovary_3</t>
+  </si>
+  <si>
+    <t>Curio_ovary_4</t>
+  </si>
+  <si>
+    <t>Curio_ovary_5</t>
+  </si>
+  <si>
+    <t>Curio_ovary_6</t>
+  </si>
+  <si>
+    <t>Curio_ovary_7</t>
+  </si>
+  <si>
+    <t>Curio_ovary_8</t>
   </si>
 </sst>
 </file>
@@ -1052,10 +1142,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F01D6A24-CDB1-1E4B-87EB-E299D59C8055}">
-  <dimension ref="A1:P128"/>
+  <dimension ref="A1:P136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="D78" zoomScale="84" workbookViewId="0">
+      <selection activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2817,6 +2907,9 @@
       <c r="D41" t="s">
         <v>98</v>
       </c>
+      <c r="E41" t="s">
+        <v>202</v>
+      </c>
       <c r="F41" t="s">
         <v>85</v>
       </c>
@@ -2839,7 +2932,7 @@
         <v>0</v>
       </c>
       <c r="M41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N41">
         <v>0</v>
@@ -3460,6 +3553,9 @@
       <c r="D55" t="s">
         <v>33</v>
       </c>
+      <c r="E55" t="s">
+        <v>203</v>
+      </c>
       <c r="F55" t="s">
         <v>193</v>
       </c>
@@ -3495,6 +3591,9 @@
       <c r="D56" t="s">
         <v>33</v>
       </c>
+      <c r="E56" t="s">
+        <v>204</v>
+      </c>
       <c r="F56" t="s">
         <v>194</v>
       </c>
@@ -3530,6 +3629,9 @@
       <c r="D57" t="s">
         <v>33</v>
       </c>
+      <c r="E57" t="s">
+        <v>205</v>
+      </c>
       <c r="F57" t="s">
         <v>195</v>
       </c>
@@ -3565,6 +3667,9 @@
       <c r="D58" t="s">
         <v>33</v>
       </c>
+      <c r="E58" t="s">
+        <v>206</v>
+      </c>
       <c r="F58" t="s">
         <v>196</v>
       </c>
@@ -3600,6 +3705,9 @@
       <c r="D59" t="s">
         <v>33</v>
       </c>
+      <c r="E59" t="s">
+        <v>207</v>
+      </c>
       <c r="F59" t="s">
         <v>197</v>
       </c>
@@ -3612,312 +3720,105 @@
       <c r="I59" t="s">
         <v>11</v>
       </c>
-      <c r="J59">
-        <v>0</v>
-      </c>
-      <c r="K59">
-        <v>0</v>
-      </c>
-      <c r="L59">
-        <v>0</v>
-      </c>
-      <c r="M59">
-        <v>0</v>
-      </c>
-      <c r="N59">
-        <v>0</v>
-      </c>
-      <c r="O59">
-        <v>0</v>
-      </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>175</v>
-      </c>
-      <c r="B60">
-        <v>2023</v>
-      </c>
-      <c r="D60" t="s">
-        <v>42</v>
-      </c>
-      <c r="E60" t="s">
-        <v>177</v>
-      </c>
       <c r="F60" t="s">
-        <v>180</v>
+        <v>224</v>
       </c>
       <c r="G60" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H60" t="s">
-        <v>36</v>
-      </c>
-      <c r="I60" t="s">
-        <v>11</v>
-      </c>
-      <c r="J60">
-        <v>0</v>
-      </c>
-      <c r="K60">
-        <v>0</v>
-      </c>
-      <c r="L60">
-        <v>0</v>
-      </c>
-      <c r="M60">
-        <v>0</v>
-      </c>
-      <c r="N60">
-        <v>0</v>
-      </c>
-      <c r="O60">
-        <v>1</v>
+        <v>223</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>175</v>
-      </c>
-      <c r="B61">
-        <v>2023</v>
-      </c>
-      <c r="D61" t="s">
-        <v>42</v>
-      </c>
-      <c r="E61" t="s">
-        <v>178</v>
-      </c>
       <c r="F61" t="s">
-        <v>181</v>
+        <v>225</v>
       </c>
       <c r="G61" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H61" t="s">
-        <v>36</v>
-      </c>
-      <c r="I61" t="s">
-        <v>11</v>
-      </c>
-      <c r="J61">
-        <v>0</v>
-      </c>
-      <c r="K61">
-        <v>0</v>
-      </c>
-      <c r="L61">
-        <v>0</v>
-      </c>
-      <c r="M61">
-        <v>0</v>
-      </c>
-      <c r="N61">
-        <v>0</v>
-      </c>
-      <c r="O61">
-        <v>1</v>
+        <v>223</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>175</v>
-      </c>
-      <c r="B62">
-        <v>2023</v>
-      </c>
-      <c r="D62" t="s">
-        <v>42</v>
-      </c>
-      <c r="E62" t="s">
-        <v>179</v>
-      </c>
       <c r="F62" t="s">
-        <v>182</v>
+        <v>226</v>
       </c>
       <c r="G62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H62" t="s">
-        <v>36</v>
-      </c>
-      <c r="I62" t="s">
-        <v>11</v>
-      </c>
-      <c r="J62">
-        <v>0</v>
-      </c>
-      <c r="K62">
-        <v>0</v>
-      </c>
-      <c r="L62">
-        <v>0</v>
-      </c>
-      <c r="M62">
-        <v>0</v>
-      </c>
-      <c r="N62">
-        <v>0</v>
-      </c>
-      <c r="O62">
-        <v>1</v>
+        <v>223</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>18</v>
-      </c>
-      <c r="B63">
-        <v>2024</v>
-      </c>
-      <c r="D63" t="s">
-        <v>44</v>
-      </c>
-      <c r="E63" t="s">
-        <v>57</v>
-      </c>
       <c r="F63" t="s">
-        <v>183</v>
+        <v>227</v>
       </c>
       <c r="G63" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="H63" t="s">
-        <v>124</v>
-      </c>
-      <c r="I63" t="s">
-        <v>11</v>
-      </c>
-      <c r="L63">
-        <v>1</v>
-      </c>
-      <c r="N63">
-        <v>0</v>
-      </c>
-      <c r="O63">
-        <v>0</v>
+        <v>223</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>18</v>
-      </c>
-      <c r="B64">
-        <v>2024</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="F64" t="s">
-        <v>184</v>
+        <v>228</v>
       </c>
       <c r="G64" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="H64" t="s">
-        <v>125</v>
-      </c>
-      <c r="L64">
-        <v>1</v>
-      </c>
-      <c r="N64">
-        <v>0</v>
-      </c>
-      <c r="O64">
-        <v>0</v>
+        <v>223</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>18</v>
-      </c>
-      <c r="B65">
-        <v>2024</v>
-      </c>
-      <c r="D65" t="s">
-        <v>45</v>
-      </c>
-      <c r="E65" t="s">
-        <v>58</v>
-      </c>
       <c r="F65" t="s">
-        <v>185</v>
+        <v>229</v>
       </c>
       <c r="G65" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="H65" t="s">
-        <v>126</v>
-      </c>
-      <c r="I65" t="s">
-        <v>12</v>
-      </c>
-      <c r="L65">
-        <v>1</v>
-      </c>
-      <c r="N65">
-        <v>0</v>
-      </c>
-      <c r="O65">
-        <v>0</v>
+        <v>223</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>18</v>
-      </c>
-      <c r="B66">
-        <v>2024</v>
-      </c>
-      <c r="E66" t="s">
-        <v>191</v>
-      </c>
       <c r="F66" t="s">
-        <v>186</v>
+        <v>230</v>
       </c>
       <c r="G66" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="H66" t="s">
-        <v>127</v>
-      </c>
-      <c r="L66">
-        <v>1</v>
-      </c>
-      <c r="N66">
-        <v>0</v>
-      </c>
-      <c r="O66">
-        <v>0</v>
+        <v>223</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>18</v>
-      </c>
-      <c r="B67">
-        <v>2024</v>
-      </c>
-      <c r="D67" t="s">
-        <v>46</v>
-      </c>
-      <c r="E67" t="s">
-        <v>59</v>
-      </c>
-      <c r="F67" s="4" t="s">
-        <v>187</v>
+      <c r="F67" t="s">
+        <v>231</v>
       </c>
       <c r="G67" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="H67" t="s">
-        <v>128</v>
-      </c>
-      <c r="I67" t="s">
-        <v>11</v>
+        <v>223</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
       </c>
       <c r="L67">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="M67">
+        <v>0</v>
       </c>
       <c r="N67">
         <v>0</v>
@@ -3928,97 +3829,163 @@
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>18</v>
+        <v>175</v>
       </c>
       <c r="B68">
-        <v>2024</v>
+        <v>2023</v>
+      </c>
+      <c r="D68" t="s">
+        <v>42</v>
       </c>
       <c r="E68" t="s">
-        <v>192</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>188</v>
+        <v>177</v>
+      </c>
+      <c r="F68" t="s">
+        <v>180</v>
       </c>
       <c r="G68" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H68" t="s">
-        <v>129</v>
+        <v>36</v>
+      </c>
+      <c r="I68" t="s">
+        <v>11</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+      <c r="K68">
+        <v>0</v>
       </c>
       <c r="L68">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="M68">
+        <v>0</v>
       </c>
       <c r="N68">
         <v>0</v>
       </c>
       <c r="O68">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>18</v>
+        <v>175</v>
       </c>
       <c r="B69">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="D69" t="s">
-        <v>47</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>189</v>
+        <v>42</v>
+      </c>
+      <c r="E69" t="s">
+        <v>178</v>
+      </c>
+      <c r="F69" t="s">
+        <v>181</v>
       </c>
       <c r="G69" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H69" t="s">
-        <v>130</v>
+        <v>36</v>
       </c>
       <c r="I69" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
+      <c r="M69">
+        <v>0</v>
       </c>
       <c r="N69">
         <v>0</v>
       </c>
       <c r="O69">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>18</v>
+        <v>175</v>
       </c>
       <c r="B70">
-        <v>2024</v>
-      </c>
-      <c r="F70" s="4" t="s">
-        <v>190</v>
+        <v>2023</v>
+      </c>
+      <c r="D70" t="s">
+        <v>42</v>
+      </c>
+      <c r="E70" t="s">
+        <v>179</v>
+      </c>
+      <c r="F70" t="s">
+        <v>182</v>
       </c>
       <c r="G70" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H70" t="s">
-        <v>131</v>
+        <v>36</v>
+      </c>
+      <c r="I70" t="s">
+        <v>11</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+      <c r="K70">
+        <v>0</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
+      <c r="M70">
+        <v>0</v>
       </c>
       <c r="N70">
         <v>0</v>
       </c>
       <c r="O70">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>48</v>
+        <v>18</v>
+      </c>
+      <c r="B71">
+        <v>2024</v>
+      </c>
+      <c r="D71" t="s">
+        <v>44</v>
+      </c>
+      <c r="E71" t="s">
+        <v>57</v>
+      </c>
+      <c r="F71" t="s">
+        <v>183</v>
       </c>
       <c r="G71" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H71" t="s">
-        <v>10</v>
+        <v>124</v>
       </c>
       <c r="I71" t="s">
         <v>11</v>
+      </c>
+      <c r="L71">
+        <v>1</v>
       </c>
       <c r="N71">
         <v>0</v>
@@ -4029,16 +3996,25 @@
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>48</v>
+        <v>18</v>
+      </c>
+      <c r="B72">
+        <v>2024</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F72" t="s">
+        <v>184</v>
       </c>
       <c r="G72" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H72" t="s">
-        <v>10</v>
-      </c>
-      <c r="I72" t="s">
-        <v>11</v>
+        <v>125</v>
+      </c>
+      <c r="L72">
+        <v>1</v>
       </c>
       <c r="N72">
         <v>0</v>
@@ -4049,16 +4025,31 @@
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>48</v>
+        <v>18</v>
+      </c>
+      <c r="B73">
+        <v>2024</v>
+      </c>
+      <c r="D73" t="s">
+        <v>45</v>
+      </c>
+      <c r="E73" t="s">
+        <v>58</v>
+      </c>
+      <c r="F73" t="s">
+        <v>185</v>
       </c>
       <c r="G73" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H73" t="s">
-        <v>10</v>
+        <v>126</v>
       </c>
       <c r="I73" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="L73">
+        <v>1</v>
       </c>
       <c r="N73">
         <v>0</v>
@@ -4069,22 +4060,22 @@
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>48</v>
+        <v>18</v>
+      </c>
+      <c r="B74">
+        <v>2024</v>
       </c>
       <c r="E74" t="s">
-        <v>60</v>
+        <v>191</v>
       </c>
       <c r="F74" t="s">
-        <v>61</v>
+        <v>186</v>
       </c>
       <c r="G74" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H74" t="s">
-        <v>10</v>
-      </c>
-      <c r="I74" t="s">
-        <v>11</v>
+        <v>127</v>
       </c>
       <c r="L74">
         <v>1</v>
@@ -4098,16 +4089,31 @@
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>48</v>
+        <v>18</v>
+      </c>
+      <c r="B75">
+        <v>2024</v>
+      </c>
+      <c r="D75" t="s">
+        <v>46</v>
+      </c>
+      <c r="E75" t="s">
+        <v>59</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>187</v>
       </c>
       <c r="G75" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H75" t="s">
-        <v>10</v>
+        <v>128</v>
       </c>
       <c r="I75" t="s">
         <v>11</v>
+      </c>
+      <c r="L75">
+        <v>1</v>
       </c>
       <c r="N75">
         <v>0</v>
@@ -4118,16 +4124,25 @@
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>48</v>
+        <v>18</v>
+      </c>
+      <c r="B76">
+        <v>2024</v>
+      </c>
+      <c r="E76" t="s">
+        <v>192</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="G76" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H76" t="s">
-        <v>10</v>
-      </c>
-      <c r="I76" t="s">
-        <v>11</v>
+        <v>129</v>
+      </c>
+      <c r="L76">
+        <v>1</v>
       </c>
       <c r="N76">
         <v>0</v>
@@ -4138,16 +4153,25 @@
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>48</v>
+        <v>18</v>
+      </c>
+      <c r="B77">
+        <v>2024</v>
+      </c>
+      <c r="D77" t="s">
+        <v>47</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>189</v>
       </c>
       <c r="G77" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H77" t="s">
-        <v>10</v>
+        <v>130</v>
       </c>
       <c r="I77" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N77">
         <v>0</v>
@@ -4158,16 +4182,19 @@
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>48</v>
+        <v>18</v>
+      </c>
+      <c r="B78">
+        <v>2024</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>190</v>
       </c>
       <c r="G78" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H78" t="s">
-        <v>10</v>
-      </c>
-      <c r="I78" t="s">
-        <v>11</v>
+        <v>131</v>
       </c>
       <c r="N78">
         <v>0</v>
@@ -4180,14 +4207,20 @@
       <c r="A79" t="s">
         <v>48</v>
       </c>
+      <c r="D79" t="s">
+        <v>221</v>
+      </c>
+      <c r="E79" t="s">
+        <v>60</v>
+      </c>
+      <c r="F79" t="s">
+        <v>61</v>
+      </c>
       <c r="G79" t="s">
         <v>48</v>
       </c>
       <c r="H79" t="s">
         <v>10</v>
-      </c>
-      <c r="I79" t="s">
-        <v>11</v>
       </c>
       <c r="N79">
         <v>0</v>
@@ -4200,14 +4233,23 @@
       <c r="A80" t="s">
         <v>48</v>
       </c>
+      <c r="D80" t="s">
+        <v>221</v>
+      </c>
+      <c r="E80" t="s">
+        <v>213</v>
+      </c>
+      <c r="F80" t="s">
+        <v>208</v>
+      </c>
       <c r="G80" t="s">
         <v>48</v>
       </c>
       <c r="H80" t="s">
-        <v>49</v>
-      </c>
-      <c r="I80" t="s">
-        <v>12</v>
+        <v>21</v>
+      </c>
+      <c r="N80">
+        <v>0</v>
       </c>
       <c r="O80">
         <v>0</v>
@@ -4217,14 +4259,23 @@
       <c r="A81" t="s">
         <v>48</v>
       </c>
+      <c r="D81" t="s">
+        <v>221</v>
+      </c>
+      <c r="E81" t="s">
+        <v>214</v>
+      </c>
+      <c r="F81" t="s">
+        <v>209</v>
+      </c>
       <c r="G81" t="s">
         <v>48</v>
       </c>
       <c r="H81" t="s">
-        <v>49</v>
-      </c>
-      <c r="I81" t="s">
-        <v>12</v>
+        <v>219</v>
+      </c>
+      <c r="N81">
+        <v>0</v>
       </c>
       <c r="O81">
         <v>0</v>
@@ -4234,14 +4285,26 @@
       <c r="A82" t="s">
         <v>48</v>
       </c>
+      <c r="D82" t="s">
+        <v>221</v>
+      </c>
+      <c r="E82" t="s">
+        <v>215</v>
+      </c>
+      <c r="F82" t="s">
+        <v>210</v>
+      </c>
       <c r="G82" t="s">
         <v>48</v>
       </c>
       <c r="H82" t="s">
-        <v>49</v>
-      </c>
-      <c r="I82" t="s">
-        <v>12</v>
+        <v>220</v>
+      </c>
+      <c r="L82">
+        <v>1</v>
+      </c>
+      <c r="N82">
+        <v>0</v>
       </c>
       <c r="O82">
         <v>0</v>
@@ -4251,16 +4314,162 @@
       <c r="A83" t="s">
         <v>48</v>
       </c>
+      <c r="D83" t="s">
+        <v>222</v>
+      </c>
+      <c r="E83" t="s">
+        <v>216</v>
+      </c>
+      <c r="F83" t="s">
+        <v>211</v>
+      </c>
       <c r="G83" t="s">
         <v>48</v>
       </c>
       <c r="H83" t="s">
+        <v>218</v>
+      </c>
+      <c r="N83">
+        <v>0</v>
+      </c>
+      <c r="O83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>48</v>
+      </c>
+      <c r="D84" t="s">
+        <v>222</v>
+      </c>
+      <c r="E84" t="s">
+        <v>217</v>
+      </c>
+      <c r="F84" t="s">
+        <v>212</v>
+      </c>
+      <c r="G84" t="s">
+        <v>48</v>
+      </c>
+      <c r="H84" t="s">
+        <v>218</v>
+      </c>
+      <c r="N84">
+        <v>0</v>
+      </c>
+      <c r="O84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>48</v>
+      </c>
+      <c r="G85" t="s">
+        <v>48</v>
+      </c>
+      <c r="H85" t="s">
         <v>49</v>
       </c>
-      <c r="I83" t="s">
+      <c r="I85" t="s">
         <v>12</v>
       </c>
-      <c r="O83">
+      <c r="N85">
+        <v>0</v>
+      </c>
+      <c r="O85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>48</v>
+      </c>
+      <c r="G86" t="s">
+        <v>48</v>
+      </c>
+      <c r="H86" t="s">
+        <v>49</v>
+      </c>
+      <c r="I86" t="s">
+        <v>12</v>
+      </c>
+      <c r="N86">
+        <v>0</v>
+      </c>
+      <c r="O86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>48</v>
+      </c>
+      <c r="G87" t="s">
+        <v>48</v>
+      </c>
+      <c r="H87" t="s">
+        <v>49</v>
+      </c>
+      <c r="I87" t="s">
+        <v>12</v>
+      </c>
+      <c r="N87">
+        <v>0</v>
+      </c>
+      <c r="O87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>48</v>
+      </c>
+      <c r="G88" t="s">
+        <v>48</v>
+      </c>
+      <c r="H88" t="s">
+        <v>49</v>
+      </c>
+      <c r="I88" t="s">
+        <v>12</v>
+      </c>
+      <c r="O88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>48</v>
+      </c>
+      <c r="G89" t="s">
+        <v>48</v>
+      </c>
+      <c r="H89" t="s">
+        <v>10</v>
+      </c>
+      <c r="I89" t="s">
+        <v>11</v>
+      </c>
+      <c r="O89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>48</v>
+      </c>
+      <c r="G90" t="s">
+        <v>48</v>
+      </c>
+      <c r="H90" t="s">
+        <v>10</v>
+      </c>
+      <c r="I90" t="s">
+        <v>11</v>
+      </c>
+      <c r="O90">
         <v>0</v>
       </c>
     </row>
@@ -4294,9 +4503,6 @@
       <c r="I92" t="s">
         <v>11</v>
       </c>
-      <c r="O92">
-        <v>0</v>
-      </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
@@ -4311,9 +4517,6 @@
       <c r="I93" t="s">
         <v>11</v>
       </c>
-      <c r="O93">
-        <v>0</v>
-      </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
@@ -4328,9 +4531,6 @@
       <c r="I94" t="s">
         <v>11</v>
       </c>
-      <c r="O94">
-        <v>0</v>
-      </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
@@ -4345,9 +4545,6 @@
       <c r="I95" t="s">
         <v>11</v>
       </c>
-      <c r="O95">
-        <v>0</v>
-      </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
@@ -4362,9 +4559,6 @@
       <c r="I96" t="s">
         <v>11</v>
       </c>
-      <c r="O96">
-        <v>0</v>
-      </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
@@ -4379,9 +4573,6 @@
       <c r="I97" t="s">
         <v>11</v>
       </c>
-      <c r="O97">
-        <v>0</v>
-      </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
@@ -4396,9 +4587,6 @@
       <c r="I98" t="s">
         <v>11</v>
       </c>
-      <c r="O98">
-        <v>0</v>
-      </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
@@ -4776,22 +4964,10 @@
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>174</v>
-      </c>
-      <c r="B121">
-        <v>2024</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D121" t="s">
-        <v>158</v>
-      </c>
-      <c r="F121" t="s">
-        <v>166</v>
+        <v>48</v>
       </c>
       <c r="G121" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="H121" t="s">
         <v>10</v>
@@ -4800,27 +4976,15 @@
         <v>11</v>
       </c>
       <c r="O121">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>174</v>
-      </c>
-      <c r="B122">
-        <v>2024</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D122" t="s">
-        <v>159</v>
-      </c>
-      <c r="F122" t="s">
-        <v>167</v>
+        <v>48</v>
       </c>
       <c r="G122" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="H122" t="s">
         <v>10</v>
@@ -4829,27 +4993,15 @@
         <v>11</v>
       </c>
       <c r="O122">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>174</v>
-      </c>
-      <c r="B123">
-        <v>2024</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D123" t="s">
-        <v>160</v>
-      </c>
-      <c r="F123" t="s">
-        <v>168</v>
+        <v>48</v>
       </c>
       <c r="G123" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="H123" t="s">
         <v>10</v>
@@ -4858,27 +5010,15 @@
         <v>11</v>
       </c>
       <c r="O123">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>174</v>
-      </c>
-      <c r="B124">
-        <v>2024</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D124" t="s">
-        <v>161</v>
-      </c>
-      <c r="F124" t="s">
-        <v>169</v>
+        <v>48</v>
       </c>
       <c r="G124" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="H124" t="s">
         <v>10</v>
@@ -4887,27 +5027,15 @@
         <v>11</v>
       </c>
       <c r="O124">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>174</v>
-      </c>
-      <c r="B125">
-        <v>2024</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D125" t="s">
-        <v>162</v>
-      </c>
-      <c r="F125" t="s">
-        <v>170</v>
+        <v>48</v>
       </c>
       <c r="G125" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="H125" t="s">
         <v>10</v>
@@ -4916,27 +5044,15 @@
         <v>11</v>
       </c>
       <c r="O125">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>174</v>
-      </c>
-      <c r="B126">
-        <v>2024</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D126" t="s">
-        <v>163</v>
-      </c>
-      <c r="F126" t="s">
-        <v>171</v>
+        <v>48</v>
       </c>
       <c r="G126" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="H126" t="s">
         <v>10</v>
@@ -4945,27 +5061,15 @@
         <v>11</v>
       </c>
       <c r="O126">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>174</v>
-      </c>
-      <c r="B127">
-        <v>2024</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D127" t="s">
-        <v>164</v>
-      </c>
-      <c r="F127" t="s">
-        <v>172</v>
+        <v>48</v>
       </c>
       <c r="G127" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="H127" t="s">
         <v>10</v>
@@ -4974,35 +5078,255 @@
         <v>11</v>
       </c>
       <c r="O127">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
+        <v>48</v>
+      </c>
+      <c r="G128" t="s">
+        <v>48</v>
+      </c>
+      <c r="H128" t="s">
+        <v>10</v>
+      </c>
+      <c r="I128" t="s">
+        <v>11</v>
+      </c>
+      <c r="O128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
         <v>174</v>
       </c>
-      <c r="B128">
+      <c r="B129">
         <v>2024</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="C129" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D129" t="s">
+        <v>158</v>
+      </c>
+      <c r="F129" t="s">
+        <v>166</v>
+      </c>
+      <c r="G129" t="s">
+        <v>30</v>
+      </c>
+      <c r="H129" t="s">
+        <v>10</v>
+      </c>
+      <c r="I129" t="s">
+        <v>11</v>
+      </c>
+      <c r="O129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>174</v>
+      </c>
+      <c r="B130">
+        <v>2024</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D130" t="s">
+        <v>159</v>
+      </c>
+      <c r="F130" t="s">
+        <v>167</v>
+      </c>
+      <c r="G130" t="s">
+        <v>30</v>
+      </c>
+      <c r="H130" t="s">
+        <v>10</v>
+      </c>
+      <c r="I130" t="s">
+        <v>11</v>
+      </c>
+      <c r="O130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>174</v>
+      </c>
+      <c r="B131">
+        <v>2024</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D131" t="s">
+        <v>160</v>
+      </c>
+      <c r="F131" t="s">
+        <v>168</v>
+      </c>
+      <c r="G131" t="s">
+        <v>30</v>
+      </c>
+      <c r="H131" t="s">
+        <v>10</v>
+      </c>
+      <c r="I131" t="s">
+        <v>11</v>
+      </c>
+      <c r="O131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>174</v>
+      </c>
+      <c r="B132">
+        <v>2024</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D132" t="s">
+        <v>161</v>
+      </c>
+      <c r="F132" t="s">
+        <v>169</v>
+      </c>
+      <c r="G132" t="s">
+        <v>30</v>
+      </c>
+      <c r="H132" t="s">
+        <v>10</v>
+      </c>
+      <c r="I132" t="s">
+        <v>11</v>
+      </c>
+      <c r="O132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>174</v>
+      </c>
+      <c r="B133">
+        <v>2024</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D133" t="s">
+        <v>162</v>
+      </c>
+      <c r="F133" t="s">
+        <v>170</v>
+      </c>
+      <c r="G133" t="s">
+        <v>30</v>
+      </c>
+      <c r="H133" t="s">
+        <v>10</v>
+      </c>
+      <c r="I133" t="s">
+        <v>11</v>
+      </c>
+      <c r="O133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>174</v>
+      </c>
+      <c r="B134">
+        <v>2024</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D134" t="s">
+        <v>163</v>
+      </c>
+      <c r="F134" t="s">
+        <v>171</v>
+      </c>
+      <c r="G134" t="s">
+        <v>30</v>
+      </c>
+      <c r="H134" t="s">
+        <v>10</v>
+      </c>
+      <c r="I134" t="s">
+        <v>11</v>
+      </c>
+      <c r="O134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>174</v>
+      </c>
+      <c r="B135">
+        <v>2024</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D135" t="s">
+        <v>164</v>
+      </c>
+      <c r="F135" t="s">
+        <v>172</v>
+      </c>
+      <c r="G135" t="s">
+        <v>30</v>
+      </c>
+      <c r="H135" t="s">
+        <v>10</v>
+      </c>
+      <c r="I135" t="s">
+        <v>11</v>
+      </c>
+      <c r="O135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>174</v>
+      </c>
+      <c r="B136">
+        <v>2024</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D136" t="s">
         <v>165</v>
       </c>
-      <c r="F128" t="s">
+      <c r="F136" t="s">
         <v>173</v>
       </c>
-      <c r="G128" t="s">
+      <c r="G136" t="s">
         <v>30</v>
       </c>
-      <c r="H128" t="s">
-        <v>10</v>
-      </c>
-      <c r="I128" t="s">
-        <v>11</v>
-      </c>
-      <c r="O128">
+      <c r="H136" t="s">
+        <v>10</v>
+      </c>
+      <c r="I136" t="s">
+        <v>11</v>
+      </c>
+      <c r="O136">
         <v>1</v>
       </c>
     </row>
@@ -5042,7 +5366,7 @@
     <hyperlink ref="C51" r:id="rId31" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{EDDD9F8D-F7A4-5E43-B44F-45FF2E5BB7C6}"/>
     <hyperlink ref="C52" r:id="rId32" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{4A2AAB32-D596-A549-A571-D384D3091028}"/>
     <hyperlink ref="C53" r:id="rId33" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{D8450049-7E05-5948-8B8D-7D886E7330B4}"/>
-    <hyperlink ref="E64" r:id="rId34" xr:uid="{B391B2BF-3E75-1345-9E6F-74B3074A31BD}"/>
+    <hyperlink ref="E72" r:id="rId34" xr:uid="{B391B2BF-3E75-1345-9E6F-74B3074A31BD}"/>
     <hyperlink ref="E2" r:id="rId35" xr:uid="{E191A043-72B0-CC4E-9B58-FE4C461D40C9}"/>
     <hyperlink ref="C14" r:id="rId36" display="https://doi.org/10.1038/s41467-024-47271-y" xr:uid="{88E6D632-2160-2B4D-AD77-9459075894C4}"/>
     <hyperlink ref="C13" r:id="rId37" display="https://doi.org/10.1038/s41467-024-47271-y" xr:uid="{ED18E71A-43E8-A644-BA73-C69B86D50DCF}"/>
@@ -5054,14 +5378,14 @@
     <hyperlink ref="C10" r:id="rId43" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{5EDBB7DA-D0A8-5C40-965B-765553AFD77F}"/>
     <hyperlink ref="C11" r:id="rId44" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{97A0DD07-EFF7-EA40-ACF2-1E199930B687}"/>
     <hyperlink ref="C12" r:id="rId45" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{F6A6BB47-C672-7F49-B245-2B27A22913F5}"/>
-    <hyperlink ref="C121" r:id="rId46" xr:uid="{501A2742-514A-AE41-A2A6-B64BEB7C049E}"/>
-    <hyperlink ref="C122" r:id="rId47" xr:uid="{84474B7C-BAD1-1C48-B481-FFCD2859CFE3}"/>
-    <hyperlink ref="C123" r:id="rId48" xr:uid="{8F95774A-3C26-EC45-A54B-6620B1F8DD8B}"/>
-    <hyperlink ref="C124" r:id="rId49" xr:uid="{B3872678-EA39-AA4E-AFE2-3D4E5C0E3234}"/>
-    <hyperlink ref="C125" r:id="rId50" xr:uid="{4BA9BDAA-D422-174B-B7BC-EF82A2B3A879}"/>
-    <hyperlink ref="C126" r:id="rId51" xr:uid="{474C7201-8B25-9F4B-A147-C5CE2B0702AB}"/>
-    <hyperlink ref="C127" r:id="rId52" xr:uid="{3CD58BFF-96D7-B144-B94C-6F1D42F7B3AF}"/>
-    <hyperlink ref="C128" r:id="rId53" xr:uid="{5229D856-741E-1F4D-8A70-F35E0AF5BAD6}"/>
+    <hyperlink ref="C129" r:id="rId46" xr:uid="{501A2742-514A-AE41-A2A6-B64BEB7C049E}"/>
+    <hyperlink ref="C130" r:id="rId47" xr:uid="{84474B7C-BAD1-1C48-B481-FFCD2859CFE3}"/>
+    <hyperlink ref="C131" r:id="rId48" xr:uid="{8F95774A-3C26-EC45-A54B-6620B1F8DD8B}"/>
+    <hyperlink ref="C132" r:id="rId49" xr:uid="{B3872678-EA39-AA4E-AFE2-3D4E5C0E3234}"/>
+    <hyperlink ref="C133" r:id="rId50" xr:uid="{4BA9BDAA-D422-174B-B7BC-EF82A2B3A879}"/>
+    <hyperlink ref="C134" r:id="rId51" xr:uid="{474C7201-8B25-9F4B-A147-C5CE2B0702AB}"/>
+    <hyperlink ref="C135" r:id="rId52" xr:uid="{3CD58BFF-96D7-B144-B94C-6F1D42F7B3AF}"/>
+    <hyperlink ref="C136" r:id="rId53" xr:uid="{5229D856-741E-1F4D-8A70-F35E0AF5BAD6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
add cosmx samples to csv
</commit_message>
<xml_diff>
--- a/Datasets_all.xlsx
+++ b/Datasets_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k23030440/Pseudovisium/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A97BF4B-3C51-2644-A060-F7CF260F0B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0861530B-15E5-2644-9338-8523A17B4841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="6380" windowWidth="28040" windowHeight="17440" xr2:uid="{419F9F52-EC29-7E45-8CDA-DBEF0D21635D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="247">
   <si>
     <t>Author</t>
   </si>
@@ -750,6 +750,33 @@
   </si>
   <si>
     <t>https://zm1oqa.bl.files.1drv.com/y4mg6GhhT2pXjR8Z07n6MfT1x_8KfVoMGXyqQVY6Iz2ttKka4oSddm8j-6D6BR2BZbaYurMp-0piwHKUNbMXyvmQYZA7o08bKmWgqmS6UZjMMKkU0gUayVX0Q1nWzF3EUg61_KZyFhsZ6pHZEWW68_4bU6E0MzUfykQl8VC1B8K2ZlJ3oNvoV3aDwuE7rUr-44eOixp552swhUzAwpfVHJTNQ</t>
+  </si>
+  <si>
+    <t>https://vgocqw.bl.files.1drv.com/y4mNw37uF9wd_xK0Q59qYpEtYmWsdnQT6OAmtNEiVvX-luZR6SbFmvplO7jD30dW1Uq9JLkMpA0qC9R5TvHgXRxeRXj5arXB0BSospaTgDzbdff_IoMuL3htinmILGBH0NYl74T6SqQq_JLOzkY1GcyIsan5E5tfZP5Y300CfL-PcdF-iIiz8-QtQxCxwtE8BzHfPnUPKjiXWpOxuLmB5FRTA</t>
+  </si>
+  <si>
+    <t>https://ifz0xa.bl.files.1drv.com/y4mTHM4bk8TtkZQkaJggGTC1iGPJQoPP0iZfdXVkKL2L7bzq9jgh2_amWkruy40nKOH_lcP8Y2A_Fek3J7XzALfPlkkJ8LI2FCkArLKtSeLjSLGwgqnVEtLEzfaKPl9Kxn2WcMMfFbzAF8WQ61Zcu9QIiSS_Vm9UODov2ixriNRQp9x_MKzyb3CiDZIl7aA0-IhR2fVXzZR32PfqxeN4oLY2g</t>
+  </si>
+  <si>
+    <t>https://8lnrra.bl.files.1drv.com/y4mhDToinyLHHx81QMnwp-79dC1YF5v-Vuwq4N7qkmtf6hHwuy_9ISUtZjBOvS55FRmMKGYz8-pKL05Oure7pZO9XCXV9Rqo7ptfRSwvTIGRuXGmqnq4todD1qvw1J-I8KZjiJxb13WCK2Zhrl1AegU5ASMABht1LKRkXQs-SVSQPbZnjiE9JB_kdpL_H_BQfWfhe0jEmbS8hpZSnOq_CVPow</t>
+  </si>
+  <si>
+    <t>https://hohnuq.bl.files.1drv.com/y4mKWx0U7VEExp1o3VrmlwAQELKMLf3aMSd8qHASSuSiuZgSl1ZxZZRH2RcLSlfihUhrR8BPq5Hr88ykOTt191KUjQD0Tl9_7o0ae4gI1OHiO2kW1YZ1inxlOLC7khOHUrlyhvYWFklAwzUVhxOooqf-wfJ3zJ715Sftb9BZ0nVtBJETqqXI-1GhWdujJIuz16yjjL3DvnkoH1VQ9qIJ7gi9A</t>
+  </si>
+  <si>
+    <t>https://kd26iq.bl.files.1drv.com/y4mtWoQzs3BK60ssvEP6GPYWbT7V4LqbqXjaS5E_tW_Q9pPhLZmkiSUKQ4amv2gG2yW2tx-Jduv4rGnhcHii1wS37li6fPh8u4S8sQp3FsnOSN8x8AoR-47QJTbGAe1BAm577OskS-omdDFuErJTaUnof4Cba33hkEhtfxMrXh3tG2DQTRT74G9Dzt_QVZHFJCKy9HlS0che6H-Z8hNWxKvpw</t>
+  </si>
+  <si>
+    <t>CosMx_nsclc_9_2</t>
+  </si>
+  <si>
+    <t>https://6wwmfw.bl.files.1drv.com/y4mtFdh7st4ROLi8ttKLd0RIRc09_5WSsqLivbKIOo-jUlcmRhlSMnpq4JSzQ1PebQuzKiEnGhmqcPATk2-kGQOk-ifvHy7UomUtS8HamIfRPWOcGd2N2VV7qX-AwwHmpAVkTYNgb3l1k0iO8y-KJCg6l5Liay75CjftQgFa3Dh7AOH7Aa0reYGAiNbIu19ATsDO_4TM4cUgYNdrfGDTkccgQ</t>
+  </si>
+  <si>
+    <t>https://zw1oqa.bl.files.1drv.com/y4mfFbvWw0PFhAAHx4QZZT1Z03ONHWTxk87yzM_hEs-cM78YgY1gUgKpGimwJqw89rx5LlNGRGe5Fp1uTcVKiq-6KPlNzd_ohcGfPSprfq-cW3AEWyTtZyZKJDtOP9JRee-4NZqHb4crj7cHHltPhAyiq40ogNQenhf2Hj-NBPW5VGDQZI_CLnXrJO_cdbNHHUVbKikY9r1JPD_G1kaHF9Gxg</t>
+  </si>
+  <si>
+    <t>https://v9qdoq.bl.files.1drv.com/y4mFR6AegFeiI9bU-0uO3bJPQ_xNSSVT4HARrAoLgJwzHiOeMJ1U36p4Pi3oyMtvOL4002GTyKtdUjaXTr_NBiq9KeccWLT7Dg6vzdWa6ggwQ2AYngYGPswvqW-P4Jiz0z-Leqgp0aKglqrWUXDZg6V7gi_xfadw5ymIyJ0YyBVagMnSbA6wSrvPaM-MYs49qCweGfkc4Nz6dwe4LYm2NPvCw</t>
   </si>
 </sst>
 </file>
@@ -1162,8 +1189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F01D6A24-CDB1-1E4B-87EB-E299D59C8055}">
   <dimension ref="A1:P136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1371,6 +1398,9 @@
       <c r="C5" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="E5" t="s">
+        <v>238</v>
+      </c>
       <c r="F5" t="s">
         <v>139</v>
       </c>
@@ -1412,6 +1442,9 @@
       <c r="C6" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="E6" t="s">
+        <v>239</v>
+      </c>
       <c r="F6" t="s">
         <v>140</v>
       </c>
@@ -1453,6 +1486,9 @@
       <c r="C7" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="E7" t="s">
+        <v>240</v>
+      </c>
       <c r="F7" t="s">
         <v>141</v>
       </c>
@@ -1494,6 +1530,9 @@
       <c r="C8" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="E8" t="s">
+        <v>241</v>
+      </c>
       <c r="F8" t="s">
         <v>142</v>
       </c>
@@ -1535,6 +1574,9 @@
       <c r="C9" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="E9" t="s">
+        <v>242</v>
+      </c>
       <c r="F9" t="s">
         <v>143</v>
       </c>
@@ -1576,8 +1618,11 @@
       <c r="C10" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="E10" t="s">
+        <v>244</v>
+      </c>
       <c r="F10" t="s">
-        <v>143</v>
+        <v>243</v>
       </c>
       <c r="G10" t="s">
         <v>137</v>
@@ -1617,6 +1662,9 @@
       <c r="C11" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="E11" t="s">
+        <v>245</v>
+      </c>
       <c r="F11" t="s">
         <v>144</v>
       </c>
@@ -1654,6 +1702,9 @@
       </c>
       <c r="C12" s="1" t="s">
         <v>147</v>
+      </c>
+      <c r="E12" t="s">
+        <v>246</v>
       </c>
       <c r="F12" t="s">
         <v>145</v>
@@ -5383,54 +5434,54 @@
     <hyperlink ref="C26" r:id="rId3" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{D024058B-65E6-7B46-8A4C-DBC60E16FDDB}"/>
     <hyperlink ref="E25" r:id="rId4" xr:uid="{81EBE112-4C5B-AA45-835C-1A9E9E25B84E}"/>
     <hyperlink ref="E22" r:id="rId5" xr:uid="{5BA81582-EC37-0D4D-B7A9-7AF8598A9DF2}"/>
-    <hyperlink ref="E54" r:id="rId6" xr:uid="{4D2D8028-39C7-A44F-964F-969588B0EFAA}"/>
-    <hyperlink ref="C27" r:id="rId7" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{8F9A199E-EC71-B249-AF59-FF24DB4609B1}"/>
-    <hyperlink ref="C28" r:id="rId8" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{853F30D2-01D5-1548-B4FF-52D758F3D556}"/>
-    <hyperlink ref="C29" r:id="rId9" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{C48DB5F5-21AE-CE4D-BB27-7CF2B2B712A7}"/>
-    <hyperlink ref="C30" r:id="rId10" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{9ED5901C-DC91-CC49-A723-A9C49A700057}"/>
-    <hyperlink ref="C31" r:id="rId11" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{681B51E0-45E0-AF4A-A5EE-28748A165692}"/>
-    <hyperlink ref="C32" r:id="rId12" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{BA262E0F-F122-CE49-B193-E111B00E4D19}"/>
-    <hyperlink ref="C33" r:id="rId13" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{2C9985A0-6AD7-9A41-9565-94AA54B8F20A}"/>
-    <hyperlink ref="C34" r:id="rId14" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{42C6419B-1F9C-464D-942C-629DBE1A763F}"/>
-    <hyperlink ref="C35" r:id="rId15" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{CFF16103-3C13-2B47-B8FA-7ED24283F351}"/>
-    <hyperlink ref="C36" r:id="rId16" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{E38CC7D2-2BD2-AC45-99BE-32F76871EC00}"/>
-    <hyperlink ref="C37" r:id="rId17" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{C9FC1701-99F3-314F-8A4C-4CCCDD235EA2}"/>
-    <hyperlink ref="C38" r:id="rId18" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{EC4E26BD-F1A6-2647-A8E9-40DA20AB83BF}"/>
-    <hyperlink ref="C39" r:id="rId19" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{B86C6F60-6096-CD42-B6D4-337F4666A137}"/>
-    <hyperlink ref="C40" r:id="rId20" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{33B4FEAD-F100-6845-A5C0-78998BA2E0AD}"/>
-    <hyperlink ref="C41" r:id="rId21" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{A7F28363-67D9-DE4F-8511-F087659BD3BB}"/>
-    <hyperlink ref="C42" r:id="rId22" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{C7DDCDCC-39CA-5A4A-9204-AC06FD62324C}"/>
-    <hyperlink ref="C43" r:id="rId23" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{CDD3098C-5532-2243-91DE-779275449D7C}"/>
-    <hyperlink ref="C44" r:id="rId24" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{2FDC7CE7-0E8D-7A43-B2CB-F08FEB0D0C86}"/>
-    <hyperlink ref="C45" r:id="rId25" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{3EAD12EB-7FAA-6644-8CD0-282CF442DD5F}"/>
-    <hyperlink ref="C46" r:id="rId26" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{37ED5057-FB64-104D-A1AD-880EE76BBBF6}"/>
-    <hyperlink ref="C47" r:id="rId27" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{919807C3-656E-5541-AC46-175D90A0E650}"/>
-    <hyperlink ref="C48" r:id="rId28" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{CFD73339-E4A6-F444-95CC-E5EF5306A91D}"/>
-    <hyperlink ref="C49" r:id="rId29" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{DE5BB967-701B-3A4E-9953-5C391D746A0E}"/>
-    <hyperlink ref="C50" r:id="rId30" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{9D9F29E0-C81C-7B44-9831-E6853C80A7FA}"/>
-    <hyperlink ref="C51" r:id="rId31" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{EDDD9F8D-F7A4-5E43-B44F-45FF2E5BB7C6}"/>
-    <hyperlink ref="C52" r:id="rId32" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{4A2AAB32-D596-A549-A571-D384D3091028}"/>
-    <hyperlink ref="C53" r:id="rId33" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{D8450049-7E05-5948-8B8D-7D886E7330B4}"/>
-    <hyperlink ref="E72" r:id="rId34" xr:uid="{B391B2BF-3E75-1345-9E6F-74B3074A31BD}"/>
-    <hyperlink ref="E2" r:id="rId35" xr:uid="{E191A043-72B0-CC4E-9B58-FE4C461D40C9}"/>
-    <hyperlink ref="C14" r:id="rId36" display="https://doi.org/10.1038/s41467-024-47271-y" xr:uid="{88E6D632-2160-2B4D-AD77-9459075894C4}"/>
-    <hyperlink ref="C13" r:id="rId37" display="https://doi.org/10.1038/s41467-024-47271-y" xr:uid="{ED18E71A-43E8-A644-BA73-C69B86D50DCF}"/>
-    <hyperlink ref="C5" r:id="rId38" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{38821B49-6042-5042-8428-B8BD186CF7FB}"/>
-    <hyperlink ref="C6" r:id="rId39" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{5C2B9BE0-AC88-2C45-87F0-F17854B8281E}"/>
-    <hyperlink ref="C7" r:id="rId40" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{2D68EF16-250B-CD4E-89AF-0D5B979194EB}"/>
-    <hyperlink ref="C8" r:id="rId41" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{FA19C14F-5330-E041-BF9D-07C424C85332}"/>
-    <hyperlink ref="C9" r:id="rId42" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{A3F8BBCD-8687-2947-AD87-50A2D562B7C0}"/>
-    <hyperlink ref="C10" r:id="rId43" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{5EDBB7DA-D0A8-5C40-965B-765553AFD77F}"/>
-    <hyperlink ref="C11" r:id="rId44" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{97A0DD07-EFF7-EA40-ACF2-1E199930B687}"/>
-    <hyperlink ref="C12" r:id="rId45" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{F6A6BB47-C672-7F49-B245-2B27A22913F5}"/>
-    <hyperlink ref="C129" r:id="rId46" xr:uid="{501A2742-514A-AE41-A2A6-B64BEB7C049E}"/>
-    <hyperlink ref="C130" r:id="rId47" xr:uid="{84474B7C-BAD1-1C48-B481-FFCD2859CFE3}"/>
-    <hyperlink ref="C131" r:id="rId48" xr:uid="{8F95774A-3C26-EC45-A54B-6620B1F8DD8B}"/>
-    <hyperlink ref="C132" r:id="rId49" xr:uid="{B3872678-EA39-AA4E-AFE2-3D4E5C0E3234}"/>
-    <hyperlink ref="C133" r:id="rId50" xr:uid="{4BA9BDAA-D422-174B-B7BC-EF82A2B3A879}"/>
-    <hyperlink ref="C134" r:id="rId51" xr:uid="{474C7201-8B25-9F4B-A147-C5CE2B0702AB}"/>
-    <hyperlink ref="C135" r:id="rId52" xr:uid="{3CD58BFF-96D7-B144-B94C-6F1D42F7B3AF}"/>
-    <hyperlink ref="C136" r:id="rId53" xr:uid="{5229D856-741E-1F4D-8A70-F35E0AF5BAD6}"/>
+    <hyperlink ref="C27" r:id="rId6" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{8F9A199E-EC71-B249-AF59-FF24DB4609B1}"/>
+    <hyperlink ref="C28" r:id="rId7" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{853F30D2-01D5-1548-B4FF-52D758F3D556}"/>
+    <hyperlink ref="C29" r:id="rId8" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{C48DB5F5-21AE-CE4D-BB27-7CF2B2B712A7}"/>
+    <hyperlink ref="C30" r:id="rId9" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{9ED5901C-DC91-CC49-A723-A9C49A700057}"/>
+    <hyperlink ref="C31" r:id="rId10" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{681B51E0-45E0-AF4A-A5EE-28748A165692}"/>
+    <hyperlink ref="C32" r:id="rId11" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{BA262E0F-F122-CE49-B193-E111B00E4D19}"/>
+    <hyperlink ref="C33" r:id="rId12" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{2C9985A0-6AD7-9A41-9565-94AA54B8F20A}"/>
+    <hyperlink ref="C34" r:id="rId13" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{42C6419B-1F9C-464D-942C-629DBE1A763F}"/>
+    <hyperlink ref="C35" r:id="rId14" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{CFF16103-3C13-2B47-B8FA-7ED24283F351}"/>
+    <hyperlink ref="C36" r:id="rId15" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{E38CC7D2-2BD2-AC45-99BE-32F76871EC00}"/>
+    <hyperlink ref="C37" r:id="rId16" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{C9FC1701-99F3-314F-8A4C-4CCCDD235EA2}"/>
+    <hyperlink ref="C38" r:id="rId17" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{EC4E26BD-F1A6-2647-A8E9-40DA20AB83BF}"/>
+    <hyperlink ref="C39" r:id="rId18" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{B86C6F60-6096-CD42-B6D4-337F4666A137}"/>
+    <hyperlink ref="C40" r:id="rId19" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{33B4FEAD-F100-6845-A5C0-78998BA2E0AD}"/>
+    <hyperlink ref="C41" r:id="rId20" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{A7F28363-67D9-DE4F-8511-F087659BD3BB}"/>
+    <hyperlink ref="C42" r:id="rId21" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{C7DDCDCC-39CA-5A4A-9204-AC06FD62324C}"/>
+    <hyperlink ref="C43" r:id="rId22" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{CDD3098C-5532-2243-91DE-779275449D7C}"/>
+    <hyperlink ref="C44" r:id="rId23" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{2FDC7CE7-0E8D-7A43-B2CB-F08FEB0D0C86}"/>
+    <hyperlink ref="C45" r:id="rId24" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{3EAD12EB-7FAA-6644-8CD0-282CF442DD5F}"/>
+    <hyperlink ref="C46" r:id="rId25" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{37ED5057-FB64-104D-A1AD-880EE76BBBF6}"/>
+    <hyperlink ref="C47" r:id="rId26" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{919807C3-656E-5541-AC46-175D90A0E650}"/>
+    <hyperlink ref="C48" r:id="rId27" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{CFD73339-E4A6-F444-95CC-E5EF5306A91D}"/>
+    <hyperlink ref="C49" r:id="rId28" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{DE5BB967-701B-3A4E-9953-5C391D746A0E}"/>
+    <hyperlink ref="C50" r:id="rId29" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{9D9F29E0-C81C-7B44-9831-E6853C80A7FA}"/>
+    <hyperlink ref="C51" r:id="rId30" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{EDDD9F8D-F7A4-5E43-B44F-45FF2E5BB7C6}"/>
+    <hyperlink ref="C52" r:id="rId31" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{4A2AAB32-D596-A549-A571-D384D3091028}"/>
+    <hyperlink ref="C53" r:id="rId32" display="https://doi.org/10.1101%2F2023.12.15.571954" xr:uid="{D8450049-7E05-5948-8B8D-7D886E7330B4}"/>
+    <hyperlink ref="E72" r:id="rId33" xr:uid="{B391B2BF-3E75-1345-9E6F-74B3074A31BD}"/>
+    <hyperlink ref="E2" r:id="rId34" xr:uid="{E191A043-72B0-CC4E-9B58-FE4C461D40C9}"/>
+    <hyperlink ref="C14" r:id="rId35" display="https://doi.org/10.1038/s41467-024-47271-y" xr:uid="{88E6D632-2160-2B4D-AD77-9459075894C4}"/>
+    <hyperlink ref="C13" r:id="rId36" display="https://doi.org/10.1038/s41467-024-47271-y" xr:uid="{ED18E71A-43E8-A644-BA73-C69B86D50DCF}"/>
+    <hyperlink ref="C5" r:id="rId37" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{38821B49-6042-5042-8428-B8BD186CF7FB}"/>
+    <hyperlink ref="C6" r:id="rId38" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{5C2B9BE0-AC88-2C45-87F0-F17854B8281E}"/>
+    <hyperlink ref="C7" r:id="rId39" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{2D68EF16-250B-CD4E-89AF-0D5B979194EB}"/>
+    <hyperlink ref="C8" r:id="rId40" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{FA19C14F-5330-E041-BF9D-07C424C85332}"/>
+    <hyperlink ref="C9" r:id="rId41" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{A3F8BBCD-8687-2947-AD87-50A2D562B7C0}"/>
+    <hyperlink ref="C10" r:id="rId42" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{5EDBB7DA-D0A8-5C40-965B-765553AFD77F}"/>
+    <hyperlink ref="C11" r:id="rId43" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{97A0DD07-EFF7-EA40-ACF2-1E199930B687}"/>
+    <hyperlink ref="C12" r:id="rId44" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{F6A6BB47-C672-7F49-B245-2B27A22913F5}"/>
+    <hyperlink ref="C129" r:id="rId45" xr:uid="{501A2742-514A-AE41-A2A6-B64BEB7C049E}"/>
+    <hyperlink ref="C130" r:id="rId46" xr:uid="{84474B7C-BAD1-1C48-B481-FFCD2859CFE3}"/>
+    <hyperlink ref="C131" r:id="rId47" xr:uid="{8F95774A-3C26-EC45-A54B-6620B1F8DD8B}"/>
+    <hyperlink ref="C132" r:id="rId48" xr:uid="{B3872678-EA39-AA4E-AFE2-3D4E5C0E3234}"/>
+    <hyperlink ref="C133" r:id="rId49" xr:uid="{4BA9BDAA-D422-174B-B7BC-EF82A2B3A879}"/>
+    <hyperlink ref="C134" r:id="rId50" xr:uid="{474C7201-8B25-9F4B-A147-C5CE2B0702AB}"/>
+    <hyperlink ref="C135" r:id="rId51" xr:uid="{3CD58BFF-96D7-B144-B94C-6F1D42F7B3AF}"/>
+    <hyperlink ref="C136" r:id="rId52" xr:uid="{5229D856-741E-1F4D-8A70-F35E0AF5BAD6}"/>
+    <hyperlink ref="E54" r:id="rId53" xr:uid="{4D2D8028-39C7-A44F-964F-969588B0EFAA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
updating csv, fixed merge and qc can handle squidpy now
</commit_message>
<xml_diff>
--- a/Datasets_all.xlsx
+++ b/Datasets_all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k23030440/Pseudovisium/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C495CA-3B6B-6747-A11F-157D121B6168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CE8B02-5685-2740-B69C-F752690DE32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="1220" windowWidth="28040" windowHeight="17440" xr2:uid="{419F9F52-EC29-7E45-8CDA-DBEF0D21635D}"/>
+    <workbookView xWindow="660" yWindow="840" windowWidth="28040" windowHeight="17440" xr2:uid="{419F9F52-EC29-7E45-8CDA-DBEF0D21635D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="319">
   <si>
     <t>Author</t>
   </si>
@@ -918,6 +918,81 @@
   </si>
   <si>
     <t>Just Visium example</t>
+  </si>
+  <si>
+    <t>Olfactory bulb</t>
+  </si>
+  <si>
+    <t>Embryo</t>
+  </si>
+  <si>
+    <t>https://www.10xgenomics.com/datasets/adult-mouse-olfactory-bulb-1-standard-1</t>
+  </si>
+  <si>
+    <t>https://www.10xgenomics.com/datasets/adult-mouse-kidney-ffpe-1-standard-1-3-0</t>
+  </si>
+  <si>
+    <t>https://www.10xgenomics.com/datasets/human-ovarian-cancer-1-standard</t>
+  </si>
+  <si>
+    <t>https://www.10xgenomics.com/datasets/human-breast-cancer-visium-fresh-frozen-whole-transcriptome-1-standard</t>
+  </si>
+  <si>
+    <t>https://www.10xgenomics.com/datasets/adult-mouse-brain-coronal-section-fresh-frozen-1-standard</t>
+  </si>
+  <si>
+    <t>https://www.10xgenomics.com/datasets/human-kidney-11-mm-capture-area-ffpe-2-standard</t>
+  </si>
+  <si>
+    <t>https://www.10xgenomics.com/datasets/visium-cytassist-mouse-embryo-11-mm-capture-area-ffpe-2-standard</t>
+  </si>
+  <si>
+    <t>Visium_olf_bulb</t>
+  </si>
+  <si>
+    <t>Visium_kidney_mouse</t>
+  </si>
+  <si>
+    <t>Visium_ovarian_cancer</t>
+  </si>
+  <si>
+    <t>Visium_breast_cancer</t>
+  </si>
+  <si>
+    <t>Visium_brain</t>
+  </si>
+  <si>
+    <t>Visium_kidney_human</t>
+  </si>
+  <si>
+    <t>Visium_embryo</t>
+  </si>
+  <si>
+    <t>https://x2ocbw.bl.files.1drv.com/y4mR1ZXpUQbQIM5hSm5DuE0RmG5mync6IyU8Iodp_RFed9yo_ueW7pSlAfrR4DBt5AqodE6EOPlzaWCL-nkCGI2G5qaEs8mdUaKpQ_Ls0FUe20j7Bo4Jh_U10utmDdvOQDEuDWHXN22SamMQkeiJjgDZPk8_WQlaQ-z_7Him8CH_If5rFUjwh0N5Hu5escMoloId2NFHR3rVvf41f8Wtw6Z1Q</t>
+  </si>
+  <si>
+    <t>https://9gwmhw.bl.files.1drv.com/y4m21lGsG84x5YvNlK65A5B6LkpxnX8NdK9AhhExllpnsfdRDHJla33U47c6opHZi6K0YoTJY54yriIsvhFU2t-D0zAZpjWmGCdoEMyjq2_F1JYsU6oqow5J5Dn0d_TDp9Cc2_shhh8OKqp-VvHSf9ihb4JNcMx9bE6bUxsUM7G6UEZqV9m9pMyTOQC9TN5JWHhKjMuPUsAo1TnBbxgJU3NYA</t>
+  </si>
+  <si>
+    <t>https://ytqaqq.bl.files.1drv.com/y4mUcOiBHdjDdYz1DvTXv4Z1gNumtEZy-i4SCfaZrOuhbZJ0EVeuXx4dNrMbqwDLVYWNa6lhuWkzN1A7-Q52KpV84jbUaXVlCSv4gxB7P46RCT6t5BzJhAIqKTr7Mfy79FiT-khixVHPHpdhG0xtfgIqE3VdcPq698O8DycPOJj4AOyM1fJd4RjtYzXlDIUhowDiJcWt2T9QGorV2GtPCzPgQ</t>
+  </si>
+  <si>
+    <t>https://qvnota.bl.files.1drv.com/y4mkTerst2qgO8awvj5KruxDYL_4YI2UKXKRZ1JzDY_-9q38xh-j_oBLaNqiKvXL5X8SWV02OuE5WLaIXMQl1A0T_T3vtK25ZMxMpKKRjrVg_fReIIgKznneVW9rrOFciAInR37ESJ-RYeT1Ay5nRJWpYCpp_OCtOgz1CAl5Usn_OpDTd-_N4ubKID2ncO985fBWxn3hHoFyhIaMX0EoAgwaw</t>
+  </si>
+  <si>
+    <t>https://cpl1pg.bl.files.1drv.com/y4mDy2m7jRRx9lJZmCLQOl0y1RyG5s85iu_dOhJnU6ICMLOyZS5hhVe8pIM9pjb_zq_ZT05dIbEDAAoU418Pz1NgxgGXyHHGK6js-ho2whljFAEcF8OkBm-G1asnkXr721e4wqb60H6Ly9jlwD0hZC6vzp5VRSQw62ABh_8tdZHIAvn6yWU9YRvdiWlHSo3uvCcukTZoeAie8bq_Kfc9XqUsQ</t>
+  </si>
+  <si>
+    <t>https://mz23kq.bl.files.1drv.com/y4mG0545nd3mPv2J2pYWehC_UoqaWMTvR6PqZnpHLhTlPZ9PaM0rh2GdYrdAygLYVHLnkcW13KKgTl6L6QgzNCJvTOT16oSmRf49h-2y4Smq3hN3bSmG0pIb9rDL9FmOfV_S_-88gtQ3Xe6LiHF-dXb2Y5rXxDmqVZH5NuMKgSkE6MQlbiHPnJsaDlnK8oI0nw_3QYjW59kgSjKCDQVl4kSag</t>
+  </si>
+  <si>
+    <t>https://cg1oba.bl.files.1drv.com/y4mx4UjKNpxmTky9p84tsyymM9CIpQ_JqEu5PJOlc9G7iix7xuYQmmQPw_sVLgMLsSI3FjDNiQE8XIe_NW72eThWHxkdY-6PZBhiT6Z9kCRzhUfYQqLvB_tqMABSD02FqjX0bSvQ60jKX9hzZhVlD4EjM2z1bWWuhmiTPIpOFPQzECsRNH_NyuwM5JtV4BmRaNNdAhumA3dDJr0V7XtzRmj4w</t>
+  </si>
+  <si>
+    <t>https://mmgp7w.bl.files.1drv.com/y4m6rrHukO15I4Z0ayjDqsKOjLK67QXYeORSWY_P7N9OW9BFqj1cIchXQ9XYsEmuQ6a4s_e-7EzEq5k5ue2SFV1id3QXPKuF58QgIy6SPOCHP7hgpv2Kq3xQZFmqhlAMrynE1NY0UUQZyF288igTxIJbjDxrJgPShPzhRKhRp1S5YorjDnKvcykv02ICqqPJZ-8hc_2nbEPrAfHvjcM_mICKA</t>
+  </si>
+  <si>
+    <t>https://kyhnwq.bl.files.1drv.com/y4mVei1sn6_3jISVzN2lgGJdq8JGByWfetd7S83TsBBEiBXjNuslaS55xKI4w3fIJAePL_putj1zH_Hl5AuaNn1epBqNhn6tsApjM_bMzn268fwpRDS4LNnzcbFUBN4SWYqIG4ue4maGC0bAbAsANZaXAXxy5tTdIjEn1VpboBvN6Y8Ds03djdxlEKigWwo45IP7soSzNSJ18NJaCws7nENZw</t>
   </si>
 </sst>
 </file>
@@ -1328,10 +1403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F01D6A24-CDB1-1E4B-87EB-E299D59C8055}">
-  <dimension ref="A1:R107"/>
+  <dimension ref="A1:R113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2107,6 +2182,9 @@
       <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="E16" t="s">
+        <v>310</v>
+      </c>
       <c r="G16" t="s">
         <v>13</v>
       </c>
@@ -2148,6 +2226,9 @@
       <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="E17" t="s">
+        <v>311</v>
+      </c>
       <c r="G17" t="s">
         <v>17</v>
       </c>
@@ -5329,7 +5410,7 @@
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>43</v>
+        <v>167</v>
       </c>
       <c r="B99">
         <v>2024</v>
@@ -5573,7 +5654,205 @@
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>167</v>
+        <v>18</v>
+      </c>
+      <c r="B107">
+        <v>2024</v>
+      </c>
+      <c r="D107" t="s">
+        <v>296</v>
+      </c>
+      <c r="E107" t="s">
+        <v>318</v>
+      </c>
+      <c r="F107" t="s">
+        <v>303</v>
+      </c>
+      <c r="G107" t="s">
+        <v>29</v>
+      </c>
+      <c r="H107" t="s">
+        <v>294</v>
+      </c>
+      <c r="I107" t="s">
+        <v>11</v>
+      </c>
+      <c r="M107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>18</v>
+      </c>
+      <c r="B108">
+        <v>2024</v>
+      </c>
+      <c r="D108" t="s">
+        <v>297</v>
+      </c>
+      <c r="E108" t="s">
+        <v>316</v>
+      </c>
+      <c r="F108" t="s">
+        <v>304</v>
+      </c>
+      <c r="G108" t="s">
+        <v>29</v>
+      </c>
+      <c r="H108" t="s">
+        <v>35</v>
+      </c>
+      <c r="I108" t="s">
+        <v>11</v>
+      </c>
+      <c r="M108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>18</v>
+      </c>
+      <c r="B109">
+        <v>2024</v>
+      </c>
+      <c r="D109" t="s">
+        <v>298</v>
+      </c>
+      <c r="E109" t="s">
+        <v>315</v>
+      </c>
+      <c r="F109" t="s">
+        <v>305</v>
+      </c>
+      <c r="G109" t="s">
+        <v>29</v>
+      </c>
+      <c r="H109" t="s">
+        <v>212</v>
+      </c>
+      <c r="I109" t="s">
+        <v>12</v>
+      </c>
+      <c r="M109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>18</v>
+      </c>
+      <c r="B110">
+        <v>2024</v>
+      </c>
+      <c r="D110" t="s">
+        <v>299</v>
+      </c>
+      <c r="E110" t="s">
+        <v>317</v>
+      </c>
+      <c r="F110" t="s">
+        <v>306</v>
+      </c>
+      <c r="G110" t="s">
+        <v>29</v>
+      </c>
+      <c r="H110" t="s">
+        <v>21</v>
+      </c>
+      <c r="I110" t="s">
+        <v>12</v>
+      </c>
+      <c r="M110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>18</v>
+      </c>
+      <c r="B111">
+        <v>2024</v>
+      </c>
+      <c r="D111" t="s">
+        <v>300</v>
+      </c>
+      <c r="E111" t="s">
+        <v>314</v>
+      </c>
+      <c r="F111" t="s">
+        <v>307</v>
+      </c>
+      <c r="G111" t="s">
+        <v>29</v>
+      </c>
+      <c r="H111" t="s">
+        <v>10</v>
+      </c>
+      <c r="I111" t="s">
+        <v>11</v>
+      </c>
+      <c r="M111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>18</v>
+      </c>
+      <c r="B112">
+        <v>2024</v>
+      </c>
+      <c r="D112" t="s">
+        <v>301</v>
+      </c>
+      <c r="E112" t="s">
+        <v>312</v>
+      </c>
+      <c r="F112" t="s">
+        <v>308</v>
+      </c>
+      <c r="G112" t="s">
+        <v>29</v>
+      </c>
+      <c r="H112" t="s">
+        <v>35</v>
+      </c>
+      <c r="I112" t="s">
+        <v>12</v>
+      </c>
+      <c r="M112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>18</v>
+      </c>
+      <c r="B113">
+        <v>2024</v>
+      </c>
+      <c r="D113" t="s">
+        <v>302</v>
+      </c>
+      <c r="E113" t="s">
+        <v>313</v>
+      </c>
+      <c r="F113" t="s">
+        <v>309</v>
+      </c>
+      <c r="G113" t="s">
+        <v>29</v>
+      </c>
+      <c r="H113" t="s">
+        <v>295</v>
+      </c>
+      <c r="I113" t="s">
+        <v>11</v>
+      </c>
+      <c r="M113">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding new generate and merge
</commit_message>
<xml_diff>
--- a/Datasets_all.xlsx
+++ b/Datasets_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k23030440/Pseudovisium/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B611964-9537-7046-AA66-71A67A720EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E929945C-1CB7-7349-AF0B-BC2C3DCB2F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="840" windowWidth="28040" windowHeight="17440" xr2:uid="{419F9F52-EC29-7E45-8CDA-DBEF0D21635D}"/>
   </bookViews>
@@ -1531,8 +1531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F01D6A24-CDB1-1E4B-87EB-E299D59C8055}">
   <dimension ref="A1:Q150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="68" workbookViewId="0">
-      <selection activeCell="N93" sqref="N93"/>
+    <sheetView tabSelected="1" topLeftCell="D65" zoomScale="68" workbookViewId="0">
+      <selection activeCell="O91" sqref="O91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
adding new visium datasets
</commit_message>
<xml_diff>
--- a/Datasets_all.xlsx
+++ b/Datasets_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k23030440/Pseudovisium/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F57566-04BC-2C4D-BF1E-6E9E94B0DC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207FB4CF-6CE0-9E45-9D15-4979A0C24657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="840" windowWidth="28040" windowHeight="17440" xr2:uid="{419F9F52-EC29-7E45-8CDA-DBEF0D21635D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="475">
   <si>
     <t>Author</t>
   </si>
@@ -1434,6 +1434,33 @@
   </si>
   <si>
     <t>Vizgen_brain_human</t>
+  </si>
+  <si>
+    <t>https://pqx5pw.bl.files.1drv.com/y4m1k6YonJXGKLiTulGsOp45us7JXJW0ZNI8hvZyeP7VbGYl11HgNc0TYiyDl9epflO41wJtZry2ViDHRCeS5jiW7CLkvYZQYgOg3SSTn-fLaJBpYjiIUZqMFG43VbM6FsUDlwmBhSs7EoEAxCYqLKHuWvJdzE_-xzvWOok3vPNUfzsNua3hTmUOoTtX907r7EjT-QTaPexJEhXESeS-nOh4w</t>
+  </si>
+  <si>
+    <t>https://zd8wmg.bl.files.1drv.com/y4mFIuvFG-rUmDJoLUuDFGNdX7z03MkzD_zewYoUBb5jICcDIcmrbHvW7ynOwYR1xnOQjtRb_4N4Yf--ZyRmCeqm8BFn7ooddnBo32j5Yy8zJzNZMJzDj5fdLYNVl7TzeOZKEQngnfI_vArehdRicQJ3pl0s5ruyyLFlqTZJYypF2NGQMRsTHEP56lVXp-b-lV8Dci5VIxjvjaniXjrXGYVHQ</t>
+  </si>
+  <si>
+    <t>https://c22gja.bl.files.1drv.com/y4mnUBXRZRVrZbMZyX5GjvNiFA-b1DkBDlXxpaJ8_bUjFZAyaMIDdtCZO-iG7rbchhTp7MHmtih05MWDGIDGNQqhUZzCKtLG5tMe4_sBpzOqTHtaQHERNKwRzBAEIW655-YBaHCwjWi_vYaNZa8F0IXRVAtye-NPQvSqQZRcBlhrM33Z6Q8Cp03BzLZ5ELZq0yK8_V-cMu0W-oz8XGMAUj6_g</t>
+  </si>
+  <si>
+    <t>https://pqx4pw.bl.files.1drv.com/y4mHCAIZBINAkxCOXgDq7kv5h0ibgonQrRMKhaqJfaCChN6eKA2qj_0fLrg6RtA2GdCsaC_VKlXr9jfKjZ8nLTm8ziKge7AGTjFAkpK00oguWuYUAflBzp6dfbmAFJbvRr5l_rxDVTFo7PTkaU4o2QEFulNg0UgB7D5wVQD6Ty8cSoHyic27HDFVuzRWsy95Qdc7uD1EEZsCI1GOyCKMfRnMQ</t>
+  </si>
+  <si>
+    <t>https://nj0ngg.bl.files.1drv.com/y4mJrLwNG_RYvQ0ua_r35d7NzQCjlppFTco6sc7C-RBR_JtVyUrqR7_5sh12Lwosv8Io2FDy9f_pauOGBLzAO57VmKGuGikPKQF5KE6rnN9ghG5Vgw7PSaEmjIt09FLQmhEH1Fx6OONripDvE0ZoMbSJr_utDdvNz2EUolQkwrdIN8AY_9MQfUq-2uaVEc6AHCA4bV3hV6fuWZGIDlJpb7UXg</t>
+  </si>
+  <si>
+    <t>https://afsp1a.bl.files.1drv.com/y4mn-IJZI3jP6_fAWmwU3BDC-2bVf1kYE3V4sJzxnk5XI2erTQ9tOvFDIMXgRZ8gCGRx0ktJDyt6W9FMZRaQRYZfJ-s3iCbqGIkGt4d3Us4rZrwFFdO8kNAyFlbPy0x47q68-pNd3BWs0pilOV-VFzXhMUsR5VUQMpPxsDgQtyor1lQ-UTkWJTD_qpGNdmEWQEUAJTnIXIaXyRk9LSSe0Ljnw</t>
+  </si>
+  <si>
+    <t>https://m8hldw.bl.files.1drv.com/y4mMEnF8k7nptGLvyoPmagBwnXxGpnIAdKQZziLupRelp2Npz0hefGTcaCpTguAJyVLOS7i_DYLyaF1A2pB1bRVvO80lrvyMdFgrcqSO29G4zz7NFKbs58C7zmfoxwMgElFLeDvP-zt8P_2tdeBmVtQt37a-yupT6Mt_wpI3v6ADou9_lRCvHK9ZrKgh69htw_qd_-JUNTwrmEG1gNq5jDW7g</t>
+  </si>
+  <si>
+    <t>https://liefsg.bl.files.1drv.com/y4mBz9z742JfXYOZ8SecerzSh5y3_37M6LJilb7LjMrpgglvGYJTKYNBE9l_4rs4kGb0R5q75m6NdW-terLoY8v1DRJ9CnleIlOIrzs-9czBbkmyuhyzFFjSJdl8iFGm2W7U-joHnaK-TVY_DqRt9HHlH70JdHtpaSyfgmvHsuLbUhrIbZ1MiDiK95hna65WmKDY8oRW3JFv12lp2GnrJ-Psw</t>
+  </si>
+  <si>
+    <t>https://dujhlw.bl.files.1drv.com/y4m3-C5tVnhLqMdZfTl3rDhHPXbNkxSXhjm58LF330E6XaDsi-y1v-Et6quwg8CPE9NW8cxTYB28qgn1lwuIFqZHroef68_Z2U9Xq9ZjwCd07qma2pnRILtV6dXrFWBLh4lZFexi34LyfeLZ5IdOlZJ5lpx45GWZ74luVsprEFcFY54r_q9bkOCGDCtcjLk02FQmhZ63VucXDLvSvEqy_USdg</t>
   </si>
 </sst>
 </file>
@@ -1861,8 +1888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F01D6A24-CDB1-1E4B-87EB-E299D59C8055}">
   <dimension ref="A1:Q181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="75" workbookViewId="0">
-      <selection activeCell="F126" sqref="F126"/>
+    <sheetView tabSelected="1" topLeftCell="D127" zoomScale="75" workbookViewId="0">
+      <selection activeCell="O159" sqref="O159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9020,7 +9047,9 @@
       <c r="D157" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="E157" s="5"/>
+      <c r="E157" s="5" t="s">
+        <v>467</v>
+      </c>
       <c r="F157" t="s">
         <v>425</v>
       </c>
@@ -9037,7 +9066,9 @@
       <c r="K157" s="4"/>
       <c r="M157" s="4"/>
       <c r="N157" s="4"/>
-      <c r="O157" s="4"/>
+      <c r="O157" s="4">
+        <v>1</v>
+      </c>
       <c r="P157" s="4"/>
       <c r="Q157" s="4"/>
     </row>
@@ -9048,7 +9079,9 @@
       <c r="D158" s="5" t="s">
         <v>397</v>
       </c>
-      <c r="E158" s="5"/>
+      <c r="E158" s="1" t="s">
+        <v>466</v>
+      </c>
       <c r="F158" t="s">
         <v>426</v>
       </c>
@@ -9076,7 +9109,9 @@
       <c r="D159" s="5" t="s">
         <v>398</v>
       </c>
-      <c r="E159" s="5"/>
+      <c r="E159" s="5" t="s">
+        <v>468</v>
+      </c>
       <c r="F159" t="s">
         <v>427</v>
       </c>
@@ -9104,7 +9139,9 @@
       <c r="D160" s="5" t="s">
         <v>399</v>
       </c>
-      <c r="E160" s="5"/>
+      <c r="E160" s="5" t="s">
+        <v>469</v>
+      </c>
       <c r="F160" t="s">
         <v>428</v>
       </c>
@@ -9132,7 +9169,9 @@
       <c r="D161" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="E161" s="5"/>
+      <c r="E161" s="5" t="s">
+        <v>470</v>
+      </c>
       <c r="F161" t="s">
         <v>429</v>
       </c>
@@ -9160,7 +9199,9 @@
       <c r="D162" s="6" t="s">
         <v>401</v>
       </c>
-      <c r="E162" s="5"/>
+      <c r="E162" s="5" t="s">
+        <v>471</v>
+      </c>
       <c r="F162" t="s">
         <v>427</v>
       </c>
@@ -9190,7 +9231,9 @@
       <c r="D163" s="5" t="s">
         <v>402</v>
       </c>
-      <c r="E163" s="5"/>
+      <c r="E163" s="5" t="s">
+        <v>472</v>
+      </c>
       <c r="F163" t="s">
         <v>430</v>
       </c>
@@ -9218,7 +9261,9 @@
       <c r="D164" s="5" t="s">
         <v>403</v>
       </c>
-      <c r="E164" s="5"/>
+      <c r="E164" s="5" t="s">
+        <v>473</v>
+      </c>
       <c r="F164" t="s">
         <v>431</v>
       </c>
@@ -9246,7 +9291,9 @@
       <c r="D165" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="E165" s="5"/>
+      <c r="E165" s="5" t="s">
+        <v>474</v>
+      </c>
       <c r="F165" t="s">
         <v>432</v>
       </c>

</xml_diff>

<commit_message>
finished adding new datasets, added a bunch of new visium hd
</commit_message>
<xml_diff>
--- a/Datasets_all.xlsx
+++ b/Datasets_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k23030440/Pseudovisium/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD03339-85D9-BE48-8327-8FD9D9D69583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C3A0C9-AB8D-3C46-B0BB-5A97D2E36637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="840" windowWidth="28040" windowHeight="17440" xr2:uid="{419F9F52-EC29-7E45-8CDA-DBEF0D21635D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="501">
   <si>
     <t>Author</t>
   </si>
@@ -1470,6 +1470,75 @@
   </si>
   <si>
     <t>Xenium_v1_lung_cancer2_human</t>
+  </si>
+  <si>
+    <t>Visium_HD_lung_cancer_human3_2um</t>
+  </si>
+  <si>
+    <t>Visium_HD_lung_cancer_human3_8um</t>
+  </si>
+  <si>
+    <t>https://jshldw.bl.files.1drv.com/y4ms6MqCzziW652_gRjGegkl8zUecHfAuyGV6v5JvUts1F809NPVh-nkQpvmifnMjp5PnqClhWhBqs7T2OuGW9tSi5qdOKQIjn17iNwE8CLj1a_wg3yb37RTBBbsbrAuFKTXvQPOCxJhtyhjpfG2NNlh86ryi4DKyYQ0pPzSLYNPaCbubrOgsBBbddHcTgqqKdmTkguHvzNufxkFmow2Fa3Pw</t>
+  </si>
+  <si>
+    <t>https://kt0ngg.bl.files.1drv.com/y4mz5t8W4MeN-UD7VoAZwwF843BEY5lP_zqa3TUFfz7YlN2UOEP9SsVD2cwbLZdL2yc7tTerLaRtOHNAwc4S87OR6NngIu84pvSKjIkU7VkWlZkfNVwx5x6vdr7RLsd4j3C5q18cWAO7bIuwO6wlb3s_QNyn-yNcX8PlWRZ_c41L23g0wF8xzNqFIECPhWnqSywyKJsT1sNGTskUAFMgDlKkg</t>
+  </si>
+  <si>
+    <t>https://wn8wmg.bl.files.1drv.com/y4mCGYfIaZ5lJLFvf7AkP5eZGerbGXT7RnCkre5ks5qcZUdfRZkm3wLXkjjOpaqiAlT5pIjGCqAX6lilcJGi-aWZIKR91FMNGK1mNxRSWcFq8CffiZHv6-njkwPgw8hF1v36cq5LInwTh82PtmcW00hmrKJMtlA5WMSqS3C_wD_SoKKNKB7k8_fr84iHbJz6UC9HMMko8-9vHBuAFIb9PdYWA</t>
+  </si>
+  <si>
+    <t>https://81op1a.bl.files.1drv.com/y4m-obTU4A9lnX79sd7-Zr9WlYcbd76wa12JqzSTgSbj49FmahDZKKpFUXAjZkU7UvIEpEupip1iENWQsMURt9r4ANEj3t9qULnOP_TRT2jOiycxFpEuqJ1dyWJ1frTaYMGAFqLYKDqdU08swoY6AsL4NNS2cM6WxnnByrwdMjq0FPgY_-hfJmW4AQ6bIFiv4XvaUZuMd5IKJjfSXL6jzXklQ</t>
+  </si>
+  <si>
+    <t>https://ivbh7a.bl.files.1drv.com/y4meRFX-F6jTxQ6n0n2_UIgiIGW9eqgCVPcodLArcSZ343fAdLtw5C0-pgphyzrcGGNOfIMHpj3LGqfRiJiH3Lq7QkrhOwMSi97l1rK1UnwtxXZooalj8oNBN55UTAL8hyDpKAPGPPj_m98KW72vNPRID6N1iGeNuwfmB6HNpuzdKfDnav1-uP8jDHqzO5XWYUPR1oIzevh-q5VCfLpNeDyAA</t>
+  </si>
+  <si>
+    <t>https://vwpvjw.bl.files.1drv.com/y4mJRTgOJPuW-m5wRmqEvPlwpXKkmLuU0KHOGgTYFtZN_ZvzCcVVrNGVjYtxpZaKDu5CMsxB1dmpUitKepE0gOIPWOcoxhl5qWvlrMz82lavtCQkrxfwcbr4dNE1GRzdq17uKq3iTCDLFlLSRE8E7_nRAz9G_oScteDZgEup4PovjdizIEyXV6H_znXjLaZ-EnnZPso6cZkyJuhSb6xKkBbyA</t>
+  </si>
+  <si>
+    <t>https://7ax5pw.bl.files.1drv.com/y4mJg0TYEL6d8Mn87Krtzuh9ogOncpj8d8HCKWJFFDJRP4Eg0wk8T5L2q7c6FUgIe3oY-dmc-5V1Eu65b4WZORhp72X6sWQhbi69VCyGn1dZmJvm894U_idUIDDYI9SRzg6w2kgsUVV4DwxAtJRPv4npVu5FnfTPbGI5TVDyxXQBlQCtcjOfYCvHAavtZTxXluSScoriRuosojho-v54dDlzQ</t>
+  </si>
+  <si>
+    <t>https://h4egsg.bl.files.1drv.com/y4mUto0V4A0OZFEX9GwrOyJXPDk4cHw9U94G-qJNOHXu2UPp_tw3aMw6zw2MZP7GywzeFQUug3s18ZEIzv8ytrVOVzReZKp8Upd1OGkzpGqLEn_fyzg3MBCSYt7pchfZkTECTMjWm2o6T56VOe3LMU9jQtTh7MgkFXPwSCCeYXP5h_a--wzTamlNMautaPj0ZSRdOngtVpUdE8swZfseRD2GQ</t>
+  </si>
+  <si>
+    <t>https://zm2hja.bl.files.1drv.com/y4m6jGCEz66BiGn116llU2b6oH6IECD6CvXBOkFz7MXF9SzMiAozL-sBpCspwy83ti0UJX3c5O1IqPks8rXeK2HwZJ3lxErF9BeN0fZD_jNV43p5TPW99gN00tLeY3q_t7JfwaImAabq__OuELRixEVze66aBCdouzv65iiSx6XphB_cJMH5v5OcN3Yqwn2MotqosSN4dz6Dr0vjUWVAM31_w</t>
+  </si>
+  <si>
+    <t>https://aejilw.bl.files.1drv.com/y4mvvlnaNeXukYu_mcdR0jtMA-O6tvrC_VbF9117PWEoVH8inX7YwaoGHguwU_KnpRP1z25q7DwoBNDW8zKo2hUfD7J_hnajsNGY8gqIbzp7POoSd-0VtKr0K_Ueri2SZpz27pqjFAXuHDaA5NjXg3vBHRsyVfXJgeAZh3tXutFbuVPObw08JNE6SW0d1Lck-AfdppqraefUxB8PtRIuFX_kw</t>
+  </si>
+  <si>
+    <t>https://jchcdw.bl.files.1drv.com/y4mwM-46GB7Nwx03K4-mNbsIa6IByHTABfGtrEviIyQqaWPYj9WLPwWhwYozo6J2yqDznWTi8UmoNqQWUnNiuJVVsrlrbL9EozsKzNzPjOY64D-esAdKp-42WqTo_OLcSP5nZlLOW8CcKtOOFzUQQaWaVnStARarmUHw1jlLLMUGyVqiWH3Xu_VHUO3nQ6MPbh30ZyDSTreTRWLW4fyL4juWA</t>
+  </si>
+  <si>
+    <t>https://kd0egg.bl.files.1drv.com/y4mYWK0E8ZacI5DtfnG_3myU3KRS14v8qiRlk_tMDeNSdmOb5jEsBkCmBIl0YTofZtzZm66wTBfioU32KG87iQwuoGO2LyiYZhjkZLX5Ytm6G3ByQ3Dga6EAPPGIu3K0q-JGmEvm80C0DWUmdi9bJDudexY0PT8e72-0dnL7kS6PeAZw2ZDtEpPXMHrZ5I4cMT-j5rz9-z2Rvk_IFdklUGm7g</t>
+  </si>
+  <si>
+    <t>https://ifap7a.bl.files.1drv.com/y4mPMOeI5_XlU7ZpirwHzmQ5YNHfLX4EMqIK59wi8yfdEVf7dcKinMnCdpnAzeq6CSTO-ECJJDKsDY5sqLPuzJBVxTBWWC9eJdWh25m8LQS8eLlR9ptkpzMFPZ_TL9C9HoPcrfE5dDhj9x6OyrczizPIiiGSZjmvhgRFID_c22KUo6j4yWDoAzCgufQd0e8ftOc2a7uBAE7fh4wYe7sFfQ0wA</t>
+  </si>
+  <si>
+    <t>https://8lo11a.bl.files.1drv.com/y4mKkHuevQWyZ_lc2GDyKHAdPTO-kjxsj_uuOpc8PD5oDFhBsPerggEzClq46J5_Dm3h3MoAZM76VY8sdaxwnwxdGWv_qAwOmyIw8XpketYucp5M2TBtSlBvOYLu5NkU6Z7WkYRt7pppd_vnY-WJIuCXDBLetkyTZ51NMnTLmbFU1T-IFFWhn2j5hJ2RkqimPu8v9pSykaYbVJ26H0AozL8Uw</t>
+  </si>
+  <si>
+    <t>https://v98nmg.bl.files.1drv.com/y4m2da2t0Ei3WvZaXfcgzKA9lJLTvTE3zjIKDXX_yV4HG52McfqJA2czgdNV1r7XZNzpig-HCoHVjxfPg0LUyjWKodJKwF3FA5WXN7v678pzekgVqNan-ADvQFF8ayAH2OXKnwQuY91XV57lirTp-avydgfoeDSHjdMXMDRZkmy940NCLnJQA86KzV7Q8m0Tpr7ea0gEF_DMfITp6OYwhskfg</t>
+  </si>
+  <si>
+    <t>https://6wxwpw.bl.files.1drv.com/y4m8EngY_ETt3BFBDbjbRS_3M9o56Dpb-D81deYFMolQHCtkutHMxITGSOZNNdEcIDQpUWdXZlSveTcQVoHS1dzBl5feins_KPeI-nOjxW9RICWdbHm5zmti30RJ4a2Mj6_6S5S1KBtRxVuKkvk0PjXMN4d5h4SoNXiDfNQwRf_ATgb6dhnhuSI6IOzkXxBt5wfIh0eSxmVXjlBkA3FzZUn8Q</t>
+  </si>
+  <si>
+    <t>https://vgpmjw.bl.files.1drv.com/y4m2OMoEElIzONqZccUAKD57PDI3W9fF532_G7gOK0DXoj-vTCXpV0279_iGphabaE4pq7gHkvHUNIcyjOz75Q4uQIyVshF18q5_Zxo0iMF_4HpZR8yfjYbOqkrYYTWaJcL_6dR7QpJO4mb_BvX7g4JZ3fD9_BsBfWNnaqOyXDWRsl-vkCtvPB2d8a4ca6dfKX3aD-Ld-6B7P7peumLT68jwQ</t>
+  </si>
+  <si>
+    <t>https://hoexsg.bl.files.1drv.com/y4m21L4G71p8bEi4lBK-H9dFvCeKOvi8N_X8MYj1CLMhN_DCuS3v6OCGsDUxe1lcl4eQBxCf1G67J2oLHxx4n2FfY1hqWyv63_uzQGLEYRBL4UTtdIoiGF6TVHb3fhSi437jKF6VDo1wveHVYX4poZZSu3K0GgxrTpjA1r07pPcNUcs2-pBjWOp17GrYGHbF8IDxPt5TFZQ4nwZ2JTg1_0lKg</t>
+  </si>
+  <si>
+    <t>https://zw2yja.bl.files.1drv.com/y4m1mvzcl219IK1A5RtwTfy-uARuI8jViAoYGfCkV7B57OSQq4VimfMB3kuQyBvt3vwWNdIftkTNWxZg4EvQt920COzw4B-oF5PMp6K0a30awnIYc09TwGj0xGMw9BYg8v9E0uWE76u_QODoc8KOjV2hjnB7JdIqTueNz7pd7AowygBS_kUvRUmOxPD4VXMl7EQulWqqKtV2R0Ryn7YWtqUog</t>
+  </si>
+  <si>
+    <t>https://aoiqlw.bl.files.1drv.com/y4mNno8jvpBDZNFeVACdWmQNcftqa6OQWJzBGKwnTkC1zxqyvsHpHrlXcemspLoW0be-zXf8UXUwwi3Fbye5RDkMvrhUnfTMe5xGZNk2Mt1-Ul_SFDw6EPe9wiGQPvN2LX0gw9aSrVYHnLJS-QWd8UZm3TJw9TNnCkxedzGA9eiytugxU0UCxDCat_oSCtnizxt3bOy-hdCBvy7HCo397ps7g</t>
+  </si>
+  <si>
+    <t>https://jchddw.bl.files.1drv.com/y4mwrSptDF4BrTN5ZtNI-wDnMoBIEHdAYvdth5qtX9faEceGQPC0oZvGE0zEzhHla25-wc6CJfRA4wt3DgkR-wX-BQ40OkeWfdkGSkK2GMfgDNr5lcJPgbajTnmGMLC2yv0gateulIEdOrGfR3L8P3ksM7UYDzyTk3CEs27F8WDNpFiNsHaNMwLFJW3GM1uLPrr6mVxwa_SL7A9XJIBKRg5jQ</t>
   </si>
 </sst>
 </file>
@@ -1895,10 +1964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F01D6A24-CDB1-1E4B-87EB-E299D59C8055}">
-  <dimension ref="A1:Q181"/>
+  <dimension ref="A1:Q183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C53" zoomScale="63" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="D131" sqref="D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5008,6 +5077,9 @@
       <c r="K60">
         <v>1</v>
       </c>
+      <c r="L60">
+        <v>1</v>
+      </c>
       <c r="N60" s="4"/>
       <c r="P60" s="4"/>
     </row>
@@ -5040,6 +5112,9 @@
       <c r="K61">
         <v>1</v>
       </c>
+      <c r="L61">
+        <v>1</v>
+      </c>
       <c r="N61" s="4"/>
       <c r="P61" s="4"/>
     </row>
@@ -5072,6 +5147,9 @@
       <c r="K62">
         <v>1</v>
       </c>
+      <c r="L62">
+        <v>1</v>
+      </c>
       <c r="N62" s="4"/>
       <c r="O62">
         <v>1</v>
@@ -5107,6 +5185,9 @@
       <c r="K63">
         <v>1</v>
       </c>
+      <c r="L63">
+        <v>1</v>
+      </c>
       <c r="N63" s="4"/>
       <c r="P63" s="4"/>
     </row>
@@ -5139,6 +5220,9 @@
       <c r="K64">
         <v>1</v>
       </c>
+      <c r="L64">
+        <v>1</v>
+      </c>
       <c r="N64" s="4"/>
       <c r="P64" s="4"/>
     </row>
@@ -5171,6 +5255,9 @@
       <c r="K65">
         <v>1</v>
       </c>
+      <c r="L65">
+        <v>1</v>
+      </c>
       <c r="N65" s="4"/>
       <c r="P65" s="4"/>
     </row>
@@ -5203,6 +5290,9 @@
       <c r="K66">
         <v>1</v>
       </c>
+      <c r="L66">
+        <v>1</v>
+      </c>
       <c r="N66" s="4"/>
       <c r="P66" s="4"/>
     </row>
@@ -5235,6 +5325,9 @@
       <c r="K67">
         <v>1</v>
       </c>
+      <c r="L67">
+        <v>1</v>
+      </c>
       <c r="N67" s="4"/>
       <c r="P67" s="4"/>
     </row>
@@ -5267,6 +5360,9 @@
       <c r="K68">
         <v>1</v>
       </c>
+      <c r="L68">
+        <v>1</v>
+      </c>
       <c r="N68" s="4"/>
       <c r="P68" s="4"/>
     </row>
@@ -5299,6 +5395,9 @@
       <c r="K69">
         <v>1</v>
       </c>
+      <c r="L69">
+        <v>1</v>
+      </c>
       <c r="N69" s="4"/>
       <c r="P69" s="4"/>
     </row>
@@ -5331,6 +5430,9 @@
       <c r="K70">
         <v>1</v>
       </c>
+      <c r="L70">
+        <v>1</v>
+      </c>
       <c r="N70" s="4"/>
       <c r="P70" s="4"/>
     </row>
@@ -5363,6 +5465,9 @@
       <c r="K71">
         <v>1</v>
       </c>
+      <c r="L71">
+        <v>1</v>
+      </c>
       <c r="N71" s="4"/>
       <c r="P71" s="4"/>
     </row>
@@ -5395,6 +5500,9 @@
       <c r="K72">
         <v>1</v>
       </c>
+      <c r="L72">
+        <v>1</v>
+      </c>
       <c r="N72" s="4"/>
       <c r="P72" s="4"/>
     </row>
@@ -5427,6 +5535,9 @@
       <c r="K73">
         <v>1</v>
       </c>
+      <c r="L73">
+        <v>1</v>
+      </c>
       <c r="N73" s="4"/>
       <c r="P73" s="4"/>
     </row>
@@ -5459,6 +5570,9 @@
       <c r="K74">
         <v>1</v>
       </c>
+      <c r="L74">
+        <v>1</v>
+      </c>
       <c r="N74" s="4"/>
       <c r="P74" s="4"/>
     </row>
@@ -5491,6 +5605,9 @@
       <c r="K75">
         <v>1</v>
       </c>
+      <c r="L75">
+        <v>1</v>
+      </c>
       <c r="N75" s="4"/>
       <c r="P75" s="4"/>
     </row>
@@ -5523,6 +5640,9 @@
       <c r="K76">
         <v>1</v>
       </c>
+      <c r="L76">
+        <v>1</v>
+      </c>
       <c r="N76" s="4"/>
       <c r="P76" s="4"/>
     </row>
@@ -7078,7 +7198,9 @@
       <c r="D108" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="E108" s="5"/>
+      <c r="E108" s="5" t="s">
+        <v>481</v>
+      </c>
       <c r="F108" t="s">
         <v>447</v>
       </c>
@@ -7093,6 +7215,9 @@
       </c>
       <c r="J108" s="4"/>
       <c r="K108">
+        <v>1</v>
+      </c>
+      <c r="L108">
         <v>1</v>
       </c>
       <c r="M108" s="4"/>
@@ -7108,7 +7233,9 @@
       </c>
       <c r="C109" s="5"/>
       <c r="D109" s="5"/>
-      <c r="E109" s="5"/>
+      <c r="E109" s="5" t="s">
+        <v>482</v>
+      </c>
       <c r="F109" t="s">
         <v>448</v>
       </c>
@@ -7123,6 +7250,9 @@
       </c>
       <c r="J109" s="4"/>
       <c r="K109">
+        <v>1</v>
+      </c>
+      <c r="L109">
         <v>1</v>
       </c>
       <c r="M109" s="4"/>
@@ -7140,7 +7270,9 @@
       <c r="D110" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="E110" s="5"/>
+      <c r="E110" s="5" t="s">
+        <v>483</v>
+      </c>
       <c r="F110" t="s">
         <v>449</v>
       </c>
@@ -7155,6 +7287,9 @@
       </c>
       <c r="J110" s="4"/>
       <c r="K110">
+        <v>1</v>
+      </c>
+      <c r="L110">
         <v>1</v>
       </c>
       <c r="M110" s="4"/>
@@ -7170,7 +7305,9 @@
       </c>
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
-      <c r="E111" s="5"/>
+      <c r="E111" s="5" t="s">
+        <v>484</v>
+      </c>
       <c r="F111" t="s">
         <v>450</v>
       </c>
@@ -7185,6 +7322,9 @@
       </c>
       <c r="J111" s="4"/>
       <c r="K111">
+        <v>1</v>
+      </c>
+      <c r="L111">
         <v>1</v>
       </c>
       <c r="M111" s="4"/>
@@ -7202,7 +7342,9 @@
       <c r="D112" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="E112" s="5"/>
+      <c r="E112" s="5" t="s">
+        <v>485</v>
+      </c>
       <c r="F112" t="s">
         <v>475</v>
       </c>
@@ -7217,6 +7359,9 @@
       </c>
       <c r="J112" s="4"/>
       <c r="K112">
+        <v>1</v>
+      </c>
+      <c r="L112">
         <v>1</v>
       </c>
       <c r="M112" s="4"/>
@@ -7232,7 +7377,9 @@
       </c>
       <c r="C113" s="5"/>
       <c r="D113" s="5"/>
-      <c r="E113" s="5"/>
+      <c r="E113" s="5" t="s">
+        <v>486</v>
+      </c>
       <c r="F113" t="s">
         <v>476</v>
       </c>
@@ -7247,6 +7394,9 @@
       </c>
       <c r="J113" s="4"/>
       <c r="K113">
+        <v>1</v>
+      </c>
+      <c r="L113">
         <v>1</v>
       </c>
       <c r="M113" s="4"/>
@@ -7264,7 +7414,9 @@
       <c r="D114" s="5" t="s">
         <v>362</v>
       </c>
-      <c r="E114" s="5"/>
+      <c r="E114" s="5" t="s">
+        <v>491</v>
+      </c>
       <c r="F114" t="s">
         <v>451</v>
       </c>
@@ -7279,6 +7431,9 @@
       </c>
       <c r="J114" s="4"/>
       <c r="K114">
+        <v>1</v>
+      </c>
+      <c r="L114">
         <v>1</v>
       </c>
       <c r="M114" s="4"/>
@@ -7294,7 +7449,9 @@
       </c>
       <c r="C115" s="5"/>
       <c r="D115" s="5"/>
-      <c r="E115" s="5"/>
+      <c r="E115" s="5" t="s">
+        <v>492</v>
+      </c>
       <c r="F115" t="s">
         <v>452</v>
       </c>
@@ -7309,6 +7466,9 @@
       </c>
       <c r="J115" s="4"/>
       <c r="K115">
+        <v>1</v>
+      </c>
+      <c r="L115">
         <v>1</v>
       </c>
       <c r="M115" s="4"/>
@@ -7326,7 +7486,9 @@
       <c r="D116" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="E116" s="5"/>
+      <c r="E116" s="5" t="s">
+        <v>493</v>
+      </c>
       <c r="F116" t="s">
         <v>454</v>
       </c>
@@ -7341,6 +7503,9 @@
       </c>
       <c r="J116" s="4"/>
       <c r="K116">
+        <v>1</v>
+      </c>
+      <c r="L116">
         <v>1</v>
       </c>
       <c r="M116" s="4"/>
@@ -7356,7 +7521,9 @@
       </c>
       <c r="C117" s="5"/>
       <c r="D117" s="5"/>
-      <c r="E117" s="5"/>
+      <c r="E117" s="5" t="s">
+        <v>494</v>
+      </c>
       <c r="F117" t="s">
         <v>453</v>
       </c>
@@ -7371,6 +7538,9 @@
       </c>
       <c r="J117" s="4"/>
       <c r="K117">
+        <v>1</v>
+      </c>
+      <c r="L117">
         <v>1</v>
       </c>
       <c r="M117" s="4"/>
@@ -7388,7 +7558,9 @@
       <c r="D118" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="E118" s="5"/>
+      <c r="E118" s="5" t="s">
+        <v>495</v>
+      </c>
       <c r="F118" t="s">
         <v>455</v>
       </c>
@@ -7405,8 +7577,14 @@
       <c r="K118">
         <v>1</v>
       </c>
+      <c r="L118">
+        <v>1</v>
+      </c>
       <c r="M118" s="4"/>
       <c r="N118" s="4"/>
+      <c r="O118">
+        <v>1</v>
+      </c>
       <c r="P118" s="4"/>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
@@ -7418,7 +7596,9 @@
       </c>
       <c r="C119" s="5"/>
       <c r="D119" s="5"/>
-      <c r="E119" s="5"/>
+      <c r="E119" s="5" t="s">
+        <v>496</v>
+      </c>
       <c r="F119" t="s">
         <v>456</v>
       </c>
@@ -7433,6 +7613,9 @@
       </c>
       <c r="J119" s="4"/>
       <c r="K119">
+        <v>1</v>
+      </c>
+      <c r="L119">
         <v>1</v>
       </c>
       <c r="M119" s="4"/>
@@ -7450,7 +7633,9 @@
       <c r="D120" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="E120" s="5"/>
+      <c r="E120" s="5" t="s">
+        <v>497</v>
+      </c>
       <c r="F120" t="s">
         <v>457</v>
       </c>
@@ -7465,6 +7650,9 @@
       </c>
       <c r="J120" s="4"/>
       <c r="K120">
+        <v>1</v>
+      </c>
+      <c r="L120">
         <v>1</v>
       </c>
       <c r="M120" s="4"/>
@@ -7480,7 +7668,9 @@
       </c>
       <c r="C121" s="5"/>
       <c r="D121" s="5"/>
-      <c r="E121" s="5"/>
+      <c r="E121" s="5" t="s">
+        <v>498</v>
+      </c>
       <c r="F121" t="s">
         <v>458</v>
       </c>
@@ -7495,6 +7685,9 @@
       </c>
       <c r="J121" s="4"/>
       <c r="K121">
+        <v>1</v>
+      </c>
+      <c r="L121">
         <v>1</v>
       </c>
       <c r="M121" s="4"/>
@@ -7512,7 +7705,9 @@
       <c r="D122" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="E122" s="5"/>
+      <c r="E122" s="5" t="s">
+        <v>499</v>
+      </c>
       <c r="F122" t="s">
         <v>459</v>
       </c>
@@ -7527,6 +7722,9 @@
       </c>
       <c r="J122" s="4"/>
       <c r="K122">
+        <v>1</v>
+      </c>
+      <c r="L122">
         <v>1</v>
       </c>
       <c r="M122" s="4"/>
@@ -7542,7 +7740,9 @@
       </c>
       <c r="C123" s="5"/>
       <c r="D123" s="5"/>
-      <c r="E123" s="5"/>
+      <c r="E123" s="5" t="s">
+        <v>500</v>
+      </c>
       <c r="F123" t="s">
         <v>460</v>
       </c>
@@ -7557,6 +7757,9 @@
       </c>
       <c r="J123" s="4"/>
       <c r="K123">
+        <v>1</v>
+      </c>
+      <c r="L123">
         <v>1</v>
       </c>
       <c r="M123" s="4"/>
@@ -7574,7 +7777,9 @@
       <c r="D124" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="E124" s="5"/>
+      <c r="E124" s="5" t="s">
+        <v>487</v>
+      </c>
       <c r="F124" t="s">
         <v>461</v>
       </c>
@@ -7589,6 +7794,9 @@
       </c>
       <c r="J124" s="4"/>
       <c r="K124">
+        <v>1</v>
+      </c>
+      <c r="L124">
         <v>1</v>
       </c>
       <c r="M124" s="4"/>
@@ -7604,7 +7812,9 @@
       </c>
       <c r="C125" s="5"/>
       <c r="D125" s="5"/>
-      <c r="E125" s="5"/>
+      <c r="E125" s="5" t="s">
+        <v>488</v>
+      </c>
       <c r="F125" t="s">
         <v>462</v>
       </c>
@@ -7619,6 +7829,9 @@
       </c>
       <c r="J125" s="4"/>
       <c r="K125">
+        <v>1</v>
+      </c>
+      <c r="L125">
         <v>1</v>
       </c>
       <c r="M125" s="4"/>
@@ -7627,97 +7840,75 @@
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="B126">
-        <v>2023</v>
-      </c>
-      <c r="D126" t="s">
-        <v>206</v>
-      </c>
-      <c r="E126" t="s">
-        <v>50</v>
+        <v>2024</v>
+      </c>
+      <c r="C126" s="5"/>
+      <c r="D126" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="E126" s="5" t="s">
+        <v>489</v>
       </c>
       <c r="F126" t="s">
-        <v>51</v>
+        <v>478</v>
       </c>
       <c r="G126" t="s">
-        <v>41</v>
-      </c>
-      <c r="H126" t="s">
-        <v>10</v>
-      </c>
-      <c r="J126" s="4">
-        <v>0</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="H126" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="I126" t="s">
+        <v>12</v>
+      </c>
+      <c r="J126" s="4"/>
       <c r="K126">
         <v>1</v>
       </c>
       <c r="L126">
         <v>1</v>
       </c>
-      <c r="M126" s="4">
-        <v>0</v>
-      </c>
-      <c r="N126" s="4">
-        <v>0</v>
-      </c>
-      <c r="O126">
-        <v>0</v>
-      </c>
-      <c r="P126" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q126">
-        <v>0</v>
-      </c>
+      <c r="M126" s="4"/>
+      <c r="N126" s="4"/>
+      <c r="P126" s="4"/>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="B127">
-        <v>2023</v>
-      </c>
-      <c r="D127" t="s">
-        <v>206</v>
-      </c>
-      <c r="E127" t="s">
-        <v>198</v>
+        <v>2024</v>
+      </c>
+      <c r="C127" s="5"/>
+      <c r="D127" s="5"/>
+      <c r="E127" s="5" t="s">
+        <v>490</v>
       </c>
       <c r="F127" t="s">
-        <v>193</v>
+        <v>479</v>
       </c>
       <c r="G127" t="s">
-        <v>41</v>
-      </c>
-      <c r="H127" t="s">
-        <v>19</v>
-      </c>
-      <c r="J127" s="4">
-        <v>0</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="H127" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="I127" t="s">
+        <v>12</v>
+      </c>
+      <c r="J127" s="4"/>
       <c r="K127">
         <v>1</v>
       </c>
       <c r="L127">
         <v>1</v>
       </c>
-      <c r="M127" s="4">
-        <v>0</v>
-      </c>
-      <c r="N127" s="4">
-        <v>0</v>
-      </c>
-      <c r="O127">
-        <v>0</v>
-      </c>
-      <c r="P127" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q127">
-        <v>0</v>
-      </c>
+      <c r="M127" s="4"/>
+      <c r="N127" s="4"/>
+      <c r="P127" s="4"/>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
@@ -7730,16 +7921,16 @@
         <v>206</v>
       </c>
       <c r="E128" t="s">
-        <v>199</v>
+        <v>50</v>
       </c>
       <c r="F128" t="s">
-        <v>194</v>
+        <v>51</v>
       </c>
       <c r="G128" t="s">
         <v>41</v>
       </c>
       <c r="H128" t="s">
-        <v>204</v>
+        <v>10</v>
       </c>
       <c r="J128" s="4">
         <v>0</v>
@@ -7777,19 +7968,16 @@
         <v>206</v>
       </c>
       <c r="E129" t="s">
-        <v>337</v>
+        <v>198</v>
       </c>
       <c r="F129" t="s">
-        <v>318</v>
+        <v>193</v>
       </c>
       <c r="G129" t="s">
         <v>41</v>
       </c>
       <c r="H129" t="s">
-        <v>319</v>
-      </c>
-      <c r="I129" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="J129" s="4">
         <v>0</v>
@@ -7827,16 +8015,16 @@
         <v>206</v>
       </c>
       <c r="E130" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F130" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G130" t="s">
         <v>41</v>
       </c>
       <c r="H130" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J130" s="4">
         <v>0</v>
@@ -7871,19 +8059,22 @@
         <v>2023</v>
       </c>
       <c r="D131" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E131" t="s">
-        <v>201</v>
+        <v>337</v>
       </c>
       <c r="F131" t="s">
-        <v>196</v>
+        <v>318</v>
       </c>
       <c r="G131" t="s">
         <v>41</v>
       </c>
       <c r="H131" t="s">
-        <v>203</v>
+        <v>319</v>
+      </c>
+      <c r="I131" t="s">
+        <v>12</v>
       </c>
       <c r="J131" s="4">
         <v>0</v>
@@ -7918,19 +8109,19 @@
         <v>2023</v>
       </c>
       <c r="D132" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E132" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F132" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G132" t="s">
         <v>41</v>
       </c>
       <c r="H132" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="J132" s="4">
         <v>0</v>
@@ -7957,39 +8148,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:17" ht="20" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>353</v>
+        <v>41</v>
       </c>
       <c r="B133">
-        <v>2024</v>
-      </c>
-      <c r="C133" s="2" t="s">
-        <v>354</v>
+        <v>2023</v>
       </c>
       <c r="D133" t="s">
-        <v>274</v>
+        <v>207</v>
       </c>
       <c r="E133" t="s">
-        <v>311</v>
+        <v>201</v>
       </c>
       <c r="F133" t="s">
-        <v>255</v>
+        <v>196</v>
       </c>
       <c r="G133" t="s">
         <v>41</v>
       </c>
       <c r="H133" t="s">
-        <v>42</v>
-      </c>
-      <c r="I133" t="s">
-        <v>12</v>
+        <v>203</v>
       </c>
       <c r="J133" s="4">
         <v>0</v>
       </c>
       <c r="K133">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L133">
         <v>1</v>
@@ -8010,39 +8195,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:17" ht="20" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>353</v>
+        <v>41</v>
       </c>
       <c r="B134">
-        <v>2024</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>354</v>
+        <v>2023</v>
       </c>
       <c r="D134" t="s">
-        <v>274</v>
+        <v>207</v>
       </c>
       <c r="E134" t="s">
-        <v>312</v>
+        <v>202</v>
       </c>
       <c r="F134" t="s">
-        <v>258</v>
+        <v>197</v>
       </c>
       <c r="G134" t="s">
         <v>41</v>
       </c>
       <c r="H134" t="s">
-        <v>42</v>
-      </c>
-      <c r="I134" t="s">
-        <v>12</v>
+        <v>203</v>
       </c>
       <c r="J134" s="4">
         <v>0</v>
       </c>
       <c r="K134">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L134">
         <v>1</v>
@@ -8077,10 +8256,10 @@
         <v>274</v>
       </c>
       <c r="E135" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F135" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G135" t="s">
         <v>41</v>
@@ -8130,10 +8309,10 @@
         <v>274</v>
       </c>
       <c r="E136" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F136" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="G136" t="s">
         <v>41</v>
@@ -8169,36 +8348,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:17" ht="20" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B137">
-        <v>2023</v>
+        <v>2024</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>354</v>
       </c>
       <c r="D137" t="s">
-        <v>214</v>
+        <v>274</v>
       </c>
       <c r="E137" t="s">
-        <v>229</v>
+        <v>313</v>
       </c>
       <c r="F137" t="s">
-        <v>210</v>
+        <v>257</v>
       </c>
       <c r="G137" t="s">
         <v>41</v>
       </c>
       <c r="H137" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="I137" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J137" s="4">
         <v>0</v>
       </c>
       <c r="K137">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L137">
         <v>1</v>
@@ -8219,39 +8401,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:17" ht="20" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B138">
-        <v>2023</v>
+        <v>2024</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>354</v>
       </c>
       <c r="D138" t="s">
-        <v>214</v>
+        <v>274</v>
       </c>
       <c r="E138" t="s">
-        <v>230</v>
+        <v>314</v>
       </c>
       <c r="F138" t="s">
-        <v>211</v>
+        <v>256</v>
       </c>
       <c r="G138" t="s">
         <v>41</v>
       </c>
       <c r="H138" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="I138" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J138" s="4">
         <v>0</v>
       </c>
       <c r="K138">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L138">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M138" s="4">
         <v>0</v>
@@ -8280,10 +8465,10 @@
         <v>214</v>
       </c>
       <c r="E139" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F139" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G139" t="s">
         <v>41</v>
@@ -8330,10 +8515,10 @@
         <v>214</v>
       </c>
       <c r="E140" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F140" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G140" t="s">
         <v>41</v>
@@ -8370,19 +8555,20 @@
       </c>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A141" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B141" s="5">
-        <v>2024</v>
-      </c>
-      <c r="C141" s="5"/>
-      <c r="D141" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="E141" s="5"/>
-      <c r="F141" s="5" t="s">
-        <v>463</v>
+      <c r="A141" t="s">
+        <v>356</v>
+      </c>
+      <c r="B141">
+        <v>2023</v>
+      </c>
+      <c r="D141" t="s">
+        <v>214</v>
+      </c>
+      <c r="E141" t="s">
+        <v>231</v>
+      </c>
+      <c r="F141" t="s">
+        <v>212</v>
       </c>
       <c r="G141" t="s">
         <v>41</v>
@@ -8391,34 +8577,51 @@
         <v>10</v>
       </c>
       <c r="I141" t="s">
-        <v>12</v>
-      </c>
-      <c r="J141" s="4"/>
-      <c r="M141" s="4"/>
-      <c r="N141" s="4"/>
-      <c r="P141" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="J141" s="4">
+        <v>0</v>
+      </c>
+      <c r="K141">
+        <v>1</v>
+      </c>
+      <c r="L141">
+        <v>1</v>
+      </c>
+      <c r="M141" s="4">
+        <v>0</v>
+      </c>
+      <c r="N141" s="4">
+        <v>0</v>
+      </c>
+      <c r="O141">
+        <v>0</v>
+      </c>
+      <c r="P141" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q141">
+        <v>0</v>
+      </c>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>160</v>
+        <v>356</v>
       </c>
       <c r="B142">
-        <v>2024</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>143</v>
+        <v>2023</v>
       </c>
       <c r="D142" t="s">
-        <v>144</v>
+        <v>214</v>
       </c>
       <c r="E142" t="s">
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="F142" t="s">
-        <v>152</v>
+        <v>213</v>
       </c>
       <c r="G142" t="s">
-        <v>394</v>
+        <v>41</v>
       </c>
       <c r="H142" t="s">
         <v>10</v>
@@ -8429,11 +8632,11 @@
       <c r="J142" s="4">
         <v>0</v>
       </c>
-      <c r="K142" s="4">
-        <v>0</v>
+      <c r="K142">
+        <v>1</v>
       </c>
       <c r="L142">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M142" s="4">
         <v>0</v>
@@ -8442,64 +8645,51 @@
         <v>0</v>
       </c>
       <c r="O142">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P142" s="4">
         <v>0</v>
       </c>
       <c r="Q142">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
-        <v>160</v>
-      </c>
-      <c r="B143">
+      <c r="A143" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B143" s="5">
         <v>2024</v>
       </c>
-      <c r="C143" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D143" t="s">
-        <v>145</v>
-      </c>
-      <c r="F143" t="s">
-        <v>153</v>
+      <c r="C143" s="5"/>
+      <c r="D143" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="E143" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="F143" s="5" t="s">
+        <v>463</v>
       </c>
       <c r="G143" t="s">
-        <v>394</v>
+        <v>41</v>
       </c>
       <c r="H143" t="s">
         <v>10</v>
       </c>
       <c r="I143" t="s">
-        <v>11</v>
-      </c>
-      <c r="J143" s="4">
-        <v>0</v>
-      </c>
-      <c r="K143" s="4">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="J143" s="4"/>
+      <c r="K143">
+        <v>1</v>
       </c>
       <c r="L143">
-        <v>0</v>
-      </c>
-      <c r="M143" s="4">
-        <v>0</v>
-      </c>
-      <c r="N143" s="4">
-        <v>0</v>
-      </c>
-      <c r="O143">
-        <v>0</v>
-      </c>
-      <c r="P143" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q143">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="M143" s="4"/>
+      <c r="N143" s="4"/>
+      <c r="P143" s="4"/>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
@@ -8512,10 +8702,13 @@
         <v>143</v>
       </c>
       <c r="D144" t="s">
-        <v>146</v>
+        <v>144</v>
+      </c>
+      <c r="E144" t="s">
+        <v>275</v>
       </c>
       <c r="F144" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G144" t="s">
         <v>394</v>
@@ -8533,7 +8726,7 @@
         <v>0</v>
       </c>
       <c r="L144">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M144" s="4">
         <v>0</v>
@@ -8542,13 +8735,13 @@
         <v>0</v>
       </c>
       <c r="O144">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P144" s="4">
         <v>0</v>
       </c>
       <c r="Q144">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.2">
@@ -8562,10 +8755,10 @@
         <v>143</v>
       </c>
       <c r="D145" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F145" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G145" t="s">
         <v>394</v>
@@ -8612,13 +8805,10 @@
         <v>143</v>
       </c>
       <c r="D146" t="s">
-        <v>148</v>
-      </c>
-      <c r="E146" t="s">
-        <v>276</v>
+        <v>146</v>
       </c>
       <c r="F146" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G146" t="s">
         <v>394</v>
@@ -8636,7 +8826,7 @@
         <v>0</v>
       </c>
       <c r="L146">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M146" s="4">
         <v>0</v>
@@ -8645,13 +8835,13 @@
         <v>0</v>
       </c>
       <c r="O146">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P146" s="4">
         <v>0</v>
       </c>
       <c r="Q146">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.2">
@@ -8665,10 +8855,10 @@
         <v>143</v>
       </c>
       <c r="D147" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F147" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G147" t="s">
         <v>394</v>
@@ -8700,7 +8890,7 @@
       <c r="P147" s="4">
         <v>0</v>
       </c>
-      <c r="Q147" s="4">
+      <c r="Q147">
         <v>0</v>
       </c>
     </row>
@@ -8715,10 +8905,13 @@
         <v>143</v>
       </c>
       <c r="D148" t="s">
-        <v>150</v>
+        <v>148</v>
+      </c>
+      <c r="E148" t="s">
+        <v>276</v>
       </c>
       <c r="F148" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G148" t="s">
         <v>394</v>
@@ -8736,7 +8929,7 @@
         <v>0</v>
       </c>
       <c r="L148">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M148" s="4">
         <v>0</v>
@@ -8745,13 +8938,13 @@
         <v>0</v>
       </c>
       <c r="O148">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P148" s="4">
         <v>0</v>
       </c>
-      <c r="Q148" s="4">
-        <v>0</v>
+      <c r="Q148">
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.2">
@@ -8765,10 +8958,10 @@
         <v>143</v>
       </c>
       <c r="D149" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F149" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G149" t="s">
         <v>394</v>
@@ -8794,7 +8987,7 @@
       <c r="N149" s="4">
         <v>0</v>
       </c>
-      <c r="O149" s="4">
+      <c r="O149">
         <v>0</v>
       </c>
       <c r="P149" s="4">
@@ -8806,25 +8999,25 @@
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
       <c r="B150">
         <v>2024</v>
       </c>
-      <c r="D150" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="E150" t="s">
-        <v>310</v>
+      <c r="C150" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D150" t="s">
+        <v>150</v>
       </c>
       <c r="F150" t="s">
-        <v>295</v>
+        <v>158</v>
       </c>
       <c r="G150" t="s">
         <v>394</v>
       </c>
       <c r="H150" t="s">
-        <v>286</v>
+        <v>10</v>
       </c>
       <c r="I150" t="s">
         <v>11</v>
@@ -8836,7 +9029,7 @@
         <v>0</v>
       </c>
       <c r="L150">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M150" s="4">
         <v>0</v>
@@ -8844,7 +9037,7 @@
       <c r="N150" s="4">
         <v>0</v>
       </c>
-      <c r="O150" s="4">
+      <c r="O150">
         <v>0</v>
       </c>
       <c r="P150" s="4">
@@ -8856,25 +9049,25 @@
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
       <c r="B151">
         <v>2024</v>
       </c>
-      <c r="D151" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E151" t="s">
-        <v>308</v>
+      <c r="C151" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D151" t="s">
+        <v>151</v>
       </c>
       <c r="F151" t="s">
-        <v>296</v>
+        <v>159</v>
       </c>
       <c r="G151" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="H151" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="I151" t="s">
         <v>11</v>
@@ -8886,7 +9079,7 @@
         <v>0</v>
       </c>
       <c r="L151">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M151" s="4">
         <v>0</v>
@@ -8912,22 +9105,22 @@
         <v>2024</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E152" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="F152" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G152" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="H152" t="s">
-        <v>205</v>
+        <v>286</v>
       </c>
       <c r="I152" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J152" s="4">
         <v>0</v>
@@ -8962,22 +9155,22 @@
         <v>2024</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E153" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F153" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G153" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H153" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="I153" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J153" s="4">
         <v>0</v>
@@ -9012,22 +9205,22 @@
         <v>2024</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E154" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F154" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G154" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H154" t="s">
-        <v>10</v>
+        <v>205</v>
       </c>
       <c r="I154" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J154" s="4">
         <v>0</v>
@@ -9062,19 +9255,19 @@
         <v>2024</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E155" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="F155" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G155" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="H155" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="I155" t="s">
         <v>12</v>
@@ -9112,19 +9305,19 @@
         <v>2024</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E156" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F156" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G156" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="H156" t="s">
-        <v>287</v>
+        <v>10</v>
       </c>
       <c r="I156" t="s">
         <v>11</v>
@@ -9155,88 +9348,122 @@
       </c>
     </row>
     <row r="157" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A157" s="5"/>
-      <c r="B157" s="5"/>
-      <c r="C157" s="5"/>
-      <c r="D157" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="E157" s="5" t="s">
-        <v>465</v>
+      <c r="A157" t="s">
+        <v>17</v>
+      </c>
+      <c r="B157">
+        <v>2024</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E157" t="s">
+        <v>304</v>
       </c>
       <c r="F157" t="s">
-        <v>424</v>
+        <v>300</v>
       </c>
       <c r="G157" t="s">
         <v>393</v>
       </c>
-      <c r="H157" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I157" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J157" s="4"/>
-      <c r="K157" s="4"/>
+      <c r="H157" t="s">
+        <v>33</v>
+      </c>
+      <c r="I157" t="s">
+        <v>12</v>
+      </c>
+      <c r="J157" s="4">
+        <v>0</v>
+      </c>
+      <c r="K157" s="4">
+        <v>0</v>
+      </c>
       <c r="L157">
         <v>1</v>
       </c>
-      <c r="M157" s="4"/>
-      <c r="N157" s="4"/>
+      <c r="M157" s="4">
+        <v>0</v>
+      </c>
+      <c r="N157" s="4">
+        <v>0</v>
+      </c>
       <c r="O157" s="4">
-        <v>1</v>
-      </c>
-      <c r="P157" s="4"/>
-      <c r="Q157" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="P157" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q157" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A158" s="5"/>
-      <c r="B158" s="5"/>
-      <c r="C158" s="5"/>
-      <c r="D158" s="5" t="s">
-        <v>396</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>464</v>
+      <c r="A158" t="s">
+        <v>17</v>
+      </c>
+      <c r="B158">
+        <v>2024</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E158" t="s">
+        <v>305</v>
       </c>
       <c r="F158" t="s">
-        <v>425</v>
+        <v>301</v>
       </c>
       <c r="G158" t="s">
         <v>393</v>
       </c>
-      <c r="H158" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I158" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J158" s="4"/>
-      <c r="K158" s="4"/>
+      <c r="H158" t="s">
+        <v>287</v>
+      </c>
+      <c r="I158" t="s">
+        <v>11</v>
+      </c>
+      <c r="J158" s="4">
+        <v>0</v>
+      </c>
+      <c r="K158" s="4">
+        <v>0</v>
+      </c>
       <c r="L158">
         <v>1</v>
       </c>
-      <c r="M158" s="4"/>
-      <c r="N158" s="4"/>
-      <c r="O158" s="4"/>
-      <c r="P158" s="4"/>
-      <c r="Q158" s="4"/>
+      <c r="M158" s="4">
+        <v>0</v>
+      </c>
+      <c r="N158" s="4">
+        <v>0</v>
+      </c>
+      <c r="O158" s="4">
+        <v>0</v>
+      </c>
+      <c r="P158" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q158" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A159" s="5"/>
+      <c r="A159" t="s">
+        <v>17</v>
+      </c>
       <c r="B159" s="5"/>
       <c r="C159" s="5"/>
-      <c r="D159" s="5" t="s">
-        <v>397</v>
+      <c r="D159" s="6" t="s">
+        <v>395</v>
       </c>
       <c r="E159" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F159" t="s">
-        <v>473</v>
+        <v>424</v>
       </c>
       <c r="G159" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H159" s="5" t="s">
         <v>10</v>
@@ -9251,31 +9478,35 @@
       </c>
       <c r="M159" s="4"/>
       <c r="N159" s="4"/>
-      <c r="O159" s="4"/>
+      <c r="O159" s="4">
+        <v>1</v>
+      </c>
       <c r="P159" s="4"/>
       <c r="Q159" s="4"/>
     </row>
     <row r="160" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A160" s="5"/>
+      <c r="A160" t="s">
+        <v>17</v>
+      </c>
       <c r="B160" s="5"/>
       <c r="C160" s="5"/>
       <c r="D160" s="5" t="s">
-        <v>398</v>
-      </c>
-      <c r="E160" s="5" t="s">
-        <v>467</v>
+        <v>396</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>464</v>
       </c>
       <c r="F160" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G160" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H160" s="5" t="s">
-        <v>404</v>
+        <v>20</v>
       </c>
       <c r="I160" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J160" s="4"/>
       <c r="K160" s="4"/>
@@ -9289,23 +9520,25 @@
       <c r="Q160" s="4"/>
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A161" s="5"/>
+      <c r="A161" t="s">
+        <v>17</v>
+      </c>
       <c r="B161" s="5"/>
       <c r="C161" s="5"/>
       <c r="D161" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E161" s="5" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F161" t="s">
-        <v>427</v>
+        <v>473</v>
       </c>
       <c r="G161" t="s">
         <v>394</v>
       </c>
       <c r="H161" s="5" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I161" s="5" t="s">
         <v>11</v>
@@ -9322,23 +9555,25 @@
       <c r="Q161" s="4"/>
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A162" s="5"/>
+      <c r="A162" t="s">
+        <v>17</v>
+      </c>
       <c r="B162" s="5"/>
       <c r="C162" s="5"/>
-      <c r="D162" s="6" t="s">
-        <v>400</v>
+      <c r="D162" s="5" t="s">
+        <v>398</v>
       </c>
       <c r="E162" s="5" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F162" t="s">
-        <v>474</v>
+        <v>426</v>
       </c>
       <c r="G162" t="s">
         <v>394</v>
       </c>
       <c r="H162" s="5" t="s">
-        <v>10</v>
+        <v>404</v>
       </c>
       <c r="I162" s="5" t="s">
         <v>11</v>
@@ -9350,30 +9585,30 @@
       </c>
       <c r="M162" s="4"/>
       <c r="N162" s="4"/>
-      <c r="O162" s="4">
-        <v>1</v>
-      </c>
+      <c r="O162" s="4"/>
       <c r="P162" s="4"/>
       <c r="Q162" s="4"/>
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A163" s="5"/>
+      <c r="A163" t="s">
+        <v>17</v>
+      </c>
       <c r="B163" s="5"/>
       <c r="C163" s="5"/>
       <c r="D163" s="5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E163" s="5" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F163" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G163" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="H163" s="5" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I163" s="5" t="s">
         <v>11</v>
@@ -9390,20 +9625,22 @@
       <c r="Q163" s="4"/>
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A164" s="5"/>
+      <c r="A164" t="s">
+        <v>17</v>
+      </c>
       <c r="B164" s="5"/>
       <c r="C164" s="5"/>
-      <c r="D164" s="5" t="s">
-        <v>402</v>
+      <c r="D164" s="6" t="s">
+        <v>400</v>
       </c>
       <c r="E164" s="5" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="F164" t="s">
-        <v>429</v>
+        <v>474</v>
       </c>
       <c r="G164" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="H164" s="5" t="s">
         <v>10</v>
@@ -9423,17 +9660,19 @@
       <c r="Q164" s="4"/>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A165" s="5"/>
+      <c r="A165" t="s">
+        <v>17</v>
+      </c>
       <c r="B165" s="5"/>
       <c r="C165" s="5"/>
       <c r="D165" s="5" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E165" s="5" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="F165" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="G165" t="s">
         <v>393</v>
@@ -9456,7 +9695,34 @@
       <c r="Q165" s="4"/>
     </row>
     <row r="166" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>17</v>
+      </c>
+      <c r="B166" s="5"/>
+      <c r="C166" s="5"/>
+      <c r="D166" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="E166" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="F166" t="s">
+        <v>429</v>
+      </c>
+      <c r="G166" t="s">
+        <v>393</v>
+      </c>
+      <c r="H166" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I166" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J166" s="4"/>
       <c r="K166" s="4"/>
+      <c r="L166">
+        <v>1</v>
+      </c>
       <c r="M166" s="4"/>
       <c r="N166" s="4"/>
       <c r="O166" s="4"/>
@@ -9464,7 +9730,34 @@
       <c r="Q166" s="4"/>
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>17</v>
+      </c>
+      <c r="B167" s="5"/>
+      <c r="C167" s="5"/>
+      <c r="D167" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="E167" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="F167" t="s">
+        <v>430</v>
+      </c>
+      <c r="G167" t="s">
+        <v>393</v>
+      </c>
+      <c r="H167" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I167" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J167" s="4"/>
       <c r="K167" s="4"/>
+      <c r="L167">
+        <v>1</v>
+      </c>
       <c r="M167" s="4"/>
       <c r="N167" s="4"/>
       <c r="O167" s="4"/>
@@ -9496,6 +9789,7 @@
       <c r="Q170" s="4"/>
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K171" s="4"/>
       <c r="M171" s="4"/>
       <c r="N171" s="4"/>
       <c r="O171" s="4"/>
@@ -9503,6 +9797,7 @@
       <c r="Q171" s="4"/>
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K172" s="4"/>
       <c r="M172" s="4"/>
       <c r="N172" s="4"/>
       <c r="O172" s="4"/>
@@ -9531,29 +9826,43 @@
       <c r="Q175" s="4"/>
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M176" s="4"/>
       <c r="N176" s="4"/>
       <c r="O176" s="4"/>
       <c r="P176" s="4"/>
-    </row>
-    <row r="177" spans="14:16" x14ac:dyDescent="0.2">
+      <c r="Q176" s="4"/>
+    </row>
+    <row r="177" spans="13:17" x14ac:dyDescent="0.2">
+      <c r="M177" s="4"/>
       <c r="N177" s="4"/>
       <c r="O177" s="4"/>
       <c r="P177" s="4"/>
-    </row>
-    <row r="178" spans="14:16" x14ac:dyDescent="0.2">
+      <c r="Q177" s="4"/>
+    </row>
+    <row r="178" spans="13:17" x14ac:dyDescent="0.2">
       <c r="N178" s="4"/>
+      <c r="O178" s="4"/>
       <c r="P178" s="4"/>
     </row>
-    <row r="179" spans="14:16" x14ac:dyDescent="0.2">
+    <row r="179" spans="13:17" x14ac:dyDescent="0.2">
       <c r="N179" s="4"/>
+      <c r="O179" s="4"/>
       <c r="P179" s="4"/>
     </row>
-    <row r="180" spans="14:16" x14ac:dyDescent="0.2">
+    <row r="180" spans="13:17" x14ac:dyDescent="0.2">
       <c r="N180" s="4"/>
       <c r="P180" s="4"/>
     </row>
-    <row r="181" spans="14:16" x14ac:dyDescent="0.2">
+    <row r="181" spans="13:17" x14ac:dyDescent="0.2">
+      <c r="N181" s="4"/>
       <c r="P181" s="4"/>
+    </row>
+    <row r="182" spans="13:17" x14ac:dyDescent="0.2">
+      <c r="N182" s="4"/>
+      <c r="P182" s="4"/>
+    </row>
+    <row r="183" spans="13:17" x14ac:dyDescent="0.2">
+      <c r="P183" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -9601,29 +9910,29 @@
     <hyperlink ref="C10" r:id="rId41" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{5EDBB7DA-D0A8-5C40-965B-765553AFD77F}"/>
     <hyperlink ref="C11" r:id="rId42" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{97A0DD07-EFF7-EA40-ACF2-1E199930B687}"/>
     <hyperlink ref="C12" r:id="rId43" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{F6A6BB47-C672-7F49-B245-2B27A22913F5}"/>
-    <hyperlink ref="C142" r:id="rId44" xr:uid="{501A2742-514A-AE41-A2A6-B64BEB7C049E}"/>
-    <hyperlink ref="C143" r:id="rId45" xr:uid="{84474B7C-BAD1-1C48-B481-FFCD2859CFE3}"/>
-    <hyperlink ref="C144" r:id="rId46" xr:uid="{8F95774A-3C26-EC45-A54B-6620B1F8DD8B}"/>
-    <hyperlink ref="C145" r:id="rId47" xr:uid="{B3872678-EA39-AA4E-AFE2-3D4E5C0E3234}"/>
-    <hyperlink ref="C146" r:id="rId48" xr:uid="{4BA9BDAA-D422-174B-B7BC-EF82A2B3A879}"/>
-    <hyperlink ref="C147" r:id="rId49" xr:uid="{474C7201-8B25-9F4B-A147-C5CE2B0702AB}"/>
-    <hyperlink ref="C148" r:id="rId50" xr:uid="{3CD58BFF-96D7-B144-B94C-6F1D42F7B3AF}"/>
-    <hyperlink ref="C149" r:id="rId51" xr:uid="{5229D856-741E-1F4D-8A70-F35E0AF5BAD6}"/>
+    <hyperlink ref="C144" r:id="rId44" xr:uid="{501A2742-514A-AE41-A2A6-B64BEB7C049E}"/>
+    <hyperlink ref="C145" r:id="rId45" xr:uid="{84474B7C-BAD1-1C48-B481-FFCD2859CFE3}"/>
+    <hyperlink ref="C146" r:id="rId46" xr:uid="{8F95774A-3C26-EC45-A54B-6620B1F8DD8B}"/>
+    <hyperlink ref="C147" r:id="rId47" xr:uid="{B3872678-EA39-AA4E-AFE2-3D4E5C0E3234}"/>
+    <hyperlink ref="C148" r:id="rId48" xr:uid="{4BA9BDAA-D422-174B-B7BC-EF82A2B3A879}"/>
+    <hyperlink ref="C149" r:id="rId49" xr:uid="{474C7201-8B25-9F4B-A147-C5CE2B0702AB}"/>
+    <hyperlink ref="C150" r:id="rId50" xr:uid="{3CD58BFF-96D7-B144-B94C-6F1D42F7B3AF}"/>
+    <hyperlink ref="C151" r:id="rId51" xr:uid="{5229D856-741E-1F4D-8A70-F35E0AF5BAD6}"/>
     <hyperlink ref="E77" r:id="rId52" xr:uid="{4D2D8028-39C7-A44F-964F-969588B0EFAA}"/>
     <hyperlink ref="E78" r:id="rId53" xr:uid="{3FFA047D-54A7-1C4F-8F99-6C3E171DAF81}"/>
     <hyperlink ref="D17" r:id="rId54" xr:uid="{3ABCF888-2DE3-F241-AF72-0A8CC3470A5F}"/>
     <hyperlink ref="D70" r:id="rId55" xr:uid="{1F241710-62DB-2E44-A747-109074C18B64}"/>
     <hyperlink ref="D72" r:id="rId56" xr:uid="{26B96861-06BB-1843-BD89-C6AE442F656F}"/>
     <hyperlink ref="D73" r:id="rId57" xr:uid="{8A7E9875-FDB3-4A44-A75E-05337B524EC2}"/>
-    <hyperlink ref="D150" r:id="rId58" xr:uid="{610B174C-804A-7040-AB83-A05706A11968}"/>
-    <hyperlink ref="D155" r:id="rId59" xr:uid="{A10F1E36-AFF2-EB41-95B1-EEB475790600}"/>
-    <hyperlink ref="D151" r:id="rId60" xr:uid="{AAE31702-CCEE-494E-AB15-F7DFD7C1277F}"/>
-    <hyperlink ref="D152" r:id="rId61" xr:uid="{0592BD43-1799-4D47-958B-F4C0BD89D869}"/>
-    <hyperlink ref="D153" r:id="rId62" xr:uid="{80001562-99A2-BD44-9DB5-C8BCF6980A1F}"/>
-    <hyperlink ref="D154" r:id="rId63" xr:uid="{4CEB79AD-A518-ED40-97BB-5F83112C6724}"/>
-    <hyperlink ref="D156" r:id="rId64" xr:uid="{63D86AFC-245D-234C-8DCF-BB70FC0FD06C}"/>
-    <hyperlink ref="D157" r:id="rId65" xr:uid="{E80A4473-FEAE-E34A-B92F-1185FF045DD5}"/>
-    <hyperlink ref="D162" r:id="rId66" xr:uid="{B0B4C14C-DEEA-574D-9011-11A44FA41DBB}"/>
+    <hyperlink ref="D152" r:id="rId58" xr:uid="{610B174C-804A-7040-AB83-A05706A11968}"/>
+    <hyperlink ref="D157" r:id="rId59" xr:uid="{A10F1E36-AFF2-EB41-95B1-EEB475790600}"/>
+    <hyperlink ref="D153" r:id="rId60" xr:uid="{AAE31702-CCEE-494E-AB15-F7DFD7C1277F}"/>
+    <hyperlink ref="D154" r:id="rId61" xr:uid="{0592BD43-1799-4D47-958B-F4C0BD89D869}"/>
+    <hyperlink ref="D155" r:id="rId62" xr:uid="{80001562-99A2-BD44-9DB5-C8BCF6980A1F}"/>
+    <hyperlink ref="D156" r:id="rId63" xr:uid="{4CEB79AD-A518-ED40-97BB-5F83112C6724}"/>
+    <hyperlink ref="D158" r:id="rId64" xr:uid="{63D86AFC-245D-234C-8DCF-BB70FC0FD06C}"/>
+    <hyperlink ref="D159" r:id="rId65" xr:uid="{E80A4473-FEAE-E34A-B92F-1185FF045DD5}"/>
+    <hyperlink ref="D164" r:id="rId66" xr:uid="{B0B4C14C-DEEA-574D-9011-11A44FA41DBB}"/>
     <hyperlink ref="D94" r:id="rId67" xr:uid="{55436074-2924-ED43-B050-F0437D753837}"/>
     <hyperlink ref="D60" r:id="rId68" xr:uid="{C80D528B-A854-B34D-8757-27BDF0C8EFD9}"/>
     <hyperlink ref="D62" r:id="rId69" xr:uid="{3C8464E7-A1B4-2340-B366-338E16BC5ECC}"/>

</xml_diff>

<commit_message>
final adjusting of used datasets
</commit_message>
<xml_diff>
--- a/Datasets_all.xlsx
+++ b/Datasets_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k23030440/Pseudovisium/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9819D32-B3B3-3247-9D0E-7AD7109CD350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D296E122-99B2-6646-973A-16778A7C1AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="840" windowWidth="28040" windowHeight="17440" xr2:uid="{419F9F52-EC29-7E45-8CDA-DBEF0D21635D}"/>
   </bookViews>
@@ -1966,8 +1966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F01D6A24-CDB1-1E4B-87EB-E299D59C8055}">
   <dimension ref="A1:Q183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E45" zoomScale="94" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="E128" zoomScale="94" workbookViewId="0">
+      <selection activeCell="L154" sqref="L154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3096,7 +3096,7 @@
         <v>0</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22">
         <v>0</v>
@@ -3446,7 +3446,7 @@
         <v>0</v>
       </c>
       <c r="L29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M29">
         <v>0</v>
@@ -5075,7 +5075,7 @@
         <v>12</v>
       </c>
       <c r="K60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L60">
         <v>1</v>
@@ -5110,7 +5110,7 @@
         <v>12</v>
       </c>
       <c r="K61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L61">
         <v>1</v>
@@ -5183,7 +5183,7 @@
         <v>12</v>
       </c>
       <c r="K63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L63">
         <v>1</v>
@@ -5218,7 +5218,7 @@
         <v>12</v>
       </c>
       <c r="K64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L64">
         <v>1</v>
@@ -5498,7 +5498,7 @@
         <v>12</v>
       </c>
       <c r="K72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L72">
         <v>1</v>
@@ -5638,7 +5638,7 @@
         <v>12</v>
       </c>
       <c r="K76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L76">
         <v>1</v>
@@ -7287,7 +7287,7 @@
       </c>
       <c r="J110" s="4"/>
       <c r="K110">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L110">
         <v>1</v>
@@ -7322,7 +7322,7 @@
       </c>
       <c r="J111" s="4"/>
       <c r="K111">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L111">
         <v>1</v>
@@ -7503,7 +7503,7 @@
       </c>
       <c r="J116" s="4"/>
       <c r="K116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L116">
         <v>1</v>
@@ -7538,7 +7538,7 @@
       </c>
       <c r="J117" s="4"/>
       <c r="K117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L117">
         <v>1</v>
@@ -7650,7 +7650,7 @@
       </c>
       <c r="J120" s="4"/>
       <c r="K120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L120">
         <v>1</v>
@@ -7685,7 +7685,7 @@
       </c>
       <c r="J121" s="4"/>
       <c r="K121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L121">
         <v>1</v>
@@ -7794,7 +7794,7 @@
       </c>
       <c r="J124" s="4"/>
       <c r="K124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L124">
         <v>1</v>
@@ -7829,7 +7829,7 @@
       </c>
       <c r="J125" s="4"/>
       <c r="K125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L125">
         <v>1</v>

</xml_diff>

<commit_message>
removing redundant xenium dataset
</commit_message>
<xml_diff>
--- a/Datasets_all.xlsx
+++ b/Datasets_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k23030440/Pseudovisium/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D296E122-99B2-6646-973A-16778A7C1AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BAC04F-D7A2-1B4C-99E7-5439A885814E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="840" windowWidth="28040" windowHeight="17440" xr2:uid="{419F9F52-EC29-7E45-8CDA-DBEF0D21635D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="499">
   <si>
     <t>Author</t>
   </si>
@@ -1205,9 +1205,6 @@
     <t>https://www.10xgenomics.com/datasets/human-colon-preview-data-xenium-human-colon-gene-expression-panel-1-standard</t>
   </si>
   <si>
-    <t>https://www.10xgenomics.com/datasets/human-skin-preview-data-xenium-human-skin-gene-expression-panel-add-on-1-standard</t>
-  </si>
-  <si>
     <t>https://www.10xgenomics.com/datasets/human-heart-data-xenium-human-multi-tissue-and-cancer-panel-1-standard</t>
   </si>
   <si>
@@ -1365,9 +1362,6 @@
   </si>
   <si>
     <t>Xenium_v1_colon_human</t>
-  </si>
-  <si>
-    <t>Xenium_v1_skin_human</t>
   </si>
   <si>
     <t>Xenium_v1_heart_human</t>
@@ -1964,10 +1958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F01D6A24-CDB1-1E4B-87EB-E299D59C8055}">
-  <dimension ref="A1:Q183"/>
+  <dimension ref="A1:Q182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E128" zoomScale="94" workbookViewId="0">
-      <selection activeCell="L154" sqref="L154"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="94" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2683,7 +2677,7 @@
         <v>186</v>
       </c>
       <c r="G14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H14" t="s">
         <v>139</v>
@@ -3531,7 +3525,7 @@
         <v>55</v>
       </c>
       <c r="G31" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H31" t="s">
         <v>20</v>
@@ -5060,10 +5054,10 @@
         <v>371</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F60" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G60" t="s">
         <v>370</v>
@@ -5095,10 +5089,10 @@
         <v>373</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F61" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G61" t="s">
         <v>370</v>
@@ -5130,10 +5124,10 @@
         <v>375</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>370</v>
@@ -5168,10 +5162,10 @@
         <v>377</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>370</v>
@@ -5203,10 +5197,10 @@
         <v>379</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>370</v>
@@ -5238,10 +5232,10 @@
         <v>381</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>370</v>
@@ -5273,10 +5267,10 @@
         <v>382</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>370</v>
@@ -5308,10 +5302,10 @@
         <v>384</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>370</v>
@@ -5343,16 +5337,16 @@
         <v>385</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F68" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G68" t="s">
         <v>369</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>12</v>
@@ -5378,10 +5372,10 @@
         <v>386</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F69" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G69" t="s">
         <v>369</v>
@@ -5413,10 +5407,10 @@
         <v>387</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F70" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G70" t="s">
         <v>369</v>
@@ -5448,10 +5442,10 @@
         <v>388</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F71" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G71" t="s">
         <v>369</v>
@@ -5483,22 +5477,22 @@
         <v>389</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>241</v>
+        <v>419</v>
       </c>
       <c r="F72" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="G72" t="s">
         <v>369</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>237</v>
+        <v>42</v>
       </c>
       <c r="I72" s="5" t="s">
         <v>12</v>
       </c>
       <c r="K72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L72">
         <v>1</v>
@@ -5514,20 +5508,20 @@
         <v>2024</v>
       </c>
       <c r="C73" s="6"/>
-      <c r="D73" s="6" t="s">
+      <c r="D73" s="5" t="s">
         <v>390</v>
       </c>
       <c r="E73" s="7" t="s">
         <v>420</v>
       </c>
       <c r="F73" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G73" t="s">
         <v>369</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>42</v>
+        <v>203</v>
       </c>
       <c r="I73" s="5" t="s">
         <v>12</v>
@@ -5553,16 +5547,16 @@
         <v>391</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="F74" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G74" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>203</v>
+        <v>405</v>
       </c>
       <c r="I74" s="5" t="s">
         <v>12</v>
@@ -5585,25 +5579,25 @@
       </c>
       <c r="C75" s="6"/>
       <c r="D75" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F75" t="s">
-        <v>446</v>
+        <v>475</v>
       </c>
       <c r="G75" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I75" s="5" t="s">
         <v>12</v>
       </c>
       <c r="K75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L75">
         <v>1</v>
@@ -5611,62 +5605,80 @@
       <c r="N75" s="4"/>
       <c r="P75" s="4"/>
     </row>
-    <row r="76" spans="1:17" ht="17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>17</v>
       </c>
       <c r="B76">
-        <v>2024</v>
-      </c>
-      <c r="C76" s="6"/>
-      <c r="D76" s="5" t="s">
-        <v>392</v>
-      </c>
-      <c r="E76" s="7" t="s">
-        <v>422</v>
+        <v>2023</v>
+      </c>
+      <c r="D76" t="s">
+        <v>162</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="F76" t="s">
-        <v>477</v>
+        <v>59</v>
       </c>
       <c r="G76" t="s">
         <v>369</v>
       </c>
-      <c r="H76" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="I76" s="5" t="s">
-        <v>12</v>
+      <c r="H76" t="s">
+        <v>22</v>
+      </c>
+      <c r="I76" t="s">
+        <v>11</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
       </c>
       <c r="K76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L76">
         <v>1</v>
       </c>
-      <c r="N76" s="4"/>
-      <c r="P76" s="4"/>
+      <c r="M76">
+        <v>0</v>
+      </c>
+      <c r="N76" s="4">
+        <v>0</v>
+      </c>
+      <c r="O76">
+        <v>0</v>
+      </c>
+      <c r="P76" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q76">
+        <v>0</v>
+      </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>17</v>
+        <v>357</v>
       </c>
       <c r="B77">
         <v>2023</v>
       </c>
+      <c r="C77" t="s">
+        <v>315</v>
+      </c>
       <c r="D77" t="s">
-        <v>162</v>
+        <v>30</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>58</v>
+        <v>188</v>
       </c>
       <c r="F77" t="s">
-        <v>59</v>
+        <v>179</v>
       </c>
       <c r="G77" t="s">
-        <v>369</v>
+        <v>31</v>
       </c>
       <c r="H77" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I77" t="s">
         <v>11</v>
@@ -5709,11 +5721,11 @@
       <c r="D78" t="s">
         <v>30</v>
       </c>
-      <c r="E78" s="1" t="s">
-        <v>188</v>
+      <c r="E78" t="s">
+        <v>189</v>
       </c>
       <c r="F78" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G78" t="s">
         <v>31</v>
@@ -5763,10 +5775,10 @@
         <v>30</v>
       </c>
       <c r="E79" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F79" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G79" t="s">
         <v>31</v>
@@ -5816,10 +5828,10 @@
         <v>30</v>
       </c>
       <c r="E80" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F80" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G80" t="s">
         <v>31</v>
@@ -5834,10 +5846,10 @@
         <v>0</v>
       </c>
       <c r="K80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M80">
         <v>0</v>
@@ -5869,10 +5881,10 @@
         <v>30</v>
       </c>
       <c r="E81" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F81" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G81" t="s">
         <v>31</v>
@@ -5883,7 +5895,7 @@
       <c r="I81" t="s">
         <v>11</v>
       </c>
-      <c r="J81">
+      <c r="J81" s="4">
         <v>0</v>
       </c>
       <c r="K81">
@@ -5892,7 +5904,7 @@
       <c r="L81">
         <v>0</v>
       </c>
-      <c r="M81">
+      <c r="M81" s="4">
         <v>0</v>
       </c>
       <c r="N81" s="4">
@@ -5910,28 +5922,28 @@
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B82">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C82" t="s">
-        <v>315</v>
+        <v>351</v>
       </c>
       <c r="D82" t="s">
-        <v>30</v>
+        <v>352</v>
       </c>
       <c r="E82" t="s">
-        <v>192</v>
+        <v>259</v>
       </c>
       <c r="F82" t="s">
-        <v>183</v>
+        <v>260</v>
       </c>
       <c r="G82" t="s">
         <v>31</v>
       </c>
       <c r="H82" t="s">
-        <v>10</v>
+        <v>208</v>
       </c>
       <c r="I82" t="s">
         <v>11</v>
@@ -5975,10 +5987,10 @@
         <v>352</v>
       </c>
       <c r="E83" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="F83" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G83" t="s">
         <v>31</v>
@@ -5993,10 +6005,10 @@
         <v>0</v>
       </c>
       <c r="K83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M83" s="4">
         <v>0</v>
@@ -6027,11 +6039,8 @@
       <c r="D84" t="s">
         <v>352</v>
       </c>
-      <c r="E84" t="s">
-        <v>268</v>
-      </c>
       <c r="F84" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="G84" t="s">
         <v>31</v>
@@ -6046,10 +6055,10 @@
         <v>0</v>
       </c>
       <c r="K84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M84" s="4">
         <v>0</v>
@@ -6080,8 +6089,11 @@
       <c r="D85" t="s">
         <v>352</v>
       </c>
+      <c r="E85" t="s">
+        <v>269</v>
+      </c>
       <c r="F85" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="G85" t="s">
         <v>31</v>
@@ -6096,10 +6108,10 @@
         <v>0</v>
       </c>
       <c r="K85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M85" s="4">
         <v>0</v>
@@ -6131,10 +6143,10 @@
         <v>352</v>
       </c>
       <c r="E86" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F86" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G86" t="s">
         <v>31</v>
@@ -6149,10 +6161,10 @@
         <v>0</v>
       </c>
       <c r="K86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M86" s="4">
         <v>0</v>
@@ -6184,10 +6196,10 @@
         <v>352</v>
       </c>
       <c r="E87" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F87" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="G87" t="s">
         <v>31</v>
@@ -6202,10 +6214,10 @@
         <v>0</v>
       </c>
       <c r="K87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M87" s="4">
         <v>0</v>
@@ -6237,10 +6249,10 @@
         <v>352</v>
       </c>
       <c r="E88" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F88" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G88" t="s">
         <v>31</v>
@@ -6255,10 +6267,10 @@
         <v>0</v>
       </c>
       <c r="K88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M88" s="4">
         <v>0</v>
@@ -6290,10 +6302,10 @@
         <v>352</v>
       </c>
       <c r="E89" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F89" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="G89" t="s">
         <v>31</v>
@@ -6331,28 +6343,25 @@
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>358</v>
+        <v>161</v>
       </c>
       <c r="B90">
-        <v>2024</v>
-      </c>
-      <c r="C90" t="s">
-        <v>351</v>
+        <v>2023</v>
       </c>
       <c r="D90" t="s">
-        <v>352</v>
+        <v>36</v>
       </c>
       <c r="E90" t="s">
-        <v>273</v>
+        <v>163</v>
       </c>
       <c r="F90" t="s">
-        <v>266</v>
+        <v>166</v>
       </c>
       <c r="G90" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H90" t="s">
-        <v>208</v>
+        <v>33</v>
       </c>
       <c r="I90" t="s">
         <v>11</v>
@@ -6393,10 +6402,10 @@
         <v>36</v>
       </c>
       <c r="E91" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F91" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G91" t="s">
         <v>32</v>
@@ -6443,10 +6452,10 @@
         <v>36</v>
       </c>
       <c r="E92" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F92" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G92" t="s">
         <v>32</v>
@@ -6484,25 +6493,25 @@
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>161</v>
+        <v>17</v>
       </c>
       <c r="B93">
-        <v>2023</v>
-      </c>
-      <c r="D93" t="s">
-        <v>36</v>
+        <v>2024</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="E93" t="s">
-        <v>165</v>
+        <v>47</v>
       </c>
       <c r="F93" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G93" t="s">
-        <v>32</v>
+        <v>209</v>
       </c>
       <c r="H93" t="s">
-        <v>33</v>
+        <v>114</v>
       </c>
       <c r="I93" t="s">
         <v>11</v>
@@ -6511,10 +6520,10 @@
         <v>0</v>
       </c>
       <c r="K93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M93" s="4">
         <v>0</v>
@@ -6523,7 +6532,7 @@
         <v>0</v>
       </c>
       <c r="O93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P93" s="4">
         <v>0</v>
@@ -6539,23 +6548,17 @@
       <c r="B94">
         <v>2024</v>
       </c>
-      <c r="D94" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E94" t="s">
-        <v>47</v>
+      <c r="E94" s="1" t="s">
+        <v>355</v>
       </c>
       <c r="F94" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G94" t="s">
         <v>209</v>
       </c>
       <c r="H94" t="s">
-        <v>114</v>
-      </c>
-      <c r="I94" t="s">
-        <v>11</v>
+        <v>115</v>
       </c>
       <c r="J94" s="4">
         <v>0</v>
@@ -6573,7 +6576,7 @@
         <v>0</v>
       </c>
       <c r="O94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P94" s="4">
         <v>0</v>
@@ -6589,17 +6592,23 @@
       <c r="B95">
         <v>2024</v>
       </c>
-      <c r="E95" s="1" t="s">
-        <v>355</v>
+      <c r="D95" t="s">
+        <v>38</v>
+      </c>
+      <c r="E95" t="s">
+        <v>48</v>
       </c>
       <c r="F95" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G95" t="s">
         <v>209</v>
       </c>
       <c r="H95" t="s">
-        <v>115</v>
+        <v>116</v>
+      </c>
+      <c r="I95" t="s">
+        <v>12</v>
       </c>
       <c r="J95" s="4">
         <v>0</v>
@@ -6633,23 +6642,17 @@
       <c r="B96">
         <v>2024</v>
       </c>
-      <c r="D96" t="s">
-        <v>38</v>
-      </c>
       <c r="E96" t="s">
-        <v>48</v>
+        <v>177</v>
       </c>
       <c r="F96" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G96" t="s">
         <v>209</v>
       </c>
       <c r="H96" t="s">
-        <v>116</v>
-      </c>
-      <c r="I96" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="J96" s="4">
         <v>0</v>
@@ -6683,17 +6686,23 @@
       <c r="B97">
         <v>2024</v>
       </c>
+      <c r="D97" t="s">
+        <v>322</v>
+      </c>
       <c r="E97" t="s">
-        <v>177</v>
+        <v>340</v>
       </c>
       <c r="F97" t="s">
-        <v>172</v>
+        <v>323</v>
       </c>
       <c r="G97" t="s">
         <v>209</v>
       </c>
       <c r="H97" t="s">
-        <v>117</v>
+        <v>325</v>
+      </c>
+      <c r="I97" t="s">
+        <v>11</v>
       </c>
       <c r="J97" s="4">
         <v>0</v>
@@ -6727,23 +6736,17 @@
       <c r="B98">
         <v>2024</v>
       </c>
-      <c r="D98" t="s">
-        <v>322</v>
-      </c>
       <c r="E98" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="F98" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="G98" t="s">
         <v>209</v>
       </c>
       <c r="H98" t="s">
-        <v>325</v>
-      </c>
-      <c r="I98" t="s">
-        <v>11</v>
+        <v>326</v>
       </c>
       <c r="J98" s="4">
         <v>0</v>
@@ -6777,17 +6780,23 @@
       <c r="B99">
         <v>2024</v>
       </c>
+      <c r="D99" t="s">
+        <v>327</v>
+      </c>
       <c r="E99" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="F99" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="G99" t="s">
         <v>209</v>
       </c>
       <c r="H99" t="s">
-        <v>326</v>
+        <v>331</v>
+      </c>
+      <c r="I99" t="s">
+        <v>11</v>
       </c>
       <c r="J99" s="4">
         <v>0</v>
@@ -6821,23 +6830,17 @@
       <c r="B100">
         <v>2024</v>
       </c>
-      <c r="D100" t="s">
-        <v>327</v>
-      </c>
       <c r="E100" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="F100" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G100" t="s">
         <v>209</v>
       </c>
       <c r="H100" t="s">
-        <v>331</v>
-      </c>
-      <c r="I100" t="s">
-        <v>11</v>
+        <v>330</v>
       </c>
       <c r="J100" s="4">
         <v>0</v>
@@ -6871,17 +6874,20 @@
       <c r="B101">
         <v>2024</v>
       </c>
+      <c r="D101" t="s">
+        <v>332</v>
+      </c>
       <c r="E101" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="F101" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="G101" t="s">
         <v>209</v>
       </c>
       <c r="H101" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="J101" s="4">
         <v>0</v>
@@ -6915,20 +6921,17 @@
       <c r="B102">
         <v>2024</v>
       </c>
-      <c r="D102" t="s">
-        <v>332</v>
-      </c>
       <c r="E102" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="F102" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="G102" t="s">
         <v>209</v>
       </c>
       <c r="H102" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="J102" s="4">
         <v>0</v>
@@ -6962,17 +6965,23 @@
       <c r="B103">
         <v>2024</v>
       </c>
+      <c r="D103" t="s">
+        <v>39</v>
+      </c>
       <c r="E103" t="s">
-        <v>341</v>
-      </c>
-      <c r="F103" t="s">
-        <v>336</v>
+        <v>49</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>173</v>
       </c>
       <c r="G103" t="s">
         <v>209</v>
       </c>
       <c r="H103" t="s">
-        <v>335</v>
+        <v>118</v>
+      </c>
+      <c r="I103" t="s">
+        <v>11</v>
       </c>
       <c r="J103" s="4">
         <v>0</v>
@@ -7006,23 +7015,17 @@
       <c r="B104">
         <v>2024</v>
       </c>
-      <c r="D104" t="s">
-        <v>39</v>
-      </c>
       <c r="E104" t="s">
-        <v>49</v>
+        <v>178</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G104" t="s">
         <v>209</v>
       </c>
       <c r="H104" t="s">
-        <v>118</v>
-      </c>
-      <c r="I104" t="s">
-        <v>11</v>
+        <v>119</v>
       </c>
       <c r="J104" s="4">
         <v>0</v>
@@ -7056,17 +7059,23 @@
       <c r="B105">
         <v>2024</v>
       </c>
+      <c r="D105" t="s">
+        <v>40</v>
+      </c>
       <c r="E105" t="s">
-        <v>178</v>
+        <v>344</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G105" t="s">
         <v>209</v>
       </c>
       <c r="H105" t="s">
-        <v>119</v>
+        <v>120</v>
+      </c>
+      <c r="I105" t="s">
+        <v>12</v>
       </c>
       <c r="J105" s="4">
         <v>0</v>
@@ -7100,23 +7109,17 @@
       <c r="B106">
         <v>2024</v>
       </c>
-      <c r="D106" t="s">
-        <v>40</v>
-      </c>
       <c r="E106" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G106" t="s">
         <v>209</v>
       </c>
       <c r="H106" t="s">
-        <v>120</v>
-      </c>
-      <c r="I106" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="J106" s="4">
         <v>0</v>
@@ -7150,42 +7153,35 @@
       <c r="B107">
         <v>2024</v>
       </c>
-      <c r="E107" t="s">
-        <v>345</v>
-      </c>
-      <c r="F107" s="4" t="s">
-        <v>176</v>
+      <c r="C107" s="5"/>
+      <c r="D107" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="F107" t="s">
+        <v>445</v>
       </c>
       <c r="G107" t="s">
         <v>209</v>
       </c>
-      <c r="H107" t="s">
-        <v>121</v>
-      </c>
-      <c r="J107" s="4">
-        <v>0</v>
-      </c>
+      <c r="H107" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="I107" t="s">
+        <v>12</v>
+      </c>
+      <c r="J107" s="4"/>
       <c r="K107">
         <v>1</v>
       </c>
       <c r="L107">
         <v>1</v>
       </c>
-      <c r="M107" s="4">
-        <v>0</v>
-      </c>
-      <c r="N107" s="4">
-        <v>0</v>
-      </c>
-      <c r="O107">
-        <v>0</v>
-      </c>
-      <c r="P107" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q107">
-        <v>0</v>
-      </c>
+      <c r="M107" s="4"/>
+      <c r="N107" s="4"/>
+      <c r="P107" s="4"/>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
@@ -7195,14 +7191,12 @@
         <v>2024</v>
       </c>
       <c r="C108" s="5"/>
-      <c r="D108" s="5" t="s">
-        <v>359</v>
-      </c>
+      <c r="D108" s="5"/>
       <c r="E108" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F108" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G108" t="s">
         <v>209</v>
@@ -7232,12 +7226,14 @@
         <v>2024</v>
       </c>
       <c r="C109" s="5"/>
-      <c r="D109" s="5"/>
+      <c r="D109" s="5" t="s">
+        <v>360</v>
+      </c>
       <c r="E109" s="5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F109" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G109" t="s">
         <v>209</v>
@@ -7250,7 +7246,7 @@
       </c>
       <c r="J109" s="4"/>
       <c r="K109">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L109">
         <v>1</v>
@@ -7267,14 +7263,12 @@
         <v>2024</v>
       </c>
       <c r="C110" s="5"/>
-      <c r="D110" s="5" t="s">
-        <v>360</v>
-      </c>
+      <c r="D110" s="5"/>
       <c r="E110" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F110" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G110" t="s">
         <v>209</v>
@@ -7304,25 +7298,27 @@
         <v>2024</v>
       </c>
       <c r="C111" s="5"/>
-      <c r="D111" s="5"/>
+      <c r="D111" s="5" t="s">
+        <v>361</v>
+      </c>
       <c r="E111" s="5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F111" t="s">
-        <v>450</v>
+        <v>473</v>
       </c>
       <c r="G111" t="s">
         <v>209</v>
       </c>
       <c r="H111" s="5" t="s">
-        <v>368</v>
+        <v>405</v>
       </c>
       <c r="I111" t="s">
         <v>12</v>
       </c>
       <c r="J111" s="4"/>
       <c r="K111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L111">
         <v>1</v>
@@ -7339,20 +7335,18 @@
         <v>2024</v>
       </c>
       <c r="C112" s="5"/>
-      <c r="D112" s="5" t="s">
-        <v>361</v>
-      </c>
+      <c r="D112" s="5"/>
       <c r="E112" s="5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F112" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G112" t="s">
         <v>209</v>
       </c>
       <c r="H112" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I112" t="s">
         <v>12</v>
@@ -7376,18 +7370,20 @@
         <v>2024</v>
       </c>
       <c r="C113" s="5"/>
-      <c r="D113" s="5"/>
+      <c r="D113" s="5" t="s">
+        <v>362</v>
+      </c>
       <c r="E113" s="5" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="F113" t="s">
-        <v>476</v>
+        <v>449</v>
       </c>
       <c r="G113" t="s">
         <v>209</v>
       </c>
       <c r="H113" s="5" t="s">
-        <v>406</v>
+        <v>254</v>
       </c>
       <c r="I113" t="s">
         <v>12</v>
@@ -7411,14 +7407,12 @@
         <v>2024</v>
       </c>
       <c r="C114" s="5"/>
-      <c r="D114" s="5" t="s">
-        <v>362</v>
-      </c>
+      <c r="D114" s="5"/>
       <c r="E114" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F114" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G114" t="s">
         <v>209</v>
@@ -7448,9 +7442,11 @@
         <v>2024</v>
       </c>
       <c r="C115" s="5"/>
-      <c r="D115" s="5"/>
+      <c r="D115" s="5" t="s">
+        <v>363</v>
+      </c>
       <c r="E115" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F115" t="s">
         <v>452</v>
@@ -7466,7 +7462,7 @@
       </c>
       <c r="J115" s="4"/>
       <c r="K115">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L115">
         <v>1</v>
@@ -7483,14 +7479,12 @@
         <v>2024</v>
       </c>
       <c r="C116" s="5"/>
-      <c r="D116" s="5" t="s">
-        <v>363</v>
-      </c>
+      <c r="D116" s="5"/>
       <c r="E116" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F116" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="G116" t="s">
         <v>209</v>
@@ -7520,9 +7514,11 @@
         <v>2024</v>
       </c>
       <c r="C117" s="5"/>
-      <c r="D117" s="5"/>
+      <c r="D117" s="5" t="s">
+        <v>364</v>
+      </c>
       <c r="E117" s="5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F117" t="s">
         <v>453</v>
@@ -7531,20 +7527,23 @@
         <v>209</v>
       </c>
       <c r="H117" s="5" t="s">
-        <v>254</v>
+        <v>10</v>
       </c>
       <c r="I117" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J117" s="4"/>
       <c r="K117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L117">
         <v>1</v>
       </c>
       <c r="M117" s="4"/>
       <c r="N117" s="4"/>
+      <c r="O117">
+        <v>1</v>
+      </c>
       <c r="P117" s="4"/>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
@@ -7555,14 +7554,12 @@
         <v>2024</v>
       </c>
       <c r="C118" s="5"/>
-      <c r="D118" s="5" t="s">
-        <v>364</v>
-      </c>
+      <c r="D118" s="5"/>
       <c r="E118" s="5" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F118" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G118" t="s">
         <v>209</v>
@@ -7582,9 +7579,6 @@
       </c>
       <c r="M118" s="4"/>
       <c r="N118" s="4"/>
-      <c r="O118">
-        <v>1</v>
-      </c>
       <c r="P118" s="4"/>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
@@ -7595,12 +7589,14 @@
         <v>2024</v>
       </c>
       <c r="C119" s="5"/>
-      <c r="D119" s="5"/>
+      <c r="D119" s="5" t="s">
+        <v>365</v>
+      </c>
       <c r="E119" s="5" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F119" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G119" t="s">
         <v>209</v>
@@ -7613,7 +7609,7 @@
       </c>
       <c r="J119" s="4"/>
       <c r="K119">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L119">
         <v>1</v>
@@ -7630,14 +7626,12 @@
         <v>2024</v>
       </c>
       <c r="C120" s="5"/>
-      <c r="D120" s="5" t="s">
-        <v>365</v>
-      </c>
+      <c r="D120" s="5"/>
       <c r="E120" s="5" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F120" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G120" t="s">
         <v>209</v>
@@ -7667,25 +7661,27 @@
         <v>2024</v>
       </c>
       <c r="C121" s="5"/>
-      <c r="D121" s="5"/>
+      <c r="D121" s="5" t="s">
+        <v>366</v>
+      </c>
       <c r="E121" s="5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F121" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G121" t="s">
         <v>209</v>
       </c>
       <c r="H121" s="5" t="s">
-        <v>10</v>
+        <v>406</v>
       </c>
       <c r="I121" t="s">
         <v>11</v>
       </c>
       <c r="J121" s="4"/>
       <c r="K121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L121">
         <v>1</v>
@@ -7702,20 +7698,18 @@
         <v>2024</v>
       </c>
       <c r="C122" s="5"/>
-      <c r="D122" s="5" t="s">
-        <v>366</v>
-      </c>
+      <c r="D122" s="5"/>
       <c r="E122" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F122" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G122" t="s">
         <v>209</v>
       </c>
       <c r="H122" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I122" t="s">
         <v>11</v>
@@ -7739,25 +7733,27 @@
         <v>2024</v>
       </c>
       <c r="C123" s="5"/>
-      <c r="D123" s="5"/>
+      <c r="D123" s="5" t="s">
+        <v>367</v>
+      </c>
       <c r="E123" s="5" t="s">
-        <v>500</v>
+        <v>485</v>
       </c>
       <c r="F123" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G123" t="s">
         <v>209</v>
       </c>
       <c r="H123" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="I123" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J123" s="4"/>
       <c r="K123">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L123">
         <v>1</v>
@@ -7774,20 +7770,18 @@
         <v>2024</v>
       </c>
       <c r="C124" s="5"/>
-      <c r="D124" s="5" t="s">
-        <v>367</v>
-      </c>
+      <c r="D124" s="5"/>
       <c r="E124" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F124" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G124" t="s">
         <v>209</v>
       </c>
       <c r="H124" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I124" t="s">
         <v>12</v>
@@ -7811,25 +7805,27 @@
         <v>2024</v>
       </c>
       <c r="C125" s="5"/>
-      <c r="D125" s="5"/>
+      <c r="D125" s="5" t="s">
+        <v>367</v>
+      </c>
       <c r="E125" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F125" t="s">
-        <v>462</v>
+        <v>476</v>
       </c>
       <c r="G125" t="s">
         <v>209</v>
       </c>
       <c r="H125" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I125" t="s">
         <v>12</v>
       </c>
       <c r="J125" s="4"/>
       <c r="K125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L125">
         <v>1</v>
@@ -7846,20 +7842,18 @@
         <v>2024</v>
       </c>
       <c r="C126" s="5"/>
-      <c r="D126" s="5" t="s">
-        <v>367</v>
-      </c>
+      <c r="D126" s="5"/>
       <c r="E126" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F126" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G126" t="s">
         <v>209</v>
       </c>
       <c r="H126" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I126" t="s">
         <v>12</v>
@@ -7877,38 +7871,50 @@
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B127">
-        <v>2024</v>
-      </c>
-      <c r="C127" s="5"/>
-      <c r="D127" s="5"/>
-      <c r="E127" s="5" t="s">
-        <v>490</v>
+        <v>2023</v>
+      </c>
+      <c r="D127" t="s">
+        <v>206</v>
+      </c>
+      <c r="E127" t="s">
+        <v>50</v>
       </c>
       <c r="F127" t="s">
-        <v>479</v>
+        <v>51</v>
       </c>
       <c r="G127" t="s">
-        <v>209</v>
-      </c>
-      <c r="H127" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="I127" t="s">
-        <v>12</v>
-      </c>
-      <c r="J127" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="H127" t="s">
+        <v>10</v>
+      </c>
+      <c r="J127" s="4">
+        <v>0</v>
+      </c>
       <c r="K127">
         <v>1</v>
       </c>
       <c r="L127">
         <v>1</v>
       </c>
-      <c r="M127" s="4"/>
-      <c r="N127" s="4"/>
-      <c r="P127" s="4"/>
+      <c r="M127" s="4">
+        <v>0</v>
+      </c>
+      <c r="N127" s="4">
+        <v>0</v>
+      </c>
+      <c r="O127">
+        <v>0</v>
+      </c>
+      <c r="P127" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q127">
+        <v>0</v>
+      </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
@@ -7921,16 +7927,16 @@
         <v>206</v>
       </c>
       <c r="E128" t="s">
-        <v>50</v>
+        <v>198</v>
       </c>
       <c r="F128" t="s">
-        <v>51</v>
+        <v>193</v>
       </c>
       <c r="G128" t="s">
         <v>41</v>
       </c>
       <c r="H128" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="J128" s="4">
         <v>0</v>
@@ -7968,16 +7974,16 @@
         <v>206</v>
       </c>
       <c r="E129" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F129" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G129" t="s">
         <v>41</v>
       </c>
       <c r="H129" t="s">
-        <v>19</v>
+        <v>204</v>
       </c>
       <c r="J129" s="4">
         <v>0</v>
@@ -8015,16 +8021,19 @@
         <v>206</v>
       </c>
       <c r="E130" t="s">
-        <v>199</v>
+        <v>337</v>
       </c>
       <c r="F130" t="s">
-        <v>194</v>
+        <v>318</v>
       </c>
       <c r="G130" t="s">
         <v>41</v>
       </c>
       <c r="H130" t="s">
-        <v>204</v>
+        <v>319</v>
+      </c>
+      <c r="I130" t="s">
+        <v>12</v>
       </c>
       <c r="J130" s="4">
         <v>0</v>
@@ -8062,19 +8071,16 @@
         <v>206</v>
       </c>
       <c r="E131" t="s">
-        <v>337</v>
+        <v>200</v>
       </c>
       <c r="F131" t="s">
-        <v>318</v>
+        <v>195</v>
       </c>
       <c r="G131" t="s">
         <v>41</v>
       </c>
       <c r="H131" t="s">
-        <v>319</v>
-      </c>
-      <c r="I131" t="s">
-        <v>12</v>
+        <v>205</v>
       </c>
       <c r="J131" s="4">
         <v>0</v>
@@ -8109,19 +8115,19 @@
         <v>2023</v>
       </c>
       <c r="D132" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E132" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F132" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G132" t="s">
         <v>41</v>
       </c>
       <c r="H132" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J132" s="4">
         <v>0</v>
@@ -8159,10 +8165,10 @@
         <v>207</v>
       </c>
       <c r="E133" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F133" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G133" t="s">
         <v>41</v>
@@ -8195,33 +8201,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:17" ht="20" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>41</v>
+        <v>353</v>
       </c>
       <c r="B134">
-        <v>2023</v>
+        <v>2024</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>354</v>
       </c>
       <c r="D134" t="s">
-        <v>207</v>
+        <v>274</v>
       </c>
       <c r="E134" t="s">
-        <v>202</v>
+        <v>311</v>
       </c>
       <c r="F134" t="s">
-        <v>197</v>
+        <v>255</v>
       </c>
       <c r="G134" t="s">
         <v>41</v>
       </c>
       <c r="H134" t="s">
-        <v>203</v>
+        <v>42</v>
+      </c>
+      <c r="I134" t="s">
+        <v>12</v>
       </c>
       <c r="J134" s="4">
         <v>0</v>
       </c>
       <c r="K134">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L134">
         <v>1</v>
@@ -8256,10 +8268,10 @@
         <v>274</v>
       </c>
       <c r="E135" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F135" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="G135" t="s">
         <v>41</v>
@@ -8309,10 +8321,10 @@
         <v>274</v>
       </c>
       <c r="E136" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F136" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G136" t="s">
         <v>41</v>
@@ -8362,10 +8374,10 @@
         <v>274</v>
       </c>
       <c r="E137" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F137" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G137" t="s">
         <v>41</v>
@@ -8401,39 +8413,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:17" ht="20" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B138">
-        <v>2024</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>354</v>
+        <v>2023</v>
       </c>
       <c r="D138" t="s">
-        <v>274</v>
+        <v>214</v>
       </c>
       <c r="E138" t="s">
-        <v>314</v>
+        <v>229</v>
       </c>
       <c r="F138" t="s">
-        <v>256</v>
+        <v>210</v>
       </c>
       <c r="G138" t="s">
         <v>41</v>
       </c>
       <c r="H138" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="I138" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J138" s="4">
         <v>0</v>
       </c>
       <c r="K138">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L138">
         <v>1</v>
@@ -8465,10 +8474,10 @@
         <v>214</v>
       </c>
       <c r="E139" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F139" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G139" t="s">
         <v>41</v>
@@ -8486,7 +8495,7 @@
         <v>1</v>
       </c>
       <c r="L139">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M139" s="4">
         <v>0</v>
@@ -8515,10 +8524,10 @@
         <v>214</v>
       </c>
       <c r="E140" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F140" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G140" t="s">
         <v>41</v>
@@ -8536,7 +8545,7 @@
         <v>1</v>
       </c>
       <c r="L140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M140" s="4">
         <v>0</v>
@@ -8565,10 +8574,10 @@
         <v>214</v>
       </c>
       <c r="E141" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F141" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G141" t="s">
         <v>41</v>
@@ -8586,7 +8595,7 @@
         <v>1</v>
       </c>
       <c r="L141">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M141" s="4">
         <v>0</v>
@@ -8605,20 +8614,21 @@
       </c>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
-        <v>356</v>
-      </c>
-      <c r="B142">
-        <v>2023</v>
-      </c>
-      <c r="D142" t="s">
-        <v>214</v>
-      </c>
-      <c r="E142" t="s">
-        <v>232</v>
-      </c>
-      <c r="F142" t="s">
-        <v>213</v>
+      <c r="A142" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B142" s="5">
+        <v>2024</v>
+      </c>
+      <c r="C142" s="5"/>
+      <c r="D142" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="E142" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="F142" s="5" t="s">
+        <v>461</v>
       </c>
       <c r="G142" t="s">
         <v>41</v>
@@ -8627,69 +8637,71 @@
         <v>10</v>
       </c>
       <c r="I142" t="s">
-        <v>11</v>
-      </c>
-      <c r="J142" s="4">
-        <v>0</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="J142" s="4"/>
       <c r="K142">
         <v>1</v>
       </c>
       <c r="L142">
-        <v>0</v>
-      </c>
-      <c r="M142" s="4">
-        <v>0</v>
-      </c>
-      <c r="N142" s="4">
-        <v>0</v>
-      </c>
-      <c r="O142">
-        <v>0</v>
-      </c>
-      <c r="P142" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q142">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="M142" s="4"/>
+      <c r="N142" s="4"/>
+      <c r="P142" s="4"/>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A143" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B143" s="5">
+      <c r="A143" t="s">
+        <v>160</v>
+      </c>
+      <c r="B143">
         <v>2024</v>
       </c>
-      <c r="C143" s="5"/>
-      <c r="D143" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="E143" s="5" t="s">
-        <v>480</v>
-      </c>
-      <c r="F143" s="5" t="s">
-        <v>463</v>
+      <c r="C143" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D143" t="s">
+        <v>144</v>
+      </c>
+      <c r="E143" t="s">
+        <v>275</v>
+      </c>
+      <c r="F143" t="s">
+        <v>152</v>
       </c>
       <c r="G143" t="s">
-        <v>41</v>
+        <v>393</v>
       </c>
       <c r="H143" t="s">
         <v>10</v>
       </c>
       <c r="I143" t="s">
-        <v>12</v>
-      </c>
-      <c r="J143" s="4"/>
-      <c r="K143">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="J143" s="4">
+        <v>0</v>
+      </c>
+      <c r="K143" s="4">
+        <v>0</v>
       </c>
       <c r="L143">
         <v>1</v>
       </c>
-      <c r="M143" s="4"/>
-      <c r="N143" s="4"/>
-      <c r="P143" s="4"/>
+      <c r="M143" s="4">
+        <v>0</v>
+      </c>
+      <c r="N143" s="4">
+        <v>0</v>
+      </c>
+      <c r="O143">
+        <v>1</v>
+      </c>
+      <c r="P143" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q143">
+        <v>1</v>
+      </c>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
@@ -8702,16 +8714,13 @@
         <v>143</v>
       </c>
       <c r="D144" t="s">
-        <v>144</v>
-      </c>
-      <c r="E144" t="s">
-        <v>275</v>
+        <v>145</v>
       </c>
       <c r="F144" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G144" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H144" t="s">
         <v>10</v>
@@ -8726,7 +8735,7 @@
         <v>0</v>
       </c>
       <c r="L144">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M144" s="4">
         <v>0</v>
@@ -8735,13 +8744,13 @@
         <v>0</v>
       </c>
       <c r="O144">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P144" s="4">
         <v>0</v>
       </c>
       <c r="Q144">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.2">
@@ -8755,13 +8764,13 @@
         <v>143</v>
       </c>
       <c r="D145" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F145" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G145" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H145" t="s">
         <v>10</v>
@@ -8805,13 +8814,13 @@
         <v>143</v>
       </c>
       <c r="D146" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F146" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G146" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H146" t="s">
         <v>10</v>
@@ -8855,13 +8864,16 @@
         <v>143</v>
       </c>
       <c r="D147" t="s">
-        <v>147</v>
+        <v>148</v>
+      </c>
+      <c r="E147" t="s">
+        <v>276</v>
       </c>
       <c r="F147" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G147" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H147" t="s">
         <v>10</v>
@@ -8876,7 +8888,7 @@
         <v>0</v>
       </c>
       <c r="L147">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M147" s="4">
         <v>0</v>
@@ -8885,13 +8897,13 @@
         <v>0</v>
       </c>
       <c r="O147">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P147" s="4">
         <v>0</v>
       </c>
       <c r="Q147">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.2">
@@ -8905,16 +8917,13 @@
         <v>143</v>
       </c>
       <c r="D148" t="s">
-        <v>148</v>
-      </c>
-      <c r="E148" t="s">
-        <v>276</v>
+        <v>149</v>
       </c>
       <c r="F148" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G148" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H148" t="s">
         <v>10</v>
@@ -8929,7 +8938,7 @@
         <v>0</v>
       </c>
       <c r="L148">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M148" s="4">
         <v>0</v>
@@ -8938,13 +8947,13 @@
         <v>0</v>
       </c>
       <c r="O148">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P148" s="4">
         <v>0</v>
       </c>
-      <c r="Q148">
-        <v>1</v>
+      <c r="Q148" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.2">
@@ -8958,13 +8967,13 @@
         <v>143</v>
       </c>
       <c r="D149" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F149" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G149" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H149" t="s">
         <v>10</v>
@@ -9008,13 +9017,13 @@
         <v>143</v>
       </c>
       <c r="D150" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F150" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G150" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H150" t="s">
         <v>10</v>
@@ -9037,7 +9046,7 @@
       <c r="N150" s="4">
         <v>0</v>
       </c>
-      <c r="O150">
+      <c r="O150" s="4">
         <v>0</v>
       </c>
       <c r="P150" s="4">
@@ -9049,25 +9058,25 @@
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>160</v>
+        <v>17</v>
       </c>
       <c r="B151">
         <v>2024</v>
       </c>
-      <c r="C151" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D151" t="s">
-        <v>151</v>
+      <c r="D151" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E151" t="s">
+        <v>310</v>
       </c>
       <c r="F151" t="s">
-        <v>159</v>
+        <v>295</v>
       </c>
       <c r="G151" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H151" t="s">
-        <v>10</v>
+        <v>286</v>
       </c>
       <c r="I151" t="s">
         <v>11</v>
@@ -9079,7 +9088,7 @@
         <v>0</v>
       </c>
       <c r="L151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M151" s="4">
         <v>0</v>
@@ -9105,19 +9114,19 @@
         <v>2024</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E152" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F152" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G152" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="H152" t="s">
-        <v>286</v>
+        <v>33</v>
       </c>
       <c r="I152" t="s">
         <v>11</v>
@@ -9155,22 +9164,22 @@
         <v>2024</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E153" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F153" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G153" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H153" t="s">
-        <v>33</v>
+        <v>205</v>
       </c>
       <c r="I153" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J153" s="4">
         <v>0</v>
@@ -9205,19 +9214,19 @@
         <v>2024</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E154" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="F154" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G154" t="s">
         <v>393</v>
       </c>
       <c r="H154" t="s">
-        <v>205</v>
+        <v>20</v>
       </c>
       <c r="I154" t="s">
         <v>12</v>
@@ -9255,22 +9264,22 @@
         <v>2024</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E155" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="F155" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="G155" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H155" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I155" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J155" s="4">
         <v>0</v>
@@ -9305,22 +9314,22 @@
         <v>2024</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E156" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F156" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G156" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="H156" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="I156" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J156" s="4">
         <v>0</v>
@@ -9355,22 +9364,22 @@
         <v>2024</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E157" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F157" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="G157" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H157" t="s">
-        <v>33</v>
+        <v>287</v>
       </c>
       <c r="I157" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J157" s="4">
         <v>0</v>
@@ -9401,51 +9410,38 @@
       <c r="A158" t="s">
         <v>17</v>
       </c>
-      <c r="B158">
-        <v>2024</v>
-      </c>
-      <c r="D158" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E158" t="s">
-        <v>305</v>
+      <c r="B158" s="5"/>
+      <c r="C158" s="5"/>
+      <c r="D158" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="E158" s="5" t="s">
+        <v>463</v>
       </c>
       <c r="F158" t="s">
-        <v>301</v>
+        <v>423</v>
       </c>
       <c r="G158" t="s">
-        <v>393</v>
-      </c>
-      <c r="H158" t="s">
-        <v>287</v>
-      </c>
-      <c r="I158" t="s">
+        <v>392</v>
+      </c>
+      <c r="H158" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I158" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J158" s="4">
-        <v>0</v>
-      </c>
-      <c r="K158" s="4">
-        <v>0</v>
-      </c>
+      <c r="J158" s="4"/>
+      <c r="K158" s="4"/>
       <c r="L158">
         <v>1</v>
       </c>
-      <c r="M158" s="4">
-        <v>0</v>
-      </c>
-      <c r="N158" s="4">
-        <v>0</v>
-      </c>
+      <c r="M158" s="4"/>
+      <c r="N158" s="4"/>
       <c r="O158" s="4">
-        <v>0</v>
-      </c>
-      <c r="P158" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q158" s="4">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="P158" s="4"/>
+      <c r="Q158" s="4"/>
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
@@ -9453,23 +9449,23 @@
       </c>
       <c r="B159" s="5"/>
       <c r="C159" s="5"/>
-      <c r="D159" s="6" t="s">
+      <c r="D159" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="E159" s="5" t="s">
-        <v>465</v>
+      <c r="E159" s="1" t="s">
+        <v>462</v>
       </c>
       <c r="F159" t="s">
         <v>424</v>
       </c>
       <c r="G159" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H159" s="5" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I159" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J159" s="4"/>
       <c r="K159" s="4"/>
@@ -9478,9 +9474,7 @@
       </c>
       <c r="M159" s="4"/>
       <c r="N159" s="4"/>
-      <c r="O159" s="4">
-        <v>1</v>
-      </c>
+      <c r="O159" s="4"/>
       <c r="P159" s="4"/>
       <c r="Q159" s="4"/>
     </row>
@@ -9493,20 +9487,20 @@
       <c r="D160" s="5" t="s">
         <v>396</v>
       </c>
-      <c r="E160" s="1" t="s">
+      <c r="E160" s="5" t="s">
         <v>464</v>
       </c>
       <c r="F160" t="s">
-        <v>425</v>
+        <v>471</v>
       </c>
       <c r="G160" t="s">
         <v>393</v>
       </c>
       <c r="H160" s="5" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I160" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J160" s="4"/>
       <c r="K160" s="4"/>
@@ -9529,16 +9523,16 @@
         <v>397</v>
       </c>
       <c r="E161" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F161" t="s">
-        <v>473</v>
+        <v>425</v>
       </c>
       <c r="G161" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H161" s="5" t="s">
-        <v>10</v>
+        <v>403</v>
       </c>
       <c r="I161" s="5" t="s">
         <v>11</v>
@@ -9564,16 +9558,16 @@
         <v>398</v>
       </c>
       <c r="E162" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F162" t="s">
         <v>426</v>
       </c>
       <c r="G162" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H162" s="5" t="s">
-        <v>404</v>
+        <v>20</v>
       </c>
       <c r="I162" s="5" t="s">
         <v>11</v>
@@ -9595,20 +9589,20 @@
       </c>
       <c r="B163" s="5"/>
       <c r="C163" s="5"/>
-      <c r="D163" s="5" t="s">
+      <c r="D163" s="6" t="s">
         <v>399</v>
       </c>
       <c r="E163" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F163" t="s">
-        <v>427</v>
+        <v>472</v>
       </c>
       <c r="G163" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H163" s="5" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I163" s="5" t="s">
         <v>11</v>
@@ -9630,17 +9624,17 @@
       </c>
       <c r="B164" s="5"/>
       <c r="C164" s="5"/>
-      <c r="D164" s="6" t="s">
+      <c r="D164" s="5" t="s">
         <v>400</v>
       </c>
       <c r="E164" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F164" t="s">
-        <v>474</v>
+        <v>427</v>
       </c>
       <c r="G164" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="H164" s="5" t="s">
         <v>10</v>
@@ -9669,13 +9663,13 @@
         <v>401</v>
       </c>
       <c r="E165" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F165" t="s">
         <v>428</v>
       </c>
       <c r="G165" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H165" s="5" t="s">
         <v>10</v>
@@ -9704,13 +9698,13 @@
         <v>402</v>
       </c>
       <c r="E166" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F166" t="s">
         <v>429</v>
       </c>
       <c r="G166" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H166" s="5" t="s">
         <v>10</v>
@@ -9730,34 +9724,7 @@
       <c r="Q166" s="4"/>
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
-        <v>17</v>
-      </c>
-      <c r="B167" s="5"/>
-      <c r="C167" s="5"/>
-      <c r="D167" s="5" t="s">
-        <v>403</v>
-      </c>
-      <c r="E167" s="5" t="s">
-        <v>472</v>
-      </c>
-      <c r="F167" t="s">
-        <v>430</v>
-      </c>
-      <c r="G167" t="s">
-        <v>393</v>
-      </c>
-      <c r="H167" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I167" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J167" s="4"/>
       <c r="K167" s="4"/>
-      <c r="L167">
-        <v>1</v>
-      </c>
       <c r="M167" s="4"/>
       <c r="N167" s="4"/>
       <c r="O167" s="4"/>
@@ -9797,7 +9764,6 @@
       <c r="Q171" s="4"/>
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="K172" s="4"/>
       <c r="M172" s="4"/>
       <c r="N172" s="4"/>
       <c r="O172" s="4"/>
@@ -9832,37 +9798,30 @@
       <c r="P176" s="4"/>
       <c r="Q176" s="4"/>
     </row>
-    <row r="177" spans="13:17" x14ac:dyDescent="0.2">
-      <c r="M177" s="4"/>
+    <row r="177" spans="14:16" x14ac:dyDescent="0.2">
       <c r="N177" s="4"/>
       <c r="O177" s="4"/>
       <c r="P177" s="4"/>
-      <c r="Q177" s="4"/>
-    </row>
-    <row r="178" spans="13:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="178" spans="14:16" x14ac:dyDescent="0.2">
       <c r="N178" s="4"/>
       <c r="O178" s="4"/>
       <c r="P178" s="4"/>
     </row>
-    <row r="179" spans="13:17" x14ac:dyDescent="0.2">
+    <row r="179" spans="14:16" x14ac:dyDescent="0.2">
       <c r="N179" s="4"/>
-      <c r="O179" s="4"/>
       <c r="P179" s="4"/>
     </row>
-    <row r="180" spans="13:17" x14ac:dyDescent="0.2">
+    <row r="180" spans="14:16" x14ac:dyDescent="0.2">
       <c r="N180" s="4"/>
       <c r="P180" s="4"/>
     </row>
-    <row r="181" spans="13:17" x14ac:dyDescent="0.2">
+    <row r="181" spans="14:16" x14ac:dyDescent="0.2">
       <c r="N181" s="4"/>
       <c r="P181" s="4"/>
     </row>
-    <row r="182" spans="13:17" x14ac:dyDescent="0.2">
-      <c r="N182" s="4"/>
+    <row r="182" spans="14:16" x14ac:dyDescent="0.2">
       <c r="P182" s="4"/>
-    </row>
-    <row r="183" spans="13:17" x14ac:dyDescent="0.2">
-      <c r="P183" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -9910,33 +9869,32 @@
     <hyperlink ref="C10" r:id="rId41" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{5EDBB7DA-D0A8-5C40-965B-765553AFD77F}"/>
     <hyperlink ref="C11" r:id="rId42" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{97A0DD07-EFF7-EA40-ACF2-1E199930B687}"/>
     <hyperlink ref="C12" r:id="rId43" display="https://doi.org/10.1038/s41587-022-01483-z" xr:uid="{F6A6BB47-C672-7F49-B245-2B27A22913F5}"/>
-    <hyperlink ref="C144" r:id="rId44" xr:uid="{501A2742-514A-AE41-A2A6-B64BEB7C049E}"/>
-    <hyperlink ref="C145" r:id="rId45" xr:uid="{84474B7C-BAD1-1C48-B481-FFCD2859CFE3}"/>
-    <hyperlink ref="C146" r:id="rId46" xr:uid="{8F95774A-3C26-EC45-A54B-6620B1F8DD8B}"/>
-    <hyperlink ref="C147" r:id="rId47" xr:uid="{B3872678-EA39-AA4E-AFE2-3D4E5C0E3234}"/>
-    <hyperlink ref="C148" r:id="rId48" xr:uid="{4BA9BDAA-D422-174B-B7BC-EF82A2B3A879}"/>
-    <hyperlink ref="C149" r:id="rId49" xr:uid="{474C7201-8B25-9F4B-A147-C5CE2B0702AB}"/>
-    <hyperlink ref="C150" r:id="rId50" xr:uid="{3CD58BFF-96D7-B144-B94C-6F1D42F7B3AF}"/>
-    <hyperlink ref="C151" r:id="rId51" xr:uid="{5229D856-741E-1F4D-8A70-F35E0AF5BAD6}"/>
-    <hyperlink ref="E77" r:id="rId52" xr:uid="{4D2D8028-39C7-A44F-964F-969588B0EFAA}"/>
-    <hyperlink ref="E78" r:id="rId53" xr:uid="{3FFA047D-54A7-1C4F-8F99-6C3E171DAF81}"/>
+    <hyperlink ref="C143" r:id="rId44" xr:uid="{501A2742-514A-AE41-A2A6-B64BEB7C049E}"/>
+    <hyperlink ref="C144" r:id="rId45" xr:uid="{84474B7C-BAD1-1C48-B481-FFCD2859CFE3}"/>
+    <hyperlink ref="C145" r:id="rId46" xr:uid="{8F95774A-3C26-EC45-A54B-6620B1F8DD8B}"/>
+    <hyperlink ref="C146" r:id="rId47" xr:uid="{B3872678-EA39-AA4E-AFE2-3D4E5C0E3234}"/>
+    <hyperlink ref="C147" r:id="rId48" xr:uid="{4BA9BDAA-D422-174B-B7BC-EF82A2B3A879}"/>
+    <hyperlink ref="C148" r:id="rId49" xr:uid="{474C7201-8B25-9F4B-A147-C5CE2B0702AB}"/>
+    <hyperlink ref="C149" r:id="rId50" xr:uid="{3CD58BFF-96D7-B144-B94C-6F1D42F7B3AF}"/>
+    <hyperlink ref="C150" r:id="rId51" xr:uid="{5229D856-741E-1F4D-8A70-F35E0AF5BAD6}"/>
+    <hyperlink ref="E76" r:id="rId52" xr:uid="{4D2D8028-39C7-A44F-964F-969588B0EFAA}"/>
+    <hyperlink ref="E77" r:id="rId53" xr:uid="{3FFA047D-54A7-1C4F-8F99-6C3E171DAF81}"/>
     <hyperlink ref="D17" r:id="rId54" xr:uid="{3ABCF888-2DE3-F241-AF72-0A8CC3470A5F}"/>
     <hyperlink ref="D70" r:id="rId55" xr:uid="{1F241710-62DB-2E44-A747-109074C18B64}"/>
-    <hyperlink ref="D72" r:id="rId56" xr:uid="{26B96861-06BB-1843-BD89-C6AE442F656F}"/>
-    <hyperlink ref="D73" r:id="rId57" xr:uid="{8A7E9875-FDB3-4A44-A75E-05337B524EC2}"/>
-    <hyperlink ref="D152" r:id="rId58" xr:uid="{610B174C-804A-7040-AB83-A05706A11968}"/>
-    <hyperlink ref="D157" r:id="rId59" xr:uid="{A10F1E36-AFF2-EB41-95B1-EEB475790600}"/>
-    <hyperlink ref="D153" r:id="rId60" xr:uid="{AAE31702-CCEE-494E-AB15-F7DFD7C1277F}"/>
-    <hyperlink ref="D154" r:id="rId61" xr:uid="{0592BD43-1799-4D47-958B-F4C0BD89D869}"/>
-    <hyperlink ref="D155" r:id="rId62" xr:uid="{80001562-99A2-BD44-9DB5-C8BCF6980A1F}"/>
-    <hyperlink ref="D156" r:id="rId63" xr:uid="{4CEB79AD-A518-ED40-97BB-5F83112C6724}"/>
-    <hyperlink ref="D158" r:id="rId64" xr:uid="{63D86AFC-245D-234C-8DCF-BB70FC0FD06C}"/>
-    <hyperlink ref="D159" r:id="rId65" xr:uid="{E80A4473-FEAE-E34A-B92F-1185FF045DD5}"/>
-    <hyperlink ref="D164" r:id="rId66" xr:uid="{B0B4C14C-DEEA-574D-9011-11A44FA41DBB}"/>
-    <hyperlink ref="D94" r:id="rId67" xr:uid="{55436074-2924-ED43-B050-F0437D753837}"/>
-    <hyperlink ref="D60" r:id="rId68" xr:uid="{C80D528B-A854-B34D-8757-27BDF0C8EFD9}"/>
-    <hyperlink ref="D62" r:id="rId69" xr:uid="{3C8464E7-A1B4-2340-B366-338E16BC5ECC}"/>
-    <hyperlink ref="E62" r:id="rId70" xr:uid="{C3AE867C-7C47-8441-BCB2-DAA772403942}"/>
+    <hyperlink ref="D72" r:id="rId56" xr:uid="{8A7E9875-FDB3-4A44-A75E-05337B524EC2}"/>
+    <hyperlink ref="D151" r:id="rId57" xr:uid="{610B174C-804A-7040-AB83-A05706A11968}"/>
+    <hyperlink ref="D156" r:id="rId58" xr:uid="{A10F1E36-AFF2-EB41-95B1-EEB475790600}"/>
+    <hyperlink ref="D152" r:id="rId59" xr:uid="{AAE31702-CCEE-494E-AB15-F7DFD7C1277F}"/>
+    <hyperlink ref="D153" r:id="rId60" xr:uid="{0592BD43-1799-4D47-958B-F4C0BD89D869}"/>
+    <hyperlink ref="D154" r:id="rId61" xr:uid="{80001562-99A2-BD44-9DB5-C8BCF6980A1F}"/>
+    <hyperlink ref="D155" r:id="rId62" xr:uid="{4CEB79AD-A518-ED40-97BB-5F83112C6724}"/>
+    <hyperlink ref="D157" r:id="rId63" xr:uid="{63D86AFC-245D-234C-8DCF-BB70FC0FD06C}"/>
+    <hyperlink ref="D158" r:id="rId64" xr:uid="{E80A4473-FEAE-E34A-B92F-1185FF045DD5}"/>
+    <hyperlink ref="D163" r:id="rId65" xr:uid="{B0B4C14C-DEEA-574D-9011-11A44FA41DBB}"/>
+    <hyperlink ref="D93" r:id="rId66" xr:uid="{55436074-2924-ED43-B050-F0437D753837}"/>
+    <hyperlink ref="D60" r:id="rId67" xr:uid="{C80D528B-A854-B34D-8757-27BDF0C8EFD9}"/>
+    <hyperlink ref="D62" r:id="rId68" xr:uid="{3C8464E7-A1B4-2340-B366-338E16BC5ECC}"/>
+    <hyperlink ref="E62" r:id="rId69" xr:uid="{C3AE867C-7C47-8441-BCB2-DAA772403942}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
adding missing species values for dataset csv
</commit_message>
<xml_diff>
--- a/Datasets_all.xlsx
+++ b/Datasets_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k23030440/Pseudovisium/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61079D83-2FF4-DE41-8117-07CB4E61C6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27939249-A59A-FD4C-A55F-D343533BF6F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="840" windowWidth="28040" windowHeight="17440" xr2:uid="{419F9F52-EC29-7E45-8CDA-DBEF0D21635D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="499">
   <si>
     <t>Author</t>
   </si>
@@ -1614,7 +1614,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1623,9 +1623,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1963,8 +1960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F01D6A24-CDB1-1E4B-87EB-E299D59C8055}">
   <dimension ref="A1:Q182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="D111" zoomScale="94" workbookViewId="0">
+      <selection activeCell="I133" sqref="I133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6564,6 +6561,9 @@
       <c r="H94" t="s">
         <v>115</v>
       </c>
+      <c r="I94" t="s">
+        <v>11</v>
+      </c>
       <c r="J94" s="4">
         <v>0</v>
       </c>
@@ -6658,6 +6658,9 @@
       <c r="H96" t="s">
         <v>117</v>
       </c>
+      <c r="I96" t="s">
+        <v>12</v>
+      </c>
       <c r="J96" s="4">
         <v>0</v>
       </c>
@@ -6752,6 +6755,9 @@
       <c r="H98" t="s">
         <v>326</v>
       </c>
+      <c r="I98" t="s">
+        <v>11</v>
+      </c>
       <c r="J98" s="4">
         <v>0</v>
       </c>
@@ -6846,6 +6852,9 @@
       <c r="H100" t="s">
         <v>330</v>
       </c>
+      <c r="I100" t="s">
+        <v>11</v>
+      </c>
       <c r="J100" s="4">
         <v>0</v>
       </c>
@@ -6893,6 +6902,9 @@
       <c r="H101" t="s">
         <v>334</v>
       </c>
+      <c r="I101" t="s">
+        <v>12</v>
+      </c>
       <c r="J101" s="4">
         <v>0</v>
       </c>
@@ -6937,6 +6949,9 @@
       <c r="H102" t="s">
         <v>335</v>
       </c>
+      <c r="I102" t="s">
+        <v>12</v>
+      </c>
       <c r="J102" s="4">
         <v>0</v>
       </c>
@@ -7031,6 +7046,9 @@
       <c r="H104" t="s">
         <v>119</v>
       </c>
+      <c r="I104" t="s">
+        <v>11</v>
+      </c>
       <c r="J104" s="4">
         <v>0</v>
       </c>
@@ -7124,6 +7142,9 @@
       </c>
       <c r="H106" t="s">
         <v>121</v>
+      </c>
+      <c r="I106" t="s">
+        <v>12</v>
       </c>
       <c r="J106" s="4">
         <v>0</v>
@@ -7895,6 +7916,9 @@
       <c r="H127" t="s">
         <v>10</v>
       </c>
+      <c r="I127" t="s">
+        <v>11</v>
+      </c>
       <c r="J127" s="4">
         <v>0</v>
       </c>
@@ -7942,6 +7966,9 @@
       <c r="H128" t="s">
         <v>19</v>
       </c>
+      <c r="I128" t="s">
+        <v>12</v>
+      </c>
       <c r="J128" s="4">
         <v>0</v>
       </c>
@@ -7989,6 +8016,9 @@
       <c r="H129" t="s">
         <v>204</v>
       </c>
+      <c r="I129" t="s">
+        <v>12</v>
+      </c>
       <c r="J129" s="4">
         <v>0</v>
       </c>
@@ -8086,6 +8116,9 @@
       <c r="H131" t="s">
         <v>205</v>
       </c>
+      <c r="I131" t="s">
+        <v>12</v>
+      </c>
       <c r="J131" s="4">
         <v>0</v>
       </c>
@@ -8133,6 +8166,9 @@
       <c r="H132" t="s">
         <v>203</v>
       </c>
+      <c r="I132" t="s">
+        <v>11</v>
+      </c>
       <c r="J132" s="4">
         <v>0</v>
       </c>
@@ -8180,6 +8216,9 @@
       <c r="H133" t="s">
         <v>203</v>
       </c>
+      <c r="I133" t="s">
+        <v>11</v>
+      </c>
       <c r="J133" s="4">
         <v>0</v>
       </c>
@@ -9410,33 +9449,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A158" s="8" t="s">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
         <v>17</v>
       </c>
-      <c r="B158" s="9"/>
-      <c r="C158" s="9"/>
-      <c r="D158" s="10" t="s">
+      <c r="B158" s="5"/>
+      <c r="C158" s="5"/>
+      <c r="D158" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="E158" s="9" t="s">
+      <c r="E158" s="5" t="s">
         <v>463</v>
       </c>
-      <c r="F158" s="8" t="s">
+      <c r="F158" t="s">
         <v>423</v>
       </c>
-      <c r="G158" s="8" t="s">
+      <c r="G158" t="s">
         <v>392</v>
       </c>
-      <c r="H158" s="9" t="s">
+      <c r="H158" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I158" s="9" t="s">
+      <c r="I158" s="5" t="s">
         <v>11</v>
       </c>
       <c r="J158" s="4"/>
       <c r="K158" s="4"/>
-      <c r="L158" s="8">
+      <c r="L158">
         <v>1</v>
       </c>
       <c r="M158" s="4"/>

</xml_diff>